<commit_message>
software base con files .c .h divisi per periferica
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="54">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
   </si>
   <si>
     <t xml:space="preserve">CIAO</t>
@@ -1650,7 +1653,7 @@
         <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
software base + 4 display gare (problema allocazione memoria)
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31257" uniqueCount="254">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -177,6 +177,606 @@
   </si>
   <si>
     <t xml:space="preserve">CIAO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roboto-Bold.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">littl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Little</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H20_P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roboto-Regular.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Te</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AQUISITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACQUISITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENDURANCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKIDPAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOCROSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACCELERATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPM LIMITER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42-123</t>
   </si>
 </sst>
 </file>
@@ -1402,20 +2002,22 @@
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
       <c r="F4"/>
       <c r="G4"/>
-      <c r="H4"/>
+      <c r="H4" t="s">
+        <v>253</v>
+      </c>
       <c r="I4"/>
       <c r="K4" s="5" t="s">
         <v>17</v>
@@ -1435,20 +2037,22 @@
     </row>
     <row r="5" spans="2:15">
       <c r="B5" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="D5">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
-      <c r="H5"/>
+      <c r="H5" t="s">
+        <v>253</v>
+      </c>
       <c r="I5"/>
       <c r="K5" s="8" t="s">
         <v>1</v>
@@ -1466,20 +2070,22 @@
     </row>
     <row r="6" spans="2:15">
       <c r="B6" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6"/>
       <c r="G6"/>
-      <c r="H6"/>
+      <c r="H6" t="s">
+        <v>253</v>
+      </c>
       <c r="I6"/>
       <c r="K6" s="8" t="s">
         <v>2</v>
@@ -1496,6 +2102,26 @@
       <c r="O6" s="11"/>
     </row>
     <row r="7" spans="2:15">
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7">
+        <v>420</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7" t="s">
+        <v>253</v>
+      </c>
+      <c r="I7"/>
       <c r="K7" s="8" t="s">
         <v>15</v>
       </c>
@@ -1513,6 +2139,26 @@
       </c>
     </row>
     <row r="8" spans="2:15">
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8">
+        <v>180</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" t="s">
+        <v>253</v>
+      </c>
+      <c r="I8"/>
       <c r="K8" s="8" t="s">
         <v>16</v>
       </c>
@@ -1647,161 +2293,2483 @@
         <v>48</v>
       </c>
       <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1">
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="B18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="B19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="B21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4">
+      <c r="B22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4">
+      <c r="B24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="B25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4">
+      <c r="B26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="B27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4">
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="B29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="B30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="B31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" ht="15" customHeight="1"/>
-    <row r="6" spans="2:10"/>
-    <row r="7" spans="2:10"/>
-    <row r="8" spans="2:10"/>
-    <row r="9" spans="2:10"/>
-    <row r="10" spans="2:10"/>
-    <row r="13" spans="2:10"/>
-    <row r="14" spans="2:10"/>
-    <row r="15" spans="2:10"/>
-    <row r="16" spans="2:10"/>
-    <row r="17" spans="4:4"/>
-    <row r="18" spans="4:4"/>
-    <row r="19" spans="4:4"/>
-    <row r="20" spans="4:4"/>
-    <row r="21" spans="4:4"/>
-    <row r="22" spans="4:4"/>
-    <row r="23" spans="4:4"/>
-    <row r="24" spans="4:4"/>
-    <row r="25" spans="4:4"/>
-    <row r="26" spans="4:4"/>
-    <row r="27" spans="4:4"/>
-    <row r="28" spans="4:4"/>
-    <row r="29" spans="4:4"/>
-    <row r="30" spans="4:4"/>
-    <row r="31" spans="4:4"/>
-    <row r="32" spans="4:4"/>
-    <row r="33" spans="4:4"/>
-    <row r="34" spans="4:4"/>
-    <row r="35" spans="4:4"/>
-    <row r="36" spans="4:4"/>
-    <row r="37" spans="4:4"/>
-    <row r="38" spans="4:4"/>
-    <row r="39" spans="4:4"/>
-    <row r="40" spans="4:4"/>
-    <row r="41" spans="4:4"/>
-    <row r="42" spans="4:4"/>
-    <row r="43" spans="4:4"/>
-    <row r="44" spans="4:4"/>
-    <row r="45" spans="4:4"/>
-    <row r="46" spans="4:4"/>
-    <row r="47" spans="4:4"/>
-    <row r="48" spans="4:4"/>
-    <row r="49" spans="4:4"/>
-    <row r="50" spans="4:4"/>
-    <row r="51" spans="4:4"/>
-    <row r="52" spans="4:4"/>
-    <row r="53" spans="4:4"/>
-    <row r="54" spans="4:4"/>
-    <row r="55" spans="4:4"/>
-    <row r="56" spans="4:4"/>
-    <row r="57" spans="4:4"/>
-    <row r="58" spans="4:4"/>
-    <row r="59" spans="4:4"/>
-    <row r="60" spans="4:4"/>
-    <row r="61" spans="4:4"/>
-    <row r="62" spans="4:4"/>
-    <row r="63" spans="4:4"/>
-    <row r="64" spans="4:4"/>
-    <row r="65" spans="4:4"/>
-    <row r="66" spans="4:4"/>
-    <row r="67" spans="4:4"/>
-    <row r="68" spans="4:4"/>
-    <row r="69" spans="4:4"/>
-    <row r="70" spans="4:4"/>
-    <row r="71" spans="4:4"/>
-    <row r="72" spans="4:4"/>
-    <row r="73" spans="4:4"/>
-    <row r="74" spans="4:4"/>
-    <row r="75" spans="4:4"/>
-    <row r="76" spans="4:4"/>
-    <row r="77" spans="4:4"/>
-    <row r="78" spans="4:4"/>
-    <row r="79" spans="4:4"/>
-    <row r="80" spans="4:4"/>
-    <row r="81" spans="4:4"/>
-    <row r="82" spans="4:4"/>
-    <row r="83" spans="4:4"/>
-    <row r="84" spans="4:4"/>
-    <row r="85" spans="4:4"/>
-    <row r="86" spans="4:4"/>
-    <row r="87" spans="4:4"/>
-    <row r="88" spans="4:4"/>
-    <row r="89" spans="4:4"/>
-    <row r="90" spans="4:4"/>
-    <row r="91" spans="4:4"/>
-    <row r="92" spans="4:4"/>
-    <row r="93" spans="4:4"/>
-    <row r="94" spans="4:4"/>
-    <row r="95" spans="4:4"/>
-    <row r="96" spans="4:4"/>
-    <row r="97" spans="4:4"/>
-    <row r="98" spans="4:4"/>
-    <row r="99" spans="4:4"/>
-    <row r="100" spans="4:4"/>
-    <row r="101" spans="4:4"/>
-    <row r="102" spans="4:4"/>
-    <row r="103" spans="4:4"/>
-    <row r="104" spans="4:4"/>
-    <row r="105" spans="4:4"/>
-    <row r="106" spans="4:4"/>
-    <row r="107" spans="4:4"/>
-    <row r="108" spans="4:4"/>
-    <row r="109" spans="4:4"/>
-    <row r="110" spans="4:4"/>
-    <row r="111" spans="4:4"/>
-    <row r="112" spans="4:4"/>
-    <row r="113" spans="4:4"/>
-    <row r="114" spans="4:4"/>
-    <row r="115" spans="4:4"/>
-    <row r="116" spans="4:4"/>
-    <row r="117" spans="4:4"/>
-    <row r="118" spans="4:4"/>
-    <row r="119" spans="4:4"/>
-    <row r="120" spans="4:4"/>
-    <row r="121" spans="4:4"/>
-    <row r="122" spans="4:4"/>
-    <row r="123" spans="4:4"/>
-    <row r="124" spans="4:4"/>
-    <row r="125" spans="4:4"/>
-    <row r="126" spans="4:4"/>
-    <row r="127" spans="4:4"/>
-    <row r="128" spans="4:4"/>
-    <row r="129" spans="4:4"/>
-    <row r="130" spans="4:4"/>
-    <row r="131" spans="4:4"/>
-    <row r="132" spans="4:4"/>
-    <row r="133" spans="4:4"/>
-    <row r="134" spans="4:4"/>
-    <row r="135" spans="4:4"/>
-    <row r="136" spans="4:4"/>
-    <row r="137" spans="4:4"/>
-    <row r="138" spans="4:4"/>
-    <row r="139" spans="4:4"/>
-    <row r="140" spans="4:4"/>
-    <row r="141" spans="4:4"/>
-    <row r="142" spans="4:4"/>
-    <row r="143" spans="4:4"/>
-    <row r="144" spans="4:4"/>
-    <row r="145" spans="4:4"/>
-    <row r="146" spans="4:4"/>
-    <row r="147" spans="4:4"/>
-    <row r="148" spans="4:4"/>
-    <row r="149" spans="4:4"/>
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="B32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" t="s">
+        <v>119</v>
+      </c>
+      <c r="F32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="B33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="B34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="B35" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" t="s">
+        <v>127</v>
+      </c>
+      <c r="F35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="B36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" t="s">
+        <v>63</v>
+      </c>
+      <c r="F36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="B37" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" t="s">
+        <v>130</v>
+      </c>
+      <c r="F37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="B38" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="B39" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4">
+      <c r="B40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4">
+      <c r="B41" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" t="s">
+        <v>63</v>
+      </c>
+      <c r="F41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4">
+      <c r="B42" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4">
+      <c r="B43" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" t="s">
+        <v>63</v>
+      </c>
+      <c r="F43" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4">
+      <c r="B44" t="s">
+        <v>139</v>
+      </c>
+      <c r="C44" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4">
+      <c r="B45" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" t="s">
+        <v>63</v>
+      </c>
+      <c r="F45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4">
+      <c r="B46" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4">
+      <c r="B47" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" t="s">
+        <v>63</v>
+      </c>
+      <c r="F47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4">
+      <c r="B48" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" t="s">
+        <v>77</v>
+      </c>
+      <c r="F48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4">
+      <c r="B49" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" t="s">
+        <v>62</v>
+      </c>
+      <c r="E49" t="s">
+        <v>63</v>
+      </c>
+      <c r="F49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4">
+      <c r="B50" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" t="s">
+        <v>78</v>
+      </c>
+      <c r="F50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4">
+      <c r="B51" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" t="s">
+        <v>62</v>
+      </c>
+      <c r="E51" t="s">
+        <v>63</v>
+      </c>
+      <c r="F51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4">
+      <c r="B52" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" t="s">
+        <v>91</v>
+      </c>
+      <c r="F52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4">
+      <c r="B53" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" t="s">
+        <v>62</v>
+      </c>
+      <c r="E53" t="s">
+        <v>63</v>
+      </c>
+      <c r="F53" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4">
+      <c r="B54" t="s">
+        <v>149</v>
+      </c>
+      <c r="C54" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" t="s">
+        <v>91</v>
+      </c>
+      <c r="F54" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4">
+      <c r="B55" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" t="s">
+        <v>62</v>
+      </c>
+      <c r="E55" t="s">
+        <v>63</v>
+      </c>
+      <c r="F55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4">
+      <c r="B56" t="s">
+        <v>151</v>
+      </c>
+      <c r="C56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56" t="s">
+        <v>49</v>
+      </c>
+      <c r="E56" t="s">
+        <v>91</v>
+      </c>
+      <c r="F56" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4">
+      <c r="B57" t="s">
+        <v>152</v>
+      </c>
+      <c r="C57" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" t="s">
+        <v>62</v>
+      </c>
+      <c r="E57" t="s">
+        <v>63</v>
+      </c>
+      <c r="F57" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4">
+      <c r="B58" t="s">
+        <v>153</v>
+      </c>
+      <c r="C58" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" t="s">
+        <v>49</v>
+      </c>
+      <c r="E58" t="s">
+        <v>91</v>
+      </c>
+      <c r="F58" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4">
+      <c r="B59" t="s">
+        <v>154</v>
+      </c>
+      <c r="C59" t="s">
+        <v>59</v>
+      </c>
+      <c r="D59" t="s">
+        <v>62</v>
+      </c>
+      <c r="E59" t="s">
+        <v>63</v>
+      </c>
+      <c r="F59" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4">
+      <c r="B60" t="s">
+        <v>155</v>
+      </c>
+      <c r="C60" t="s">
+        <v>59</v>
+      </c>
+      <c r="D60" t="s">
+        <v>49</v>
+      </c>
+      <c r="E60" t="s">
+        <v>91</v>
+      </c>
+      <c r="F60" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="4:4">
+      <c r="B61" t="s">
+        <v>156</v>
+      </c>
+      <c r="C61" t="s">
+        <v>59</v>
+      </c>
+      <c r="D61" t="s">
+        <v>62</v>
+      </c>
+      <c r="E61" t="s">
+        <v>63</v>
+      </c>
+      <c r="F61" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="4:4">
+      <c r="B62" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" t="s">
+        <v>59</v>
+      </c>
+      <c r="D62" t="s">
+        <v>49</v>
+      </c>
+      <c r="E62" t="s">
+        <v>91</v>
+      </c>
+      <c r="F62" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="4:4">
+      <c r="B63" t="s">
+        <v>158</v>
+      </c>
+      <c r="C63" t="s">
+        <v>105</v>
+      </c>
+      <c r="D63" t="s">
+        <v>62</v>
+      </c>
+      <c r="E63" t="s">
+        <v>106</v>
+      </c>
+      <c r="F63" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="4:4">
+      <c r="B64" t="s">
+        <v>159</v>
+      </c>
+      <c r="C64" t="s">
+        <v>56</v>
+      </c>
+      <c r="D64" t="s">
+        <v>62</v>
+      </c>
+      <c r="E64" t="s">
+        <v>111</v>
+      </c>
+      <c r="F64" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4">
+      <c r="B65" t="s">
+        <v>160</v>
+      </c>
+      <c r="C65" t="s">
+        <v>56</v>
+      </c>
+      <c r="D65" t="s">
+        <v>62</v>
+      </c>
+      <c r="E65" t="s">
+        <v>112</v>
+      </c>
+      <c r="F65" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4">
+      <c r="B66" t="s">
+        <v>161</v>
+      </c>
+      <c r="C66" t="s">
+        <v>42</v>
+      </c>
+      <c r="D66" t="s">
+        <v>62</v>
+      </c>
+      <c r="E66" t="s">
+        <v>63</v>
+      </c>
+      <c r="F66" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4">
+      <c r="B67" t="s">
+        <v>162</v>
+      </c>
+      <c r="C67" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" t="s">
+        <v>119</v>
+      </c>
+      <c r="F67" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4">
+      <c r="B68" t="s">
+        <v>163</v>
+      </c>
+      <c r="C68" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" t="s">
+        <v>62</v>
+      </c>
+      <c r="E68" t="s">
+        <v>63</v>
+      </c>
+      <c r="F68" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4">
+      <c r="B69" t="s">
+        <v>164</v>
+      </c>
+      <c r="C69" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" t="s">
+        <v>49</v>
+      </c>
+      <c r="E69" t="s">
+        <v>86</v>
+      </c>
+      <c r="F69" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4">
+      <c r="B70" t="s">
+        <v>165</v>
+      </c>
+      <c r="C70" t="s">
+        <v>56</v>
+      </c>
+      <c r="D70" t="s">
+        <v>62</v>
+      </c>
+      <c r="E70" t="s">
+        <v>127</v>
+      </c>
+      <c r="F70" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4">
+      <c r="B71" t="s">
+        <v>166</v>
+      </c>
+      <c r="C71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D71" t="s">
+        <v>62</v>
+      </c>
+      <c r="E71" t="s">
+        <v>63</v>
+      </c>
+      <c r="F71" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4">
+      <c r="B72" t="s">
+        <v>167</v>
+      </c>
+      <c r="C72" t="s">
+        <v>59</v>
+      </c>
+      <c r="D72" t="s">
+        <v>49</v>
+      </c>
+      <c r="E72" t="s">
+        <v>130</v>
+      </c>
+      <c r="F72" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="4:4">
+      <c r="B73" t="s">
+        <v>168</v>
+      </c>
+      <c r="C73" t="s">
+        <v>56</v>
+      </c>
+      <c r="D73" t="s">
+        <v>62</v>
+      </c>
+      <c r="E73" t="s">
+        <v>170</v>
+      </c>
+      <c r="F73" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="4:4">
+      <c r="B74" t="s">
+        <v>171</v>
+      </c>
+      <c r="C74" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" t="s">
+        <v>62</v>
+      </c>
+      <c r="E74" t="s">
+        <v>63</v>
+      </c>
+      <c r="F74" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="4:4">
+      <c r="B75" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" t="s">
+        <v>49</v>
+      </c>
+      <c r="E75" t="s">
+        <v>84</v>
+      </c>
+      <c r="F75" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="4:4">
+      <c r="B76" t="s">
+        <v>173</v>
+      </c>
+      <c r="C76" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" t="s">
+        <v>62</v>
+      </c>
+      <c r="E76" t="s">
+        <v>63</v>
+      </c>
+      <c r="F76" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="77" spans="4:4">
+      <c r="B77" t="s">
+        <v>174</v>
+      </c>
+      <c r="C77" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" t="s">
+        <v>49</v>
+      </c>
+      <c r="E77" t="s">
+        <v>83</v>
+      </c>
+      <c r="F77" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4">
+      <c r="B78" t="s">
+        <v>175</v>
+      </c>
+      <c r="C78" t="s">
+        <v>56</v>
+      </c>
+      <c r="D78" t="s">
+        <v>62</v>
+      </c>
+      <c r="E78" t="s">
+        <v>63</v>
+      </c>
+      <c r="F78" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="4:4">
+      <c r="B79" t="s">
+        <v>176</v>
+      </c>
+      <c r="C79" t="s">
+        <v>56</v>
+      </c>
+      <c r="D79" t="s">
+        <v>49</v>
+      </c>
+      <c r="E79" t="s">
+        <v>81</v>
+      </c>
+      <c r="F79" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="4:4">
+      <c r="B80" t="s">
+        <v>177</v>
+      </c>
+      <c r="C80" t="s">
+        <v>56</v>
+      </c>
+      <c r="D80" t="s">
+        <v>62</v>
+      </c>
+      <c r="E80" t="s">
+        <v>63</v>
+      </c>
+      <c r="F80" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4">
+      <c r="B81" t="s">
+        <v>178</v>
+      </c>
+      <c r="C81" t="s">
+        <v>56</v>
+      </c>
+      <c r="D81" t="s">
+        <v>49</v>
+      </c>
+      <c r="E81" t="s">
+        <v>82</v>
+      </c>
+      <c r="F81" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4">
+      <c r="B82" t="s">
+        <v>179</v>
+      </c>
+      <c r="C82" t="s">
+        <v>56</v>
+      </c>
+      <c r="D82" t="s">
+        <v>62</v>
+      </c>
+      <c r="E82" t="s">
+        <v>63</v>
+      </c>
+      <c r="F82" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4">
+      <c r="B83" t="s">
+        <v>180</v>
+      </c>
+      <c r="C83" t="s">
+        <v>56</v>
+      </c>
+      <c r="D83" t="s">
+        <v>49</v>
+      </c>
+      <c r="E83" t="s">
+        <v>77</v>
+      </c>
+      <c r="F83" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4">
+      <c r="B84" t="s">
+        <v>181</v>
+      </c>
+      <c r="C84" t="s">
+        <v>56</v>
+      </c>
+      <c r="D84" t="s">
+        <v>62</v>
+      </c>
+      <c r="E84" t="s">
+        <v>63</v>
+      </c>
+      <c r="F84" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="4:4">
+      <c r="B85" t="s">
+        <v>182</v>
+      </c>
+      <c r="C85" t="s">
+        <v>56</v>
+      </c>
+      <c r="D85" t="s">
+        <v>49</v>
+      </c>
+      <c r="E85" t="s">
+        <v>78</v>
+      </c>
+      <c r="F85" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="86" spans="4:4">
+      <c r="B86" t="s">
+        <v>183</v>
+      </c>
+      <c r="C86" t="s">
+        <v>59</v>
+      </c>
+      <c r="D86" t="s">
+        <v>62</v>
+      </c>
+      <c r="E86" t="s">
+        <v>63</v>
+      </c>
+      <c r="F86" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4">
+      <c r="B87" t="s">
+        <v>184</v>
+      </c>
+      <c r="C87" t="s">
+        <v>59</v>
+      </c>
+      <c r="D87" t="s">
+        <v>49</v>
+      </c>
+      <c r="E87" t="s">
+        <v>91</v>
+      </c>
+      <c r="F87" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="4:4">
+      <c r="B88" t="s">
+        <v>185</v>
+      </c>
+      <c r="C88" t="s">
+        <v>59</v>
+      </c>
+      <c r="D88" t="s">
+        <v>62</v>
+      </c>
+      <c r="E88" t="s">
+        <v>63</v>
+      </c>
+      <c r="F88" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="4:4">
+      <c r="B89" t="s">
+        <v>186</v>
+      </c>
+      <c r="C89" t="s">
+        <v>59</v>
+      </c>
+      <c r="D89" t="s">
+        <v>49</v>
+      </c>
+      <c r="E89" t="s">
+        <v>91</v>
+      </c>
+      <c r="F89" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="4:4">
+      <c r="B90" t="s">
+        <v>187</v>
+      </c>
+      <c r="C90" t="s">
+        <v>59</v>
+      </c>
+      <c r="D90" t="s">
+        <v>62</v>
+      </c>
+      <c r="E90" t="s">
+        <v>63</v>
+      </c>
+      <c r="F90" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="91" spans="4:4">
+      <c r="B91" t="s">
+        <v>188</v>
+      </c>
+      <c r="C91" t="s">
+        <v>59</v>
+      </c>
+      <c r="D91" t="s">
+        <v>49</v>
+      </c>
+      <c r="E91" t="s">
+        <v>91</v>
+      </c>
+      <c r="F91" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="4:4">
+      <c r="B92" t="s">
+        <v>189</v>
+      </c>
+      <c r="C92" t="s">
+        <v>59</v>
+      </c>
+      <c r="D92" t="s">
+        <v>62</v>
+      </c>
+      <c r="E92" t="s">
+        <v>63</v>
+      </c>
+      <c r="F92" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93" spans="4:4">
+      <c r="B93" t="s">
+        <v>190</v>
+      </c>
+      <c r="C93" t="s">
+        <v>59</v>
+      </c>
+      <c r="D93" t="s">
+        <v>49</v>
+      </c>
+      <c r="E93" t="s">
+        <v>91</v>
+      </c>
+      <c r="F93" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="94" spans="4:4">
+      <c r="B94" t="s">
+        <v>191</v>
+      </c>
+      <c r="C94" t="s">
+        <v>59</v>
+      </c>
+      <c r="D94" t="s">
+        <v>62</v>
+      </c>
+      <c r="E94" t="s">
+        <v>63</v>
+      </c>
+      <c r="F94" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="95" spans="4:4">
+      <c r="B95" t="s">
+        <v>192</v>
+      </c>
+      <c r="C95" t="s">
+        <v>59</v>
+      </c>
+      <c r="D95" t="s">
+        <v>49</v>
+      </c>
+      <c r="E95" t="s">
+        <v>91</v>
+      </c>
+      <c r="F95" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="96" spans="4:4">
+      <c r="B96" t="s">
+        <v>193</v>
+      </c>
+      <c r="C96" t="s">
+        <v>59</v>
+      </c>
+      <c r="D96" t="s">
+        <v>62</v>
+      </c>
+      <c r="E96" t="s">
+        <v>63</v>
+      </c>
+      <c r="F96" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4">
+      <c r="B97" t="s">
+        <v>194</v>
+      </c>
+      <c r="C97" t="s">
+        <v>59</v>
+      </c>
+      <c r="D97" t="s">
+        <v>49</v>
+      </c>
+      <c r="E97" t="s">
+        <v>91</v>
+      </c>
+      <c r="F97" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4">
+      <c r="B98" t="s">
+        <v>195</v>
+      </c>
+      <c r="C98" t="s">
+        <v>105</v>
+      </c>
+      <c r="D98" t="s">
+        <v>62</v>
+      </c>
+      <c r="E98" t="s">
+        <v>106</v>
+      </c>
+      <c r="F98" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4">
+      <c r="B99" t="s">
+        <v>196</v>
+      </c>
+      <c r="C99" t="s">
+        <v>56</v>
+      </c>
+      <c r="D99" t="s">
+        <v>62</v>
+      </c>
+      <c r="E99" t="s">
+        <v>111</v>
+      </c>
+      <c r="F99" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="100" spans="4:4">
+      <c r="B100" t="s">
+        <v>197</v>
+      </c>
+      <c r="C100" t="s">
+        <v>56</v>
+      </c>
+      <c r="D100" t="s">
+        <v>62</v>
+      </c>
+      <c r="E100" t="s">
+        <v>112</v>
+      </c>
+      <c r="F100" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4">
+      <c r="B101" t="s">
+        <v>198</v>
+      </c>
+      <c r="C101" t="s">
+        <v>42</v>
+      </c>
+      <c r="D101" t="s">
+        <v>62</v>
+      </c>
+      <c r="E101" t="s">
+        <v>63</v>
+      </c>
+      <c r="F101" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4">
+      <c r="B102" t="s">
+        <v>199</v>
+      </c>
+      <c r="C102" t="s">
+        <v>42</v>
+      </c>
+      <c r="D102" t="s">
+        <v>49</v>
+      </c>
+      <c r="E102" t="s">
+        <v>119</v>
+      </c>
+      <c r="F102" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103" spans="4:4">
+      <c r="B103" t="s">
+        <v>200</v>
+      </c>
+      <c r="C103" t="s">
+        <v>42</v>
+      </c>
+      <c r="D103" t="s">
+        <v>62</v>
+      </c>
+      <c r="E103" t="s">
+        <v>63</v>
+      </c>
+      <c r="F103" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="104" spans="4:4">
+      <c r="B104" t="s">
+        <v>201</v>
+      </c>
+      <c r="C104" t="s">
+        <v>42</v>
+      </c>
+      <c r="D104" t="s">
+        <v>49</v>
+      </c>
+      <c r="E104" t="s">
+        <v>86</v>
+      </c>
+      <c r="F104" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="105" spans="4:4">
+      <c r="B105" t="s">
+        <v>202</v>
+      </c>
+      <c r="C105" t="s">
+        <v>56</v>
+      </c>
+      <c r="D105" t="s">
+        <v>62</v>
+      </c>
+      <c r="E105" t="s">
+        <v>127</v>
+      </c>
+      <c r="F105" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="106" spans="4:4">
+      <c r="B106" t="s">
+        <v>203</v>
+      </c>
+      <c r="C106" t="s">
+        <v>59</v>
+      </c>
+      <c r="D106" t="s">
+        <v>62</v>
+      </c>
+      <c r="E106" t="s">
+        <v>63</v>
+      </c>
+      <c r="F106" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="107" spans="4:4">
+      <c r="B107" t="s">
+        <v>204</v>
+      </c>
+      <c r="C107" t="s">
+        <v>59</v>
+      </c>
+      <c r="D107" t="s">
+        <v>49</v>
+      </c>
+      <c r="E107" t="s">
+        <v>130</v>
+      </c>
+      <c r="F107" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108" spans="4:4">
+      <c r="B108" t="s">
+        <v>205</v>
+      </c>
+      <c r="C108" t="s">
+        <v>56</v>
+      </c>
+      <c r="D108" t="s">
+        <v>62</v>
+      </c>
+      <c r="E108" t="s">
+        <v>241</v>
+      </c>
+      <c r="F108" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="109" spans="4:4">
+      <c r="B109" t="s">
+        <v>206</v>
+      </c>
+      <c r="C109" t="s">
+        <v>56</v>
+      </c>
+      <c r="D109" t="s">
+        <v>62</v>
+      </c>
+      <c r="E109" t="s">
+        <v>63</v>
+      </c>
+      <c r="F109" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="110" spans="4:4">
+      <c r="B110" t="s">
+        <v>207</v>
+      </c>
+      <c r="C110" t="s">
+        <v>56</v>
+      </c>
+      <c r="D110" t="s">
+        <v>49</v>
+      </c>
+      <c r="E110" t="s">
+        <v>84</v>
+      </c>
+      <c r="F110" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="111" spans="4:4">
+      <c r="B111" t="s">
+        <v>208</v>
+      </c>
+      <c r="C111" t="s">
+        <v>56</v>
+      </c>
+      <c r="D111" t="s">
+        <v>62</v>
+      </c>
+      <c r="E111" t="s">
+        <v>63</v>
+      </c>
+      <c r="F111" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="112" spans="4:4">
+      <c r="B112" t="s">
+        <v>209</v>
+      </c>
+      <c r="C112" t="s">
+        <v>56</v>
+      </c>
+      <c r="D112" t="s">
+        <v>49</v>
+      </c>
+      <c r="E112" t="s">
+        <v>83</v>
+      </c>
+      <c r="F112" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4">
+      <c r="B113" t="s">
+        <v>210</v>
+      </c>
+      <c r="C113" t="s">
+        <v>56</v>
+      </c>
+      <c r="D113" t="s">
+        <v>62</v>
+      </c>
+      <c r="E113" t="s">
+        <v>63</v>
+      </c>
+      <c r="F113" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4">
+      <c r="B114" t="s">
+        <v>211</v>
+      </c>
+      <c r="C114" t="s">
+        <v>56</v>
+      </c>
+      <c r="D114" t="s">
+        <v>49</v>
+      </c>
+      <c r="E114" t="s">
+        <v>81</v>
+      </c>
+      <c r="F114" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4">
+      <c r="B115" t="s">
+        <v>212</v>
+      </c>
+      <c r="C115" t="s">
+        <v>56</v>
+      </c>
+      <c r="D115" t="s">
+        <v>62</v>
+      </c>
+      <c r="E115" t="s">
+        <v>63</v>
+      </c>
+      <c r="F115" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="116" spans="4:4">
+      <c r="B116" t="s">
+        <v>213</v>
+      </c>
+      <c r="C116" t="s">
+        <v>56</v>
+      </c>
+      <c r="D116" t="s">
+        <v>49</v>
+      </c>
+      <c r="E116" t="s">
+        <v>82</v>
+      </c>
+      <c r="F116" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4">
+      <c r="B117" t="s">
+        <v>214</v>
+      </c>
+      <c r="C117" t="s">
+        <v>56</v>
+      </c>
+      <c r="D117" t="s">
+        <v>62</v>
+      </c>
+      <c r="E117" t="s">
+        <v>63</v>
+      </c>
+      <c r="F117" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="118" spans="4:4">
+      <c r="B118" t="s">
+        <v>215</v>
+      </c>
+      <c r="C118" t="s">
+        <v>56</v>
+      </c>
+      <c r="D118" t="s">
+        <v>49</v>
+      </c>
+      <c r="E118" t="s">
+        <v>77</v>
+      </c>
+      <c r="F118" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="119" spans="4:4">
+      <c r="B119" t="s">
+        <v>216</v>
+      </c>
+      <c r="C119" t="s">
+        <v>56</v>
+      </c>
+      <c r="D119" t="s">
+        <v>62</v>
+      </c>
+      <c r="E119" t="s">
+        <v>63</v>
+      </c>
+      <c r="F119" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="120" spans="4:4">
+      <c r="B120" t="s">
+        <v>217</v>
+      </c>
+      <c r="C120" t="s">
+        <v>56</v>
+      </c>
+      <c r="D120" t="s">
+        <v>49</v>
+      </c>
+      <c r="E120" t="s">
+        <v>78</v>
+      </c>
+      <c r="F120" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="121" spans="4:4">
+      <c r="B121" t="s">
+        <v>218</v>
+      </c>
+      <c r="C121" t="s">
+        <v>59</v>
+      </c>
+      <c r="D121" t="s">
+        <v>62</v>
+      </c>
+      <c r="E121" t="s">
+        <v>63</v>
+      </c>
+      <c r="F121" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="122" spans="4:4">
+      <c r="B122" t="s">
+        <v>219</v>
+      </c>
+      <c r="C122" t="s">
+        <v>59</v>
+      </c>
+      <c r="D122" t="s">
+        <v>49</v>
+      </c>
+      <c r="E122" t="s">
+        <v>91</v>
+      </c>
+      <c r="F122" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="123" spans="4:4">
+      <c r="B123" t="s">
+        <v>220</v>
+      </c>
+      <c r="C123" t="s">
+        <v>59</v>
+      </c>
+      <c r="D123" t="s">
+        <v>62</v>
+      </c>
+      <c r="E123" t="s">
+        <v>63</v>
+      </c>
+      <c r="F123" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="124" spans="4:4">
+      <c r="B124" t="s">
+        <v>221</v>
+      </c>
+      <c r="C124" t="s">
+        <v>59</v>
+      </c>
+      <c r="D124" t="s">
+        <v>49</v>
+      </c>
+      <c r="E124" t="s">
+        <v>91</v>
+      </c>
+      <c r="F124" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="125" spans="4:4">
+      <c r="B125" t="s">
+        <v>222</v>
+      </c>
+      <c r="C125" t="s">
+        <v>59</v>
+      </c>
+      <c r="D125" t="s">
+        <v>62</v>
+      </c>
+      <c r="E125" t="s">
+        <v>63</v>
+      </c>
+      <c r="F125" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="126" spans="4:4">
+      <c r="B126" t="s">
+        <v>223</v>
+      </c>
+      <c r="C126" t="s">
+        <v>59</v>
+      </c>
+      <c r="D126" t="s">
+        <v>49</v>
+      </c>
+      <c r="E126" t="s">
+        <v>91</v>
+      </c>
+      <c r="F126" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="127" spans="4:4">
+      <c r="B127" t="s">
+        <v>224</v>
+      </c>
+      <c r="C127" t="s">
+        <v>59</v>
+      </c>
+      <c r="D127" t="s">
+        <v>62</v>
+      </c>
+      <c r="E127" t="s">
+        <v>63</v>
+      </c>
+      <c r="F127" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="128" spans="4:4">
+      <c r="B128" t="s">
+        <v>225</v>
+      </c>
+      <c r="C128" t="s">
+        <v>59</v>
+      </c>
+      <c r="D128" t="s">
+        <v>49</v>
+      </c>
+      <c r="E128" t="s">
+        <v>91</v>
+      </c>
+      <c r="F128" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="129" spans="4:4">
+      <c r="B129" t="s">
+        <v>226</v>
+      </c>
+      <c r="C129" t="s">
+        <v>59</v>
+      </c>
+      <c r="D129" t="s">
+        <v>62</v>
+      </c>
+      <c r="E129" t="s">
+        <v>63</v>
+      </c>
+      <c r="F129" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4">
+      <c r="B130" t="s">
+        <v>227</v>
+      </c>
+      <c r="C130" t="s">
+        <v>59</v>
+      </c>
+      <c r="D130" t="s">
+        <v>49</v>
+      </c>
+      <c r="E130" t="s">
+        <v>91</v>
+      </c>
+      <c r="F130" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="131" spans="4:4">
+      <c r="B131" t="s">
+        <v>228</v>
+      </c>
+      <c r="C131" t="s">
+        <v>59</v>
+      </c>
+      <c r="D131" t="s">
+        <v>62</v>
+      </c>
+      <c r="E131" t="s">
+        <v>63</v>
+      </c>
+      <c r="F131" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="132" spans="4:4">
+      <c r="B132" t="s">
+        <v>229</v>
+      </c>
+      <c r="C132" t="s">
+        <v>59</v>
+      </c>
+      <c r="D132" t="s">
+        <v>49</v>
+      </c>
+      <c r="E132" t="s">
+        <v>91</v>
+      </c>
+      <c r="F132" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="133" spans="4:4">
+      <c r="B133" t="s">
+        <v>230</v>
+      </c>
+      <c r="C133" t="s">
+        <v>105</v>
+      </c>
+      <c r="D133" t="s">
+        <v>62</v>
+      </c>
+      <c r="E133" t="s">
+        <v>106</v>
+      </c>
+      <c r="F133" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="134" spans="4:4">
+      <c r="B134" t="s">
+        <v>231</v>
+      </c>
+      <c r="C134" t="s">
+        <v>56</v>
+      </c>
+      <c r="D134" t="s">
+        <v>62</v>
+      </c>
+      <c r="E134" t="s">
+        <v>111</v>
+      </c>
+      <c r="F134" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="135" spans="4:4">
+      <c r="B135" t="s">
+        <v>232</v>
+      </c>
+      <c r="C135" t="s">
+        <v>56</v>
+      </c>
+      <c r="D135" t="s">
+        <v>62</v>
+      </c>
+      <c r="E135" t="s">
+        <v>112</v>
+      </c>
+      <c r="F135" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="136" spans="4:4">
+      <c r="B136" t="s">
+        <v>233</v>
+      </c>
+      <c r="C136" t="s">
+        <v>42</v>
+      </c>
+      <c r="D136" t="s">
+        <v>62</v>
+      </c>
+      <c r="E136" t="s">
+        <v>63</v>
+      </c>
+      <c r="F136" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="137" spans="4:4">
+      <c r="B137" t="s">
+        <v>234</v>
+      </c>
+      <c r="C137" t="s">
+        <v>42</v>
+      </c>
+      <c r="D137" t="s">
+        <v>49</v>
+      </c>
+      <c r="E137" t="s">
+        <v>119</v>
+      </c>
+      <c r="F137" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="138" spans="4:4">
+      <c r="B138" t="s">
+        <v>235</v>
+      </c>
+      <c r="C138" t="s">
+        <v>42</v>
+      </c>
+      <c r="D138" t="s">
+        <v>62</v>
+      </c>
+      <c r="E138" t="s">
+        <v>63</v>
+      </c>
+      <c r="F138" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="139" spans="4:4">
+      <c r="B139" t="s">
+        <v>236</v>
+      </c>
+      <c r="C139" t="s">
+        <v>42</v>
+      </c>
+      <c r="D139" t="s">
+        <v>49</v>
+      </c>
+      <c r="E139" t="s">
+        <v>86</v>
+      </c>
+      <c r="F139" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="140" spans="4:4">
+      <c r="B140" t="s">
+        <v>237</v>
+      </c>
+      <c r="C140" t="s">
+        <v>56</v>
+      </c>
+      <c r="D140" t="s">
+        <v>62</v>
+      </c>
+      <c r="E140" t="s">
+        <v>127</v>
+      </c>
+      <c r="F140" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="141" spans="4:4">
+      <c r="B141" t="s">
+        <v>238</v>
+      </c>
+      <c r="C141" t="s">
+        <v>59</v>
+      </c>
+      <c r="D141" t="s">
+        <v>62</v>
+      </c>
+      <c r="E141" t="s">
+        <v>63</v>
+      </c>
+      <c r="F141" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="142" spans="4:4">
+      <c r="B142" t="s">
+        <v>239</v>
+      </c>
+      <c r="C142" t="s">
+        <v>59</v>
+      </c>
+      <c r="D142" t="s">
+        <v>49</v>
+      </c>
+      <c r="E142" t="s">
+        <v>130</v>
+      </c>
+      <c r="F142" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="143" spans="4:4">
+      <c r="B143" t="s">
+        <v>240</v>
+      </c>
+      <c r="C143" t="s">
+        <v>56</v>
+      </c>
+      <c r="D143" t="s">
+        <v>62</v>
+      </c>
+      <c r="E143" t="s">
+        <v>242</v>
+      </c>
+      <c r="F143" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="144" spans="4:4">
+      <c r="B144" t="s">
+        <v>243</v>
+      </c>
+      <c r="C144" t="s">
+        <v>56</v>
+      </c>
+      <c r="D144" t="s">
+        <v>62</v>
+      </c>
+      <c r="E144" t="s">
+        <v>246</v>
+      </c>
+      <c r="F144" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="145" spans="4:4">
+      <c r="B145" t="s">
+        <v>244</v>
+      </c>
+      <c r="C145" t="s">
+        <v>59</v>
+      </c>
+      <c r="D145" t="s">
+        <v>62</v>
+      </c>
+      <c r="E145" t="s">
+        <v>63</v>
+      </c>
+      <c r="F145" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="146" spans="4:4">
+      <c r="B146" t="s">
+        <v>245</v>
+      </c>
+      <c r="C146" t="s">
+        <v>59</v>
+      </c>
+      <c r="D146" t="s">
+        <v>49</v>
+      </c>
+      <c r="E146" t="s">
+        <v>119</v>
+      </c>
+      <c r="F146" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="147" spans="4:4">
+      <c r="B147" t="s">
+        <v>249</v>
+      </c>
+      <c r="C147" t="s">
+        <v>56</v>
+      </c>
+      <c r="D147" t="s">
+        <v>62</v>
+      </c>
+      <c r="E147" t="s">
+        <v>246</v>
+      </c>
+      <c r="F147" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="148" spans="4:4">
+      <c r="B148" t="s">
+        <v>250</v>
+      </c>
+      <c r="C148" t="s">
+        <v>59</v>
+      </c>
+      <c r="D148" t="s">
+        <v>62</v>
+      </c>
+      <c r="E148" t="s">
+        <v>63</v>
+      </c>
+      <c r="F148" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="149" spans="4:4">
+      <c r="B149" t="s">
+        <v>251</v>
+      </c>
+      <c r="C149" t="s">
+        <v>59</v>
+      </c>
+      <c r="D149" t="s">
+        <v>49</v>
+      </c>
+      <c r="E149" t="s">
+        <v>119</v>
+      </c>
+      <c r="F149" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="150" spans="4:4"/>
     <row r="151" spans="4:4"/>
     <row r="152" spans="4:4"/>

</xml_diff>

<commit_message>
software base + 4 display gare (refresh schermi+ tipo dato indicatore)
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31257" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34903" uniqueCount="258">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -777,6 +777,18 @@
   </si>
   <si>
     <t xml:space="preserve">42-123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId151</t>
   </si>
 </sst>
 </file>
@@ -2707,7 +2719,7 @@
         <v>62</v>
       </c>
       <c r="E28" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="F28" t="s">
         <v>50</v>
@@ -3302,7 +3314,7 @@
         <v>62</v>
       </c>
       <c r="E63" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="F63" t="s">
         <v>50</v>
@@ -3897,7 +3909,7 @@
         <v>62</v>
       </c>
       <c r="E98" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="F98" t="s">
         <v>50</v>
@@ -4492,7 +4504,7 @@
         <v>62</v>
       </c>
       <c r="E133" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="F133" t="s">
         <v>50</v>
@@ -4770,10 +4782,74 @@
         <v>50</v>
       </c>
     </row>
-    <row r="150" spans="4:4"/>
-    <row r="151" spans="4:4"/>
-    <row r="152" spans="4:4"/>
-    <row r="153" spans="4:4"/>
+    <row r="150" spans="4:4">
+      <c r="B150" t="s">
+        <v>254</v>
+      </c>
+      <c r="C150" t="s">
+        <v>105</v>
+      </c>
+      <c r="D150" t="s">
+        <v>49</v>
+      </c>
+      <c r="E150" t="s">
+        <v>106</v>
+      </c>
+      <c r="F150" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="151" spans="4:4">
+      <c r="B151" t="s">
+        <v>255</v>
+      </c>
+      <c r="C151" t="s">
+        <v>105</v>
+      </c>
+      <c r="D151" t="s">
+        <v>49</v>
+      </c>
+      <c r="E151" t="s">
+        <v>106</v>
+      </c>
+      <c r="F151" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="152" spans="4:4">
+      <c r="B152" t="s">
+        <v>256</v>
+      </c>
+      <c r="C152" t="s">
+        <v>105</v>
+      </c>
+      <c r="D152" t="s">
+        <v>49</v>
+      </c>
+      <c r="E152" t="s">
+        <v>106</v>
+      </c>
+      <c r="F152" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="153" spans="4:4">
+      <c r="B153" t="s">
+        <v>257</v>
+      </c>
+      <c r="C153" t="s">
+        <v>105</v>
+      </c>
+      <c r="D153" t="s">
+        <v>49</v>
+      </c>
+      <c r="E153" t="s">
+        <v>106</v>
+      </c>
+      <c r="F153" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="154" spans="4:4"/>
     <row r="155" spans="4:4"/>
     <row r="156" spans="4:4"/>

</xml_diff>

<commit_message>
7 display, manca la logica dei 3 display aggiunti
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34903" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107023" uniqueCount="376">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -789,6 +789,360 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">END</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH2O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId163</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRIVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRIVE MODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IND_TIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENDURA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId194</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId197</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
   </si>
 </sst>
 </file>
@@ -4850,96 +5204,1536 @@
         <v>50</v>
       </c>
     </row>
-    <row r="154" spans="4:4"/>
-    <row r="155" spans="4:4"/>
-    <row r="156" spans="4:4"/>
-    <row r="157" spans="4:4"/>
-    <row r="158" spans="4:4"/>
-    <row r="159" spans="4:4"/>
-    <row r="160" spans="4:4"/>
-    <row r="161" spans="4:4"/>
-    <row r="162" spans="4:4"/>
-    <row r="163" spans="4:4"/>
-    <row r="164" spans="4:4"/>
-    <row r="165" spans="4:4"/>
-    <row r="166" spans="4:4"/>
-    <row r="167" spans="4:4"/>
-    <row r="168" spans="4:4"/>
-    <row r="169" spans="4:4"/>
-    <row r="170" spans="4:4"/>
-    <row r="171" spans="4:4"/>
-    <row r="172" spans="4:4"/>
-    <row r="173" spans="4:4"/>
-    <row r="174" spans="4:4"/>
-    <row r="175" spans="4:4"/>
-    <row r="176" spans="4:4"/>
-    <row r="177" spans="4:4"/>
-    <row r="178" spans="4:4"/>
-    <row r="179" spans="4:4"/>
-    <row r="180" spans="4:4"/>
-    <row r="181" spans="4:4"/>
-    <row r="182" spans="4:4"/>
-    <row r="183" spans="4:4"/>
-    <row r="184" spans="4:4"/>
-    <row r="185" spans="4:4"/>
-    <row r="186" spans="4:4"/>
-    <row r="187" spans="4:4"/>
-    <row r="188" spans="4:4"/>
-    <row r="189" spans="4:4"/>
-    <row r="190" spans="4:4"/>
-    <row r="191" spans="4:4"/>
-    <row r="192" spans="4:4"/>
-    <row r="193" spans="4:4"/>
-    <row r="194" spans="4:4"/>
-    <row r="195" spans="4:4"/>
-    <row r="196" spans="4:4"/>
-    <row r="197" spans="4:4"/>
-    <row r="198" spans="4:4"/>
-    <row r="199" spans="4:4"/>
-    <row r="200" spans="4:4"/>
-    <row r="201" spans="4:4"/>
-    <row r="202" spans="4:4"/>
-    <row r="203" spans="4:4"/>
-    <row r="204" spans="4:4"/>
-    <row r="205" spans="4:4"/>
-    <row r="206" spans="4:4"/>
-    <row r="207" spans="4:4"/>
-    <row r="208" spans="4:4"/>
-    <row r="209" spans="4:4"/>
-    <row r="210" spans="4:4"/>
-    <row r="211" spans="4:4"/>
-    <row r="212" spans="4:4"/>
-    <row r="213" spans="4:4"/>
-    <row r="214" spans="4:4"/>
-    <row r="215" spans="4:4"/>
-    <row r="216" spans="4:4"/>
-    <row r="217" spans="4:4"/>
-    <row r="218" spans="4:4"/>
-    <row r="219" spans="4:4"/>
-    <row r="220" spans="4:4"/>
-    <row r="221" spans="4:4"/>
-    <row r="222" spans="4:4"/>
-    <row r="223" spans="4:4"/>
-    <row r="224" spans="4:4"/>
-    <row r="225" spans="4:4"/>
-    <row r="226" spans="4:4"/>
-    <row r="227" spans="4:4"/>
-    <row r="228" spans="4:4"/>
-    <row r="229" spans="4:4"/>
-    <row r="230" spans="4:4"/>
-    <row r="231" spans="4:4"/>
-    <row r="232" spans="4:4"/>
-    <row r="233" spans="4:4"/>
-    <row r="234" spans="4:4"/>
-    <row r="235" spans="4:4"/>
-    <row r="236" spans="4:4"/>
-    <row r="237" spans="4:4"/>
-    <row r="238" spans="4:4"/>
-    <row r="239" spans="4:4"/>
-    <row r="240" spans="4:4"/>
-    <row r="241" spans="4:4"/>
-    <row r="242" spans="4:4"/>
-    <row r="243" spans="4:4"/>
+    <row r="154" spans="4:4">
+      <c r="B154" t="s">
+        <v>258</v>
+      </c>
+      <c r="C154" t="s">
+        <v>59</v>
+      </c>
+      <c r="D154" t="s">
+        <v>49</v>
+      </c>
+      <c r="E154" t="s">
+        <v>242</v>
+      </c>
+      <c r="F154" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="155" spans="4:4">
+      <c r="B155" t="s">
+        <v>259</v>
+      </c>
+      <c r="C155" t="s">
+        <v>59</v>
+      </c>
+      <c r="D155" t="s">
+        <v>49</v>
+      </c>
+      <c r="E155" t="s">
+        <v>133</v>
+      </c>
+      <c r="F155" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="156" spans="4:4">
+      <c r="B156" t="s">
+        <v>260</v>
+      </c>
+      <c r="C156" t="s">
+        <v>59</v>
+      </c>
+      <c r="D156" t="s">
+        <v>49</v>
+      </c>
+      <c r="E156" t="s">
+        <v>241</v>
+      </c>
+      <c r="F156" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="157" spans="4:4">
+      <c r="B157" t="s">
+        <v>261</v>
+      </c>
+      <c r="C157" t="s">
+        <v>59</v>
+      </c>
+      <c r="D157" t="s">
+        <v>49</v>
+      </c>
+      <c r="E157" t="s">
+        <v>170</v>
+      </c>
+      <c r="F157" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="158" spans="4:4">
+      <c r="B158" t="s">
+        <v>263</v>
+      </c>
+      <c r="C158" t="s">
+        <v>56</v>
+      </c>
+      <c r="D158" t="s">
+        <v>62</v>
+      </c>
+      <c r="E158" t="s">
+        <v>63</v>
+      </c>
+      <c r="F158" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="159" spans="4:4">
+      <c r="B159" t="s">
+        <v>264</v>
+      </c>
+      <c r="C159" t="s">
+        <v>56</v>
+      </c>
+      <c r="D159" t="s">
+        <v>49</v>
+      </c>
+      <c r="E159" t="s">
+        <v>84</v>
+      </c>
+      <c r="F159" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="160" spans="4:4">
+      <c r="B160" t="s">
+        <v>265</v>
+      </c>
+      <c r="C160" t="s">
+        <v>56</v>
+      </c>
+      <c r="D160" t="s">
+        <v>62</v>
+      </c>
+      <c r="E160" t="s">
+        <v>63</v>
+      </c>
+      <c r="F160" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="161" spans="4:4">
+      <c r="B161" t="s">
+        <v>266</v>
+      </c>
+      <c r="C161" t="s">
+        <v>56</v>
+      </c>
+      <c r="D161" t="s">
+        <v>49</v>
+      </c>
+      <c r="E161" t="s">
+        <v>83</v>
+      </c>
+      <c r="F161" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="162" spans="4:4">
+      <c r="B162" t="s">
+        <v>267</v>
+      </c>
+      <c r="C162" t="s">
+        <v>56</v>
+      </c>
+      <c r="D162" t="s">
+        <v>62</v>
+      </c>
+      <c r="E162" t="s">
+        <v>63</v>
+      </c>
+      <c r="F162" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="163" spans="4:4">
+      <c r="B163" t="s">
+        <v>270</v>
+      </c>
+      <c r="C163" t="s">
+        <v>56</v>
+      </c>
+      <c r="D163" t="s">
+        <v>49</v>
+      </c>
+      <c r="E163" t="s">
+        <v>81</v>
+      </c>
+      <c r="F163" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="164" spans="4:4">
+      <c r="B164" t="s">
+        <v>274</v>
+      </c>
+      <c r="C164" t="s">
+        <v>56</v>
+      </c>
+      <c r="D164" t="s">
+        <v>62</v>
+      </c>
+      <c r="E164" t="s">
+        <v>63</v>
+      </c>
+      <c r="F164" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="165" spans="4:4">
+      <c r="B165" t="s">
+        <v>275</v>
+      </c>
+      <c r="C165" t="s">
+        <v>56</v>
+      </c>
+      <c r="D165" t="s">
+        <v>49</v>
+      </c>
+      <c r="E165" t="s">
+        <v>82</v>
+      </c>
+      <c r="F165" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="166" spans="4:4">
+      <c r="B166" t="s">
+        <v>276</v>
+      </c>
+      <c r="C166" t="s">
+        <v>56</v>
+      </c>
+      <c r="D166" t="s">
+        <v>62</v>
+      </c>
+      <c r="E166" t="s">
+        <v>63</v>
+      </c>
+      <c r="F166" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="167" spans="4:4">
+      <c r="B167" t="s">
+        <v>277</v>
+      </c>
+      <c r="C167" t="s">
+        <v>56</v>
+      </c>
+      <c r="D167" t="s">
+        <v>49</v>
+      </c>
+      <c r="E167" t="s">
+        <v>77</v>
+      </c>
+      <c r="F167" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="168" spans="4:4">
+      <c r="B168" t="s">
+        <v>278</v>
+      </c>
+      <c r="C168" t="s">
+        <v>56</v>
+      </c>
+      <c r="D168" t="s">
+        <v>62</v>
+      </c>
+      <c r="E168" t="s">
+        <v>63</v>
+      </c>
+      <c r="F168" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="169" spans="4:4">
+      <c r="B169" t="s">
+        <v>279</v>
+      </c>
+      <c r="C169" t="s">
+        <v>56</v>
+      </c>
+      <c r="D169" t="s">
+        <v>49</v>
+      </c>
+      <c r="E169" t="s">
+        <v>78</v>
+      </c>
+      <c r="F169" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="170" spans="4:4">
+      <c r="B170" t="s">
+        <v>280</v>
+      </c>
+      <c r="C170" t="s">
+        <v>59</v>
+      </c>
+      <c r="D170" t="s">
+        <v>62</v>
+      </c>
+      <c r="E170" t="s">
+        <v>63</v>
+      </c>
+      <c r="F170" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="171" spans="4:4">
+      <c r="B171" t="s">
+        <v>281</v>
+      </c>
+      <c r="C171" t="s">
+        <v>59</v>
+      </c>
+      <c r="D171" t="s">
+        <v>49</v>
+      </c>
+      <c r="E171" t="s">
+        <v>91</v>
+      </c>
+      <c r="F171" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="172" spans="4:4">
+      <c r="B172" t="s">
+        <v>282</v>
+      </c>
+      <c r="C172" t="s">
+        <v>59</v>
+      </c>
+      <c r="D172" t="s">
+        <v>62</v>
+      </c>
+      <c r="E172" t="s">
+        <v>63</v>
+      </c>
+      <c r="F172" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="173" spans="4:4">
+      <c r="B173" t="s">
+        <v>283</v>
+      </c>
+      <c r="C173" t="s">
+        <v>59</v>
+      </c>
+      <c r="D173" t="s">
+        <v>49</v>
+      </c>
+      <c r="E173" t="s">
+        <v>91</v>
+      </c>
+      <c r="F173" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="174" spans="4:4">
+      <c r="B174" t="s">
+        <v>284</v>
+      </c>
+      <c r="C174" t="s">
+        <v>59</v>
+      </c>
+      <c r="D174" t="s">
+        <v>62</v>
+      </c>
+      <c r="E174" t="s">
+        <v>63</v>
+      </c>
+      <c r="F174" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="175" spans="4:4">
+      <c r="B175" t="s">
+        <v>285</v>
+      </c>
+      <c r="C175" t="s">
+        <v>59</v>
+      </c>
+      <c r="D175" t="s">
+        <v>49</v>
+      </c>
+      <c r="E175" t="s">
+        <v>91</v>
+      </c>
+      <c r="F175" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="176" spans="4:4">
+      <c r="B176" t="s">
+        <v>286</v>
+      </c>
+      <c r="C176" t="s">
+        <v>59</v>
+      </c>
+      <c r="D176" t="s">
+        <v>62</v>
+      </c>
+      <c r="E176" t="s">
+        <v>63</v>
+      </c>
+      <c r="F176" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="177" spans="4:4">
+      <c r="B177" t="s">
+        <v>287</v>
+      </c>
+      <c r="C177" t="s">
+        <v>59</v>
+      </c>
+      <c r="D177" t="s">
+        <v>49</v>
+      </c>
+      <c r="E177" t="s">
+        <v>91</v>
+      </c>
+      <c r="F177" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="178" spans="4:4">
+      <c r="B178" t="s">
+        <v>288</v>
+      </c>
+      <c r="C178" t="s">
+        <v>59</v>
+      </c>
+      <c r="D178" t="s">
+        <v>62</v>
+      </c>
+      <c r="E178" t="s">
+        <v>63</v>
+      </c>
+      <c r="F178" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="179" spans="4:4">
+      <c r="B179" t="s">
+        <v>289</v>
+      </c>
+      <c r="C179" t="s">
+        <v>59</v>
+      </c>
+      <c r="D179" t="s">
+        <v>49</v>
+      </c>
+      <c r="E179" t="s">
+        <v>91</v>
+      </c>
+      <c r="F179" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="180" spans="4:4">
+      <c r="B180" t="s">
+        <v>290</v>
+      </c>
+      <c r="C180" t="s">
+        <v>59</v>
+      </c>
+      <c r="D180" t="s">
+        <v>62</v>
+      </c>
+      <c r="E180" t="s">
+        <v>63</v>
+      </c>
+      <c r="F180" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="181" spans="4:4">
+      <c r="B181" t="s">
+        <v>291</v>
+      </c>
+      <c r="C181" t="s">
+        <v>59</v>
+      </c>
+      <c r="D181" t="s">
+        <v>49</v>
+      </c>
+      <c r="E181" t="s">
+        <v>91</v>
+      </c>
+      <c r="F181" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="182" spans="4:4">
+      <c r="B182" t="s">
+        <v>292</v>
+      </c>
+      <c r="C182" t="s">
+        <v>56</v>
+      </c>
+      <c r="D182" t="s">
+        <v>62</v>
+      </c>
+      <c r="E182" t="s">
+        <v>63</v>
+      </c>
+      <c r="F182" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="183" spans="4:4">
+      <c r="B183" t="s">
+        <v>294</v>
+      </c>
+      <c r="C183" t="s">
+        <v>59</v>
+      </c>
+      <c r="D183" t="s">
+        <v>62</v>
+      </c>
+      <c r="E183" t="s">
+        <v>63</v>
+      </c>
+      <c r="F183" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="184" spans="4:4">
+      <c r="B184" t="s">
+        <v>300</v>
+      </c>
+      <c r="C184" t="s">
+        <v>59</v>
+      </c>
+      <c r="D184" t="s">
+        <v>49</v>
+      </c>
+      <c r="E184" t="s">
+        <v>302</v>
+      </c>
+      <c r="F184" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="185" spans="4:4">
+      <c r="B185" t="s">
+        <v>304</v>
+      </c>
+      <c r="C185" t="s">
+        <v>56</v>
+      </c>
+      <c r="D185" t="s">
+        <v>49</v>
+      </c>
+      <c r="E185" t="s">
+        <v>299</v>
+      </c>
+      <c r="F185" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="186" spans="4:4">
+      <c r="B186" t="s">
+        <v>305</v>
+      </c>
+      <c r="C186" t="s">
+        <v>59</v>
+      </c>
+      <c r="D186" t="s">
+        <v>62</v>
+      </c>
+      <c r="E186" t="s">
+        <v>310</v>
+      </c>
+      <c r="F186" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="187" spans="4:4">
+      <c r="B187" t="s">
+        <v>306</v>
+      </c>
+      <c r="C187" t="s">
+        <v>59</v>
+      </c>
+      <c r="D187" t="s">
+        <v>62</v>
+      </c>
+      <c r="E187" t="s">
+        <v>309</v>
+      </c>
+      <c r="F187" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="188" spans="4:4">
+      <c r="B188" t="s">
+        <v>311</v>
+      </c>
+      <c r="C188" t="s">
+        <v>59</v>
+      </c>
+      <c r="D188" t="s">
+        <v>62</v>
+      </c>
+      <c r="E188" t="s">
+        <v>63</v>
+      </c>
+      <c r="F188" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="189" spans="4:4">
+      <c r="B189" t="s">
+        <v>312</v>
+      </c>
+      <c r="C189" t="s">
+        <v>59</v>
+      </c>
+      <c r="D189" t="s">
+        <v>49</v>
+      </c>
+      <c r="E189" t="s">
+        <v>81</v>
+      </c>
+      <c r="F189" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="190" spans="4:4">
+      <c r="B190" t="s">
+        <v>315</v>
+      </c>
+      <c r="C190" t="s">
+        <v>59</v>
+      </c>
+      <c r="D190" t="s">
+        <v>62</v>
+      </c>
+      <c r="E190" t="s">
+        <v>63</v>
+      </c>
+      <c r="F190" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="191" spans="4:4">
+      <c r="B191" t="s">
+        <v>316</v>
+      </c>
+      <c r="C191" t="s">
+        <v>59</v>
+      </c>
+      <c r="D191" t="s">
+        <v>49</v>
+      </c>
+      <c r="E191" t="s">
+        <v>83</v>
+      </c>
+      <c r="F191" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="192" spans="4:4">
+      <c r="B192" t="s">
+        <v>319</v>
+      </c>
+      <c r="C192" t="s">
+        <v>59</v>
+      </c>
+      <c r="D192" t="s">
+        <v>62</v>
+      </c>
+      <c r="E192" t="s">
+        <v>63</v>
+      </c>
+      <c r="F192" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="193" spans="4:4">
+      <c r="B193" t="s">
+        <v>320</v>
+      </c>
+      <c r="C193" t="s">
+        <v>59</v>
+      </c>
+      <c r="D193" t="s">
+        <v>49</v>
+      </c>
+      <c r="E193" t="s">
+        <v>84</v>
+      </c>
+      <c r="F193" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="194" spans="4:4">
+      <c r="B194" t="s">
+        <v>321</v>
+      </c>
+      <c r="C194" t="s">
+        <v>59</v>
+      </c>
+      <c r="D194" t="s">
+        <v>62</v>
+      </c>
+      <c r="E194" t="s">
+        <v>63</v>
+      </c>
+      <c r="F194" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="195" spans="4:4">
+      <c r="B195" t="s">
+        <v>322</v>
+      </c>
+      <c r="C195" t="s">
+        <v>59</v>
+      </c>
+      <c r="D195" t="s">
+        <v>49</v>
+      </c>
+      <c r="E195" t="s">
+        <v>82</v>
+      </c>
+      <c r="F195" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="196" spans="4:4">
+      <c r="B196" t="s">
+        <v>324</v>
+      </c>
+      <c r="C196" t="s">
+        <v>59</v>
+      </c>
+      <c r="D196" t="s">
+        <v>62</v>
+      </c>
+      <c r="E196" t="s">
+        <v>63</v>
+      </c>
+      <c r="F196" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="197" spans="4:4">
+      <c r="B197" t="s">
+        <v>325</v>
+      </c>
+      <c r="C197" t="s">
+        <v>59</v>
+      </c>
+      <c r="D197" t="s">
+        <v>49</v>
+      </c>
+      <c r="E197" t="s">
+        <v>91</v>
+      </c>
+      <c r="F197" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="198" spans="4:4">
+      <c r="B198" t="s">
+        <v>326</v>
+      </c>
+      <c r="C198" t="s">
+        <v>59</v>
+      </c>
+      <c r="D198" t="s">
+        <v>62</v>
+      </c>
+      <c r="E198" t="s">
+        <v>63</v>
+      </c>
+      <c r="F198" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="199" spans="4:4">
+      <c r="B199" t="s">
+        <v>327</v>
+      </c>
+      <c r="C199" t="s">
+        <v>59</v>
+      </c>
+      <c r="D199" t="s">
+        <v>49</v>
+      </c>
+      <c r="E199" t="s">
+        <v>91</v>
+      </c>
+      <c r="F199" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="200" spans="4:4">
+      <c r="B200" t="s">
+        <v>328</v>
+      </c>
+      <c r="C200" t="s">
+        <v>59</v>
+      </c>
+      <c r="D200" t="s">
+        <v>62</v>
+      </c>
+      <c r="E200" t="s">
+        <v>63</v>
+      </c>
+      <c r="F200" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="201" spans="4:4">
+      <c r="B201" t="s">
+        <v>329</v>
+      </c>
+      <c r="C201" t="s">
+        <v>59</v>
+      </c>
+      <c r="D201" t="s">
+        <v>49</v>
+      </c>
+      <c r="E201" t="s">
+        <v>91</v>
+      </c>
+      <c r="F201" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="202" spans="4:4">
+      <c r="B202" t="s">
+        <v>330</v>
+      </c>
+      <c r="C202" t="s">
+        <v>59</v>
+      </c>
+      <c r="D202" t="s">
+        <v>62</v>
+      </c>
+      <c r="E202" t="s">
+        <v>63</v>
+      </c>
+      <c r="F202" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="203" spans="4:4">
+      <c r="B203" t="s">
+        <v>331</v>
+      </c>
+      <c r="C203" t="s">
+        <v>59</v>
+      </c>
+      <c r="D203" t="s">
+        <v>49</v>
+      </c>
+      <c r="E203" t="s">
+        <v>91</v>
+      </c>
+      <c r="F203" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="204" spans="4:4">
+      <c r="B204" t="s">
+        <v>332</v>
+      </c>
+      <c r="C204" t="s">
+        <v>59</v>
+      </c>
+      <c r="D204" t="s">
+        <v>62</v>
+      </c>
+      <c r="E204" t="s">
+        <v>63</v>
+      </c>
+      <c r="F204" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="205" spans="4:4">
+      <c r="B205" t="s">
+        <v>333</v>
+      </c>
+      <c r="C205" t="s">
+        <v>59</v>
+      </c>
+      <c r="D205" t="s">
+        <v>49</v>
+      </c>
+      <c r="E205" t="s">
+        <v>91</v>
+      </c>
+      <c r="F205" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="206" spans="4:4">
+      <c r="B206" t="s">
+        <v>334</v>
+      </c>
+      <c r="C206" t="s">
+        <v>59</v>
+      </c>
+      <c r="D206" t="s">
+        <v>62</v>
+      </c>
+      <c r="E206" t="s">
+        <v>63</v>
+      </c>
+      <c r="F206" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="207" spans="4:4">
+      <c r="B207" t="s">
+        <v>335</v>
+      </c>
+      <c r="C207" t="s">
+        <v>59</v>
+      </c>
+      <c r="D207" t="s">
+        <v>49</v>
+      </c>
+      <c r="E207" t="s">
+        <v>91</v>
+      </c>
+      <c r="F207" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="208" spans="4:4">
+      <c r="B208" t="s">
+        <v>336</v>
+      </c>
+      <c r="C208" t="s">
+        <v>59</v>
+      </c>
+      <c r="D208" t="s">
+        <v>62</v>
+      </c>
+      <c r="E208" t="s">
+        <v>63</v>
+      </c>
+      <c r="F208" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="209" spans="4:4">
+      <c r="B209" t="s">
+        <v>337</v>
+      </c>
+      <c r="C209" t="s">
+        <v>59</v>
+      </c>
+      <c r="D209" t="s">
+        <v>49</v>
+      </c>
+      <c r="E209" t="s">
+        <v>91</v>
+      </c>
+      <c r="F209" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="210" spans="4:4">
+      <c r="B210" t="s">
+        <v>338</v>
+      </c>
+      <c r="C210" t="s">
+        <v>59</v>
+      </c>
+      <c r="D210" t="s">
+        <v>62</v>
+      </c>
+      <c r="E210" t="s">
+        <v>63</v>
+      </c>
+      <c r="F210" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="211" spans="4:4">
+      <c r="B211" t="s">
+        <v>339</v>
+      </c>
+      <c r="C211" t="s">
+        <v>59</v>
+      </c>
+      <c r="D211" t="s">
+        <v>49</v>
+      </c>
+      <c r="E211" t="s">
+        <v>91</v>
+      </c>
+      <c r="F211" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="212" spans="4:4">
+      <c r="B212" t="s">
+        <v>340</v>
+      </c>
+      <c r="C212" t="s">
+        <v>59</v>
+      </c>
+      <c r="D212" t="s">
+        <v>62</v>
+      </c>
+      <c r="E212" t="s">
+        <v>63</v>
+      </c>
+      <c r="F212" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="213" spans="4:4">
+      <c r="B213" t="s">
+        <v>341</v>
+      </c>
+      <c r="C213" t="s">
+        <v>59</v>
+      </c>
+      <c r="D213" t="s">
+        <v>49</v>
+      </c>
+      <c r="E213" t="s">
+        <v>84</v>
+      </c>
+      <c r="F213" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="214" spans="4:4">
+      <c r="B214" t="s">
+        <v>342</v>
+      </c>
+      <c r="C214" t="s">
+        <v>59</v>
+      </c>
+      <c r="D214" t="s">
+        <v>62</v>
+      </c>
+      <c r="E214" t="s">
+        <v>63</v>
+      </c>
+      <c r="F214" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="215" spans="4:4">
+      <c r="B215" t="s">
+        <v>343</v>
+      </c>
+      <c r="C215" t="s">
+        <v>59</v>
+      </c>
+      <c r="D215" t="s">
+        <v>49</v>
+      </c>
+      <c r="E215" t="s">
+        <v>83</v>
+      </c>
+      <c r="F215" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="216" spans="4:4">
+      <c r="B216" t="s">
+        <v>344</v>
+      </c>
+      <c r="C216" t="s">
+        <v>59</v>
+      </c>
+      <c r="D216" t="s">
+        <v>62</v>
+      </c>
+      <c r="E216" t="s">
+        <v>63</v>
+      </c>
+      <c r="F216" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="217" spans="4:4">
+      <c r="B217" t="s">
+        <v>345</v>
+      </c>
+      <c r="C217" t="s">
+        <v>59</v>
+      </c>
+      <c r="D217" t="s">
+        <v>49</v>
+      </c>
+      <c r="E217" t="s">
+        <v>81</v>
+      </c>
+      <c r="F217" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="218" spans="4:4">
+      <c r="B218" t="s">
+        <v>346</v>
+      </c>
+      <c r="C218" t="s">
+        <v>59</v>
+      </c>
+      <c r="D218" t="s">
+        <v>62</v>
+      </c>
+      <c r="E218" t="s">
+        <v>63</v>
+      </c>
+      <c r="F218" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="219" spans="4:4">
+      <c r="B219" t="s">
+        <v>347</v>
+      </c>
+      <c r="C219" t="s">
+        <v>59</v>
+      </c>
+      <c r="D219" t="s">
+        <v>49</v>
+      </c>
+      <c r="E219" t="s">
+        <v>82</v>
+      </c>
+      <c r="F219" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="220" spans="4:4">
+      <c r="B220" t="s">
+        <v>348</v>
+      </c>
+      <c r="C220" t="s">
+        <v>59</v>
+      </c>
+      <c r="D220" t="s">
+        <v>62</v>
+      </c>
+      <c r="E220" t="s">
+        <v>63</v>
+      </c>
+      <c r="F220" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="221" spans="4:4">
+      <c r="B221" t="s">
+        <v>349</v>
+      </c>
+      <c r="C221" t="s">
+        <v>59</v>
+      </c>
+      <c r="D221" t="s">
+        <v>49</v>
+      </c>
+      <c r="E221" t="s">
+        <v>84</v>
+      </c>
+      <c r="F221" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="222" spans="4:4">
+      <c r="B222" t="s">
+        <v>350</v>
+      </c>
+      <c r="C222" t="s">
+        <v>59</v>
+      </c>
+      <c r="D222" t="s">
+        <v>62</v>
+      </c>
+      <c r="E222" t="s">
+        <v>63</v>
+      </c>
+      <c r="F222" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="223" spans="4:4">
+      <c r="B223" t="s">
+        <v>351</v>
+      </c>
+      <c r="C223" t="s">
+        <v>59</v>
+      </c>
+      <c r="D223" t="s">
+        <v>49</v>
+      </c>
+      <c r="E223" t="s">
+        <v>83</v>
+      </c>
+      <c r="F223" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="224" spans="4:4">
+      <c r="B224" t="s">
+        <v>352</v>
+      </c>
+      <c r="C224" t="s">
+        <v>59</v>
+      </c>
+      <c r="D224" t="s">
+        <v>62</v>
+      </c>
+      <c r="E224" t="s">
+        <v>63</v>
+      </c>
+      <c r="F224" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="225" spans="4:4">
+      <c r="B225" t="s">
+        <v>353</v>
+      </c>
+      <c r="C225" t="s">
+        <v>59</v>
+      </c>
+      <c r="D225" t="s">
+        <v>49</v>
+      </c>
+      <c r="E225" t="s">
+        <v>81</v>
+      </c>
+      <c r="F225" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="226" spans="4:4">
+      <c r="B226" t="s">
+        <v>354</v>
+      </c>
+      <c r="C226" t="s">
+        <v>59</v>
+      </c>
+      <c r="D226" t="s">
+        <v>62</v>
+      </c>
+      <c r="E226" t="s">
+        <v>63</v>
+      </c>
+      <c r="F226" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="227" spans="4:4">
+      <c r="B227" t="s">
+        <v>355</v>
+      </c>
+      <c r="C227" t="s">
+        <v>59</v>
+      </c>
+      <c r="D227" t="s">
+        <v>49</v>
+      </c>
+      <c r="E227" t="s">
+        <v>82</v>
+      </c>
+      <c r="F227" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="228" spans="4:4">
+      <c r="B228" t="s">
+        <v>356</v>
+      </c>
+      <c r="C228" t="s">
+        <v>59</v>
+      </c>
+      <c r="D228" t="s">
+        <v>62</v>
+      </c>
+      <c r="E228" t="s">
+        <v>63</v>
+      </c>
+      <c r="F228" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="229" spans="4:4">
+      <c r="B229" t="s">
+        <v>358</v>
+      </c>
+      <c r="C229" t="s">
+        <v>59</v>
+      </c>
+      <c r="D229" t="s">
+        <v>62</v>
+      </c>
+      <c r="E229" t="s">
+        <v>63</v>
+      </c>
+      <c r="F229" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="230" spans="4:4">
+      <c r="B230" t="s">
+        <v>359</v>
+      </c>
+      <c r="C230" t="s">
+        <v>59</v>
+      </c>
+      <c r="D230" t="s">
+        <v>49</v>
+      </c>
+      <c r="E230" t="s">
+        <v>91</v>
+      </c>
+      <c r="F230" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="231" spans="4:4">
+      <c r="B231" t="s">
+        <v>360</v>
+      </c>
+      <c r="C231" t="s">
+        <v>59</v>
+      </c>
+      <c r="D231" t="s">
+        <v>62</v>
+      </c>
+      <c r="E231" t="s">
+        <v>63</v>
+      </c>
+      <c r="F231" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="232" spans="4:4">
+      <c r="B232" t="s">
+        <v>361</v>
+      </c>
+      <c r="C232" t="s">
+        <v>59</v>
+      </c>
+      <c r="D232" t="s">
+        <v>49</v>
+      </c>
+      <c r="E232" t="s">
+        <v>91</v>
+      </c>
+      <c r="F232" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="233" spans="4:4">
+      <c r="B233" t="s">
+        <v>362</v>
+      </c>
+      <c r="C233" t="s">
+        <v>59</v>
+      </c>
+      <c r="D233" t="s">
+        <v>62</v>
+      </c>
+      <c r="E233" t="s">
+        <v>63</v>
+      </c>
+      <c r="F233" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="234" spans="4:4">
+      <c r="B234" t="s">
+        <v>363</v>
+      </c>
+      <c r="C234" t="s">
+        <v>59</v>
+      </c>
+      <c r="D234" t="s">
+        <v>49</v>
+      </c>
+      <c r="E234" t="s">
+        <v>91</v>
+      </c>
+      <c r="F234" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="235" spans="4:4">
+      <c r="B235" t="s">
+        <v>364</v>
+      </c>
+      <c r="C235" t="s">
+        <v>59</v>
+      </c>
+      <c r="D235" t="s">
+        <v>62</v>
+      </c>
+      <c r="E235" t="s">
+        <v>63</v>
+      </c>
+      <c r="F235" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="236" spans="4:4">
+      <c r="B236" t="s">
+        <v>365</v>
+      </c>
+      <c r="C236" t="s">
+        <v>59</v>
+      </c>
+      <c r="D236" t="s">
+        <v>49</v>
+      </c>
+      <c r="E236" t="s">
+        <v>91</v>
+      </c>
+      <c r="F236" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="237" spans="4:4">
+      <c r="B237" t="s">
+        <v>366</v>
+      </c>
+      <c r="C237" t="s">
+        <v>59</v>
+      </c>
+      <c r="D237" t="s">
+        <v>62</v>
+      </c>
+      <c r="E237" t="s">
+        <v>63</v>
+      </c>
+      <c r="F237" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="238" spans="4:4">
+      <c r="B238" t="s">
+        <v>367</v>
+      </c>
+      <c r="C238" t="s">
+        <v>59</v>
+      </c>
+      <c r="D238" t="s">
+        <v>49</v>
+      </c>
+      <c r="E238" t="s">
+        <v>91</v>
+      </c>
+      <c r="F238" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="239" spans="4:4">
+      <c r="B239" t="s">
+        <v>368</v>
+      </c>
+      <c r="C239" t="s">
+        <v>59</v>
+      </c>
+      <c r="D239" t="s">
+        <v>62</v>
+      </c>
+      <c r="E239" t="s">
+        <v>63</v>
+      </c>
+      <c r="F239" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="240" spans="4:4">
+      <c r="B240" t="s">
+        <v>369</v>
+      </c>
+      <c r="C240" t="s">
+        <v>59</v>
+      </c>
+      <c r="D240" t="s">
+        <v>49</v>
+      </c>
+      <c r="E240" t="s">
+        <v>91</v>
+      </c>
+      <c r="F240" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="241" spans="4:4">
+      <c r="B241" t="s">
+        <v>370</v>
+      </c>
+      <c r="C241" t="s">
+        <v>59</v>
+      </c>
+      <c r="D241" t="s">
+        <v>62</v>
+      </c>
+      <c r="E241" t="s">
+        <v>63</v>
+      </c>
+      <c r="F241" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="242" spans="4:4">
+      <c r="B242" t="s">
+        <v>371</v>
+      </c>
+      <c r="C242" t="s">
+        <v>59</v>
+      </c>
+      <c r="D242" t="s">
+        <v>49</v>
+      </c>
+      <c r="E242" t="s">
+        <v>91</v>
+      </c>
+      <c r="F242" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="243" spans="4:4">
+      <c r="B243" t="s">
+        <v>373</v>
+      </c>
+      <c r="C243" t="s">
+        <v>59</v>
+      </c>
+      <c r="D243" t="s">
+        <v>49</v>
+      </c>
+      <c r="E243" t="s">
+        <v>91</v>
+      </c>
+      <c r="F243" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="244" spans="4:4"/>
     <row r="245" spans="4:4"/>
     <row r="246" spans="4:4"/>

</xml_diff>

<commit_message>
schermo funziona da aggiungere il pwm
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="54">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1441,7 +1441,7 @@
         <v>41</v>
       </c>
       <c r="D5">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E5">
         <v>4</v>

</xml_diff>

<commit_message>
grafica sistemata, rifatte le due schermate di debug (da controllare la logica)
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218231" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296845" uniqueCount="463">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1395,6 +1395,15 @@
   </si>
   <si>
     <t xml:space="preserve">.&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Littl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LittleMedium</t>
   </si>
 </sst>
 </file>
@@ -2759,6 +2768,25 @@
       </c>
     </row>
     <row r="8" spans="2:15">
+      <c r="B8" t="s">
+        <v>462</v>
+      </c>
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8">
+        <v>45</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" t="s">
+        <v>455</v>
+      </c>
       <c r="I8"/>
       <c r="K8" s="8" t="s">
         <v>16</v>
@@ -5886,7 +5914,7 @@
         <v>311</v>
       </c>
       <c r="C180" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D180" t="s">
         <v>62</v>
@@ -5903,7 +5931,7 @@
         <v>312</v>
       </c>
       <c r="C181" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D181" t="s">
         <v>49</v>
@@ -5920,7 +5948,7 @@
         <v>315</v>
       </c>
       <c r="C182" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D182" t="s">
         <v>62</v>
@@ -5937,7 +5965,7 @@
         <v>316</v>
       </c>
       <c r="C183" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D183" t="s">
         <v>49</v>
@@ -5954,7 +5982,7 @@
         <v>319</v>
       </c>
       <c r="C184" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D184" t="s">
         <v>62</v>
@@ -5971,7 +5999,7 @@
         <v>320</v>
       </c>
       <c r="C185" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D185" t="s">
         <v>49</v>
@@ -5988,7 +6016,7 @@
         <v>321</v>
       </c>
       <c r="C186" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D186" t="s">
         <v>62</v>
@@ -6005,7 +6033,7 @@
         <v>322</v>
       </c>
       <c r="C187" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D187" t="s">
         <v>49</v>
@@ -6022,7 +6050,7 @@
         <v>324</v>
       </c>
       <c r="C188" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D188" t="s">
         <v>62</v>
@@ -6039,7 +6067,7 @@
         <v>325</v>
       </c>
       <c r="C189" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D189" t="s">
         <v>49</v>
@@ -6056,7 +6084,7 @@
         <v>326</v>
       </c>
       <c r="C190" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D190" t="s">
         <v>62</v>
@@ -6073,7 +6101,7 @@
         <v>327</v>
       </c>
       <c r="C191" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D191" t="s">
         <v>49</v>
@@ -6090,7 +6118,7 @@
         <v>328</v>
       </c>
       <c r="C192" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D192" t="s">
         <v>62</v>
@@ -6107,7 +6135,7 @@
         <v>329</v>
       </c>
       <c r="C193" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D193" t="s">
         <v>49</v>
@@ -6124,7 +6152,7 @@
         <v>330</v>
       </c>
       <c r="C194" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D194" t="s">
         <v>62</v>
@@ -6141,7 +6169,7 @@
         <v>331</v>
       </c>
       <c r="C195" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D195" t="s">
         <v>49</v>
@@ -6158,7 +6186,7 @@
         <v>332</v>
       </c>
       <c r="C196" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D196" t="s">
         <v>62</v>
@@ -6175,7 +6203,7 @@
         <v>333</v>
       </c>
       <c r="C197" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D197" t="s">
         <v>49</v>
@@ -6192,7 +6220,7 @@
         <v>334</v>
       </c>
       <c r="C198" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D198" t="s">
         <v>62</v>
@@ -6209,7 +6237,7 @@
         <v>335</v>
       </c>
       <c r="C199" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D199" t="s">
         <v>49</v>
@@ -6226,7 +6254,7 @@
         <v>336</v>
       </c>
       <c r="C200" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D200" t="s">
         <v>62</v>
@@ -6243,7 +6271,7 @@
         <v>337</v>
       </c>
       <c r="C201" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D201" t="s">
         <v>49</v>
@@ -6260,7 +6288,7 @@
         <v>338</v>
       </c>
       <c r="C202" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D202" t="s">
         <v>62</v>
@@ -6277,7 +6305,7 @@
         <v>339</v>
       </c>
       <c r="C203" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D203" t="s">
         <v>49</v>
@@ -6294,7 +6322,7 @@
         <v>340</v>
       </c>
       <c r="C204" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D204" t="s">
         <v>62</v>
@@ -6311,7 +6339,7 @@
         <v>341</v>
       </c>
       <c r="C205" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D205" t="s">
         <v>49</v>
@@ -6328,7 +6356,7 @@
         <v>342</v>
       </c>
       <c r="C206" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D206" t="s">
         <v>62</v>
@@ -6345,7 +6373,7 @@
         <v>343</v>
       </c>
       <c r="C207" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D207" t="s">
         <v>49</v>
@@ -6362,7 +6390,7 @@
         <v>344</v>
       </c>
       <c r="C208" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D208" t="s">
         <v>62</v>
@@ -6379,7 +6407,7 @@
         <v>345</v>
       </c>
       <c r="C209" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D209" t="s">
         <v>49</v>
@@ -6396,7 +6424,7 @@
         <v>346</v>
       </c>
       <c r="C210" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D210" t="s">
         <v>62</v>
@@ -6413,7 +6441,7 @@
         <v>347</v>
       </c>
       <c r="C211" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D211" t="s">
         <v>49</v>
@@ -6430,7 +6458,7 @@
         <v>348</v>
       </c>
       <c r="C212" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D212" t="s">
         <v>62</v>
@@ -6447,7 +6475,7 @@
         <v>349</v>
       </c>
       <c r="C213" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D213" t="s">
         <v>49</v>
@@ -6464,7 +6492,7 @@
         <v>350</v>
       </c>
       <c r="C214" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D214" t="s">
         <v>62</v>
@@ -6481,7 +6509,7 @@
         <v>351</v>
       </c>
       <c r="C215" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D215" t="s">
         <v>49</v>
@@ -6498,7 +6526,7 @@
         <v>352</v>
       </c>
       <c r="C216" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D216" t="s">
         <v>62</v>
@@ -6515,7 +6543,7 @@
         <v>353</v>
       </c>
       <c r="C217" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D217" t="s">
         <v>49</v>
@@ -6532,7 +6560,7 @@
         <v>354</v>
       </c>
       <c r="C218" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D218" t="s">
         <v>62</v>
@@ -6549,7 +6577,7 @@
         <v>355</v>
       </c>
       <c r="C219" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D219" t="s">
         <v>49</v>
@@ -6566,7 +6594,7 @@
         <v>356</v>
       </c>
       <c r="C220" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D220" t="s">
         <v>62</v>
@@ -6583,7 +6611,7 @@
         <v>358</v>
       </c>
       <c r="C221" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D221" t="s">
         <v>62</v>
@@ -6600,7 +6628,7 @@
         <v>359</v>
       </c>
       <c r="C222" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D222" t="s">
         <v>49</v>
@@ -6617,7 +6645,7 @@
         <v>360</v>
       </c>
       <c r="C223" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D223" t="s">
         <v>62</v>
@@ -6634,7 +6662,7 @@
         <v>361</v>
       </c>
       <c r="C224" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D224" t="s">
         <v>49</v>
@@ -6651,7 +6679,7 @@
         <v>362</v>
       </c>
       <c r="C225" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D225" t="s">
         <v>62</v>
@@ -6668,7 +6696,7 @@
         <v>363</v>
       </c>
       <c r="C226" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D226" t="s">
         <v>49</v>
@@ -6685,7 +6713,7 @@
         <v>364</v>
       </c>
       <c r="C227" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D227" t="s">
         <v>62</v>
@@ -6702,7 +6730,7 @@
         <v>365</v>
       </c>
       <c r="C228" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D228" t="s">
         <v>49</v>
@@ -6719,7 +6747,7 @@
         <v>366</v>
       </c>
       <c r="C229" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D229" t="s">
         <v>62</v>
@@ -6736,7 +6764,7 @@
         <v>367</v>
       </c>
       <c r="C230" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D230" t="s">
         <v>49</v>
@@ -6753,7 +6781,7 @@
         <v>368</v>
       </c>
       <c r="C231" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D231" t="s">
         <v>62</v>
@@ -6770,7 +6798,7 @@
         <v>369</v>
       </c>
       <c r="C232" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D232" t="s">
         <v>49</v>
@@ -6787,7 +6815,7 @@
         <v>370</v>
       </c>
       <c r="C233" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D233" t="s">
         <v>62</v>
@@ -6804,7 +6832,7 @@
         <v>371</v>
       </c>
       <c r="C234" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D234" t="s">
         <v>49</v>
@@ -6821,7 +6849,7 @@
         <v>373</v>
       </c>
       <c r="C235" t="s">
-        <v>59</v>
+        <v>462</v>
       </c>
       <c r="D235" t="s">
         <v>49</v>
@@ -6844,7 +6872,7 @@
         <v>49</v>
       </c>
       <c r="E236" t="s">
-        <v>458</v>
+        <v>63</v>
       </c>
       <c r="F236" t="s">
         <v>50</v>
@@ -6901,24 +6929,312 @@
         <v>50</v>
       </c>
     </row>
-    <row r="240" spans="4:4"/>
-    <row r="241" spans="4:4"/>
-    <row r="242" spans="4:4"/>
-    <row r="243" spans="4:4"/>
-    <row r="244" spans="4:4"/>
-    <row r="245" spans="4:4"/>
-    <row r="246" spans="4:4"/>
-    <row r="247" spans="4:4"/>
-    <row r="248" spans="4:4"/>
-    <row r="249" spans="4:4"/>
-    <row r="250" spans="4:4"/>
-    <row r="251" spans="4:4"/>
-    <row r="252" spans="4:4"/>
-    <row r="253" spans="4:4"/>
-    <row r="254" spans="4:4"/>
-    <row r="255" spans="4:4"/>
-    <row r="256" spans="4:4"/>
-    <row r="257" spans="4:4"/>
+    <row r="240" spans="4:4">
+      <c r="B240" t="s">
+        <v>380</v>
+      </c>
+      <c r="C240" t="s">
+        <v>105</v>
+      </c>
+      <c r="D240" t="s">
+        <v>49</v>
+      </c>
+      <c r="E240" t="s">
+        <v>106</v>
+      </c>
+      <c r="F240" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="241" spans="4:4">
+      <c r="B241" t="s">
+        <v>381</v>
+      </c>
+      <c r="C241" t="s">
+        <v>105</v>
+      </c>
+      <c r="D241" t="s">
+        <v>49</v>
+      </c>
+      <c r="E241" t="s">
+        <v>106</v>
+      </c>
+      <c r="F241" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="242" spans="4:4">
+      <c r="B242" t="s">
+        <v>382</v>
+      </c>
+      <c r="C242" t="s">
+        <v>105</v>
+      </c>
+      <c r="D242" t="s">
+        <v>49</v>
+      </c>
+      <c r="E242" t="s">
+        <v>106</v>
+      </c>
+      <c r="F242" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="243" spans="4:4">
+      <c r="B243" t="s">
+        <v>383</v>
+      </c>
+      <c r="C243" t="s">
+        <v>105</v>
+      </c>
+      <c r="D243" t="s">
+        <v>49</v>
+      </c>
+      <c r="E243" t="s">
+        <v>106</v>
+      </c>
+      <c r="F243" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="244" spans="4:4">
+      <c r="B244" t="s">
+        <v>384</v>
+      </c>
+      <c r="C244" t="s">
+        <v>462</v>
+      </c>
+      <c r="D244" t="s">
+        <v>62</v>
+      </c>
+      <c r="E244" t="s">
+        <v>63</v>
+      </c>
+      <c r="F244" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="245" spans="4:4">
+      <c r="B245" t="s">
+        <v>385</v>
+      </c>
+      <c r="C245" t="s">
+        <v>462</v>
+      </c>
+      <c r="D245" t="s">
+        <v>49</v>
+      </c>
+      <c r="E245" t="s">
+        <v>77</v>
+      </c>
+      <c r="F245" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="246" spans="4:4">
+      <c r="B246" t="s">
+        <v>386</v>
+      </c>
+      <c r="C246" t="s">
+        <v>462</v>
+      </c>
+      <c r="D246" t="s">
+        <v>62</v>
+      </c>
+      <c r="E246" t="s">
+        <v>63</v>
+      </c>
+      <c r="F246" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="247" spans="4:4">
+      <c r="B247" t="s">
+        <v>387</v>
+      </c>
+      <c r="C247" t="s">
+        <v>462</v>
+      </c>
+      <c r="D247" t="s">
+        <v>49</v>
+      </c>
+      <c r="E247" t="s">
+        <v>91</v>
+      </c>
+      <c r="F247" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="248" spans="4:4">
+      <c r="B248" t="s">
+        <v>388</v>
+      </c>
+      <c r="C248" t="s">
+        <v>462</v>
+      </c>
+      <c r="D248" t="s">
+        <v>62</v>
+      </c>
+      <c r="E248" t="s">
+        <v>63</v>
+      </c>
+      <c r="F248" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="249" spans="4:4">
+      <c r="B249" t="s">
+        <v>389</v>
+      </c>
+      <c r="C249" t="s">
+        <v>462</v>
+      </c>
+      <c r="D249" t="s">
+        <v>49</v>
+      </c>
+      <c r="E249" t="s">
+        <v>91</v>
+      </c>
+      <c r="F249" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="250" spans="4:4">
+      <c r="B250" t="s">
+        <v>390</v>
+      </c>
+      <c r="C250" t="s">
+        <v>462</v>
+      </c>
+      <c r="D250" t="s">
+        <v>62</v>
+      </c>
+      <c r="E250" t="s">
+        <v>63</v>
+      </c>
+      <c r="F250" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="251" spans="4:4">
+      <c r="B251" t="s">
+        <v>391</v>
+      </c>
+      <c r="C251" t="s">
+        <v>462</v>
+      </c>
+      <c r="D251" t="s">
+        <v>49</v>
+      </c>
+      <c r="E251" t="s">
+        <v>77</v>
+      </c>
+      <c r="F251" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="252" spans="4:4">
+      <c r="B252" t="s">
+        <v>392</v>
+      </c>
+      <c r="C252" t="s">
+        <v>462</v>
+      </c>
+      <c r="D252" t="s">
+        <v>62</v>
+      </c>
+      <c r="E252" t="s">
+        <v>63</v>
+      </c>
+      <c r="F252" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="253" spans="4:4">
+      <c r="B253" t="s">
+        <v>393</v>
+      </c>
+      <c r="C253" t="s">
+        <v>462</v>
+      </c>
+      <c r="D253" t="s">
+        <v>49</v>
+      </c>
+      <c r="E253" t="s">
+        <v>91</v>
+      </c>
+      <c r="F253" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="254" spans="4:4">
+      <c r="B254" t="s">
+        <v>394</v>
+      </c>
+      <c r="C254" t="s">
+        <v>462</v>
+      </c>
+      <c r="D254" t="s">
+        <v>62</v>
+      </c>
+      <c r="E254" t="s">
+        <v>63</v>
+      </c>
+      <c r="F254" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="255" spans="4:4">
+      <c r="B255" t="s">
+        <v>395</v>
+      </c>
+      <c r="C255" t="s">
+        <v>462</v>
+      </c>
+      <c r="D255" t="s">
+        <v>49</v>
+      </c>
+      <c r="E255" t="s">
+        <v>77</v>
+      </c>
+      <c r="F255" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="256" spans="4:4">
+      <c r="B256" t="s">
+        <v>396</v>
+      </c>
+      <c r="C256" t="s">
+        <v>462</v>
+      </c>
+      <c r="D256" t="s">
+        <v>62</v>
+      </c>
+      <c r="E256" t="s">
+        <v>63</v>
+      </c>
+      <c r="F256" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="257" spans="4:4">
+      <c r="B257" t="s">
+        <v>397</v>
+      </c>
+      <c r="C257" t="s">
+        <v>462</v>
+      </c>
+      <c r="D257" t="s">
+        <v>49</v>
+      </c>
+      <c r="E257" t="s">
+        <v>91</v>
+      </c>
+      <c r="F257" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="258" spans="4:4"/>
     <row r="259" spans="4:4"/>
     <row r="260" spans="4:4"/>

</xml_diff>

<commit_message>
popup cambio modalità e clutch ok
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296845" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332984" uniqueCount="465">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1404,6 +1404,12 @@
   </si>
   <si>
     <t xml:space="preserve">LittleMedium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">READY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
   </si>
 </sst>
 </file>
@@ -6863,13 +6869,13 @@
     </row>
     <row r="236" spans="4:4">
       <c r="B236" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="C236" t="s">
         <v>105</v>
       </c>
       <c r="D236" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E236" t="s">
         <v>63</v>
@@ -6880,7 +6886,7 @@
     </row>
     <row r="237" spans="4:4">
       <c r="B237" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C237" t="s">
         <v>105</v>
@@ -6889,7 +6895,7 @@
         <v>49</v>
       </c>
       <c r="E237" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="F237" t="s">
         <v>50</v>
@@ -6897,13 +6903,13 @@
     </row>
     <row r="238" spans="4:4">
       <c r="B238" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C238" t="s">
-        <v>105</v>
+        <v>462</v>
       </c>
       <c r="D238" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E238" t="s">
         <v>63</v>
@@ -6914,16 +6920,16 @@
     </row>
     <row r="239" spans="4:4">
       <c r="B239" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="C239" t="s">
-        <v>105</v>
+        <v>462</v>
       </c>
       <c r="D239" t="s">
         <v>49</v>
       </c>
       <c r="E239" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="F239" t="s">
         <v>50</v>
@@ -6931,16 +6937,16 @@
     </row>
     <row r="240" spans="4:4">
       <c r="B240" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C240" t="s">
-        <v>105</v>
+        <v>462</v>
       </c>
       <c r="D240" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E240" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="F240" t="s">
         <v>50</v>
@@ -6948,16 +6954,16 @@
     </row>
     <row r="241" spans="4:4">
       <c r="B241" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="C241" t="s">
-        <v>105</v>
+        <v>462</v>
       </c>
       <c r="D241" t="s">
         <v>49</v>
       </c>
       <c r="E241" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="F241" t="s">
         <v>50</v>
@@ -6965,16 +6971,16 @@
     </row>
     <row r="242" spans="4:4">
       <c r="B242" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="C242" t="s">
-        <v>105</v>
+        <v>462</v>
       </c>
       <c r="D242" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E242" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="F242" t="s">
         <v>50</v>
@@ -6982,16 +6988,16 @@
     </row>
     <row r="243" spans="4:4">
       <c r="B243" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="C243" t="s">
-        <v>105</v>
+        <v>462</v>
       </c>
       <c r="D243" t="s">
         <v>49</v>
       </c>
       <c r="E243" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="F243" t="s">
         <v>50</v>
@@ -6999,7 +7005,7 @@
     </row>
     <row r="244" spans="4:4">
       <c r="B244" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="C244" t="s">
         <v>462</v>
@@ -7016,7 +7022,7 @@
     </row>
     <row r="245" spans="4:4">
       <c r="B245" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="C245" t="s">
         <v>462</v>
@@ -7033,7 +7039,7 @@
     </row>
     <row r="246" spans="4:4">
       <c r="B246" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="C246" t="s">
         <v>462</v>
@@ -7050,7 +7056,7 @@
     </row>
     <row r="247" spans="4:4">
       <c r="B247" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="C247" t="s">
         <v>462</v>
@@ -7067,7 +7073,7 @@
     </row>
     <row r="248" spans="4:4">
       <c r="B248" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="C248" t="s">
         <v>462</v>
@@ -7084,7 +7090,7 @@
     </row>
     <row r="249" spans="4:4">
       <c r="B249" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="C249" t="s">
         <v>462</v>
@@ -7093,7 +7099,7 @@
         <v>49</v>
       </c>
       <c r="E249" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F249" t="s">
         <v>50</v>
@@ -7101,7 +7107,7 @@
     </row>
     <row r="250" spans="4:4">
       <c r="B250" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="C250" t="s">
         <v>462</v>
@@ -7118,7 +7124,7 @@
     </row>
     <row r="251" spans="4:4">
       <c r="B251" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="C251" t="s">
         <v>462</v>
@@ -7127,7 +7133,7 @@
         <v>49</v>
       </c>
       <c r="E251" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F251" t="s">
         <v>50</v>
@@ -7135,16 +7141,16 @@
     </row>
     <row r="252" spans="4:4">
       <c r="B252" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="C252" t="s">
-        <v>462</v>
+        <v>59</v>
       </c>
       <c r="D252" t="s">
         <v>62</v>
       </c>
       <c r="E252" t="s">
-        <v>63</v>
+        <v>242</v>
       </c>
       <c r="F252" t="s">
         <v>50</v>
@@ -7152,16 +7158,16 @@
     </row>
     <row r="253" spans="4:4">
       <c r="B253" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="C253" t="s">
-        <v>462</v>
+        <v>59</v>
       </c>
       <c r="D253" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E253" t="s">
-        <v>91</v>
+        <v>133</v>
       </c>
       <c r="F253" t="s">
         <v>50</v>
@@ -7169,16 +7175,16 @@
     </row>
     <row r="254" spans="4:4">
       <c r="B254" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="C254" t="s">
-        <v>462</v>
+        <v>59</v>
       </c>
       <c r="D254" t="s">
         <v>62</v>
       </c>
       <c r="E254" t="s">
-        <v>63</v>
+        <v>241</v>
       </c>
       <c r="F254" t="s">
         <v>50</v>
@@ -7186,16 +7192,16 @@
     </row>
     <row r="255" spans="4:4">
       <c r="B255" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="C255" t="s">
-        <v>462</v>
+        <v>59</v>
       </c>
       <c r="D255" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E255" t="s">
-        <v>77</v>
+        <v>170</v>
       </c>
       <c r="F255" t="s">
         <v>50</v>
@@ -7203,10 +7209,10 @@
     </row>
     <row r="256" spans="4:4">
       <c r="B256" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="C256" t="s">
-        <v>462</v>
+        <v>59</v>
       </c>
       <c r="D256" t="s">
         <v>62</v>
@@ -7220,26 +7226,106 @@
     </row>
     <row r="257" spans="4:4">
       <c r="B257" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="C257" t="s">
-        <v>462</v>
+        <v>105</v>
       </c>
       <c r="D257" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E257" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F257" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="258" spans="4:4"/>
-    <row r="259" spans="4:4"/>
-    <row r="260" spans="4:4"/>
-    <row r="261" spans="4:4"/>
-    <row r="262" spans="4:4"/>
+    <row r="258" spans="4:4">
+      <c r="B258" t="s">
+        <v>404</v>
+      </c>
+      <c r="C258" t="s">
+        <v>105</v>
+      </c>
+      <c r="D258" t="s">
+        <v>49</v>
+      </c>
+      <c r="E258" t="s">
+        <v>106</v>
+      </c>
+      <c r="F258" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="259" spans="4:4">
+      <c r="B259" t="s">
+        <v>405</v>
+      </c>
+      <c r="C259" t="s">
+        <v>105</v>
+      </c>
+      <c r="D259" t="s">
+        <v>62</v>
+      </c>
+      <c r="E259" t="s">
+        <v>63</v>
+      </c>
+      <c r="F259" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="260" spans="4:4">
+      <c r="B260" t="s">
+        <v>406</v>
+      </c>
+      <c r="C260" t="s">
+        <v>105</v>
+      </c>
+      <c r="D260" t="s">
+        <v>49</v>
+      </c>
+      <c r="E260" t="s">
+        <v>106</v>
+      </c>
+      <c r="F260" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="261" spans="4:4">
+      <c r="B261" t="s">
+        <v>407</v>
+      </c>
+      <c r="C261" t="s">
+        <v>105</v>
+      </c>
+      <c r="D261" t="s">
+        <v>62</v>
+      </c>
+      <c r="E261" t="s">
+        <v>63</v>
+      </c>
+      <c r="F261" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="262" spans="4:4">
+      <c r="B262" t="s">
+        <v>408</v>
+      </c>
+      <c r="C262" t="s">
+        <v>105</v>
+      </c>
+      <c r="D262" t="s">
+        <v>49</v>
+      </c>
+      <c r="E262" t="s">
+        <v>106</v>
+      </c>
+      <c r="F262" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="263" spans="4:4"/>
     <row r="264" spans="4:4"/>
     <row r="265" spans="4:4"/>

</xml_diff>

<commit_message>
provare acc - grafica sistemata
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332984" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407376" uniqueCount="481">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1410,6 +1410,56 @@
   </si>
   <si>
     <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ciao
+lue&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;READY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium_00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium_Large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;RE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;vaul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roboto-BoldItalic.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roboto-Black.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA</t>
   </si>
 </sst>
 </file>
@@ -2809,6 +2859,26 @@
       <c r="O8" s="11"/>
     </row>
     <row r="9" spans="2:15">
+      <c r="B9" t="s">
+        <v>469</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9">
+        <v>80</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9" t="s">
+        <v>455</v>
+      </c>
+      <c r="I9"/>
       <c r="K9" s="12" t="s">
         <v>14</v>
       </c>
@@ -2826,6 +2896,26 @@
       </c>
     </row>
     <row r="10" spans="2:15">
+      <c r="B10" t="s">
+        <v>473</v>
+      </c>
+      <c r="C10" t="s">
+        <v>475</v>
+      </c>
+      <c r="D10">
+        <v>90</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10" t="s">
+        <v>455</v>
+      </c>
+      <c r="I10"/>
       <c r="K10" s="12" t="s">
         <v>36</v>
       </c>
@@ -7144,7 +7234,7 @@
         <v>398</v>
       </c>
       <c r="C252" t="s">
-        <v>59</v>
+        <v>469</v>
       </c>
       <c r="D252" t="s">
         <v>62</v>
@@ -7161,7 +7251,7 @@
         <v>399</v>
       </c>
       <c r="C253" t="s">
-        <v>59</v>
+        <v>469</v>
       </c>
       <c r="D253" t="s">
         <v>62</v>
@@ -7178,7 +7268,7 @@
         <v>400</v>
       </c>
       <c r="C254" t="s">
-        <v>59</v>
+        <v>469</v>
       </c>
       <c r="D254" t="s">
         <v>62</v>
@@ -7195,7 +7285,7 @@
         <v>401</v>
       </c>
       <c r="C255" t="s">
-        <v>59</v>
+        <v>469</v>
       </c>
       <c r="D255" t="s">
         <v>62</v>
@@ -7212,7 +7302,7 @@
         <v>402</v>
       </c>
       <c r="C256" t="s">
-        <v>59</v>
+        <v>473</v>
       </c>
       <c r="D256" t="s">
         <v>62</v>
@@ -7326,7 +7416,23 @@
         <v>50</v>
       </c>
     </row>
-    <row r="263" spans="4:4"/>
+    <row r="263" spans="4:4">
+      <c r="B263" t="s">
+        <v>409</v>
+      </c>
+      <c r="C263" t="s">
+        <v>473</v>
+      </c>
+      <c r="D263" t="s">
+        <v>49</v>
+      </c>
+      <c r="E263" t="s">
+        <v>480</v>
+      </c>
+      <c r="F263" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="264" spans="4:4"/>
     <row r="265" spans="4:4"/>
     <row r="266" spans="4:4"/>

</xml_diff>

<commit_message>
logica acc ok - logica autox da testare - schermata startup cambiata
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407376" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415343" uniqueCount="482">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1460,6 +1460,9 @@
   </si>
   <si>
     <t xml:space="preserve">AA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;R</t>
   </si>
 </sst>
 </file>
@@ -2903,7 +2906,7 @@
         <v>475</v>
       </c>
       <c r="D10">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -7299,10 +7302,10 @@
     </row>
     <row r="256" spans="4:4">
       <c r="B256" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C256" t="s">
-        <v>473</v>
+        <v>105</v>
       </c>
       <c r="D256" t="s">
         <v>62</v>
@@ -7316,16 +7319,16 @@
     </row>
     <row r="257" spans="4:4">
       <c r="B257" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C257" t="s">
         <v>105</v>
       </c>
       <c r="D257" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E257" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="F257" t="s">
         <v>50</v>
@@ -7333,16 +7336,16 @@
     </row>
     <row r="258" spans="4:4">
       <c r="B258" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C258" t="s">
         <v>105</v>
       </c>
       <c r="D258" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E258" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="F258" t="s">
         <v>50</v>
@@ -7350,16 +7353,16 @@
     </row>
     <row r="259" spans="4:4">
       <c r="B259" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C259" t="s">
         <v>105</v>
       </c>
       <c r="D259" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E259" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="F259" t="s">
         <v>50</v>
@@ -7367,16 +7370,16 @@
     </row>
     <row r="260" spans="4:4">
       <c r="B260" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C260" t="s">
         <v>105</v>
       </c>
       <c r="D260" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E260" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="F260" t="s">
         <v>50</v>
@@ -7384,16 +7387,16 @@
     </row>
     <row r="261" spans="4:4">
       <c r="B261" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C261" t="s">
         <v>105</v>
       </c>
       <c r="D261" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E261" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="F261" t="s">
         <v>50</v>
@@ -7401,16 +7404,16 @@
     </row>
     <row r="262" spans="4:4">
       <c r="B262" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="C262" t="s">
-        <v>105</v>
+        <v>473</v>
       </c>
       <c r="D262" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E262" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="F262" t="s">
         <v>50</v>
@@ -7427,14 +7430,46 @@
         <v>49</v>
       </c>
       <c r="E263" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
       <c r="F263" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="264" spans="4:4"/>
-    <row r="265" spans="4:4"/>
+    <row r="264" spans="4:4">
+      <c r="B264" t="s">
+        <v>410</v>
+      </c>
+      <c r="C264" t="s">
+        <v>473</v>
+      </c>
+      <c r="D264" t="s">
+        <v>62</v>
+      </c>
+      <c r="E264" t="s">
+        <v>63</v>
+      </c>
+      <c r="F264" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="265" spans="4:4">
+      <c r="B265" t="s">
+        <v>411</v>
+      </c>
+      <c r="C265" t="s">
+        <v>473</v>
+      </c>
+      <c r="D265" t="s">
+        <v>49</v>
+      </c>
+      <c r="E265" t="s">
+        <v>463</v>
+      </c>
+      <c r="F265" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="266" spans="4:4"/>
     <row r="267" spans="4:4"/>
     <row r="268" spans="4:4"/>

</xml_diff>

<commit_message>
sistemata la grafica di debug mode e board debug mode - da implementare la logica
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415343" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679794" uniqueCount="680">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1463,6 +1463,795 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;value&gt;R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Little_Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_6
+</t>
   </si>
 </sst>
 </file>
@@ -2934,6 +3723,26 @@
       <c r="O10" s="15"/>
     </row>
     <row r="11" spans="2:15">
+      <c r="B11" t="s">
+        <v>482</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11">
+        <v>35</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11" t="s">
+        <v>455</v>
+      </c>
+      <c r="I11"/>
       <c r="K11" s="16"/>
     </row>
     <row r="12" spans="2:15">
@@ -6013,7 +6822,7 @@
         <v>311</v>
       </c>
       <c r="C180" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D180" t="s">
         <v>62</v>
@@ -6030,7 +6839,7 @@
         <v>312</v>
       </c>
       <c r="C181" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D181" t="s">
         <v>49</v>
@@ -6047,7 +6856,7 @@
         <v>315</v>
       </c>
       <c r="C182" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D182" t="s">
         <v>62</v>
@@ -6064,7 +6873,7 @@
         <v>316</v>
       </c>
       <c r="C183" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D183" t="s">
         <v>49</v>
@@ -6081,7 +6890,7 @@
         <v>319</v>
       </c>
       <c r="C184" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D184" t="s">
         <v>62</v>
@@ -6098,7 +6907,7 @@
         <v>320</v>
       </c>
       <c r="C185" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D185" t="s">
         <v>49</v>
@@ -6115,7 +6924,7 @@
         <v>321</v>
       </c>
       <c r="C186" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D186" t="s">
         <v>62</v>
@@ -6132,7 +6941,7 @@
         <v>322</v>
       </c>
       <c r="C187" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D187" t="s">
         <v>49</v>
@@ -6149,7 +6958,7 @@
         <v>324</v>
       </c>
       <c r="C188" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D188" t="s">
         <v>62</v>
@@ -6166,7 +6975,7 @@
         <v>325</v>
       </c>
       <c r="C189" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D189" t="s">
         <v>49</v>
@@ -6183,7 +6992,7 @@
         <v>326</v>
       </c>
       <c r="C190" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D190" t="s">
         <v>62</v>
@@ -6200,7 +7009,7 @@
         <v>327</v>
       </c>
       <c r="C191" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D191" t="s">
         <v>49</v>
@@ -6217,7 +7026,7 @@
         <v>328</v>
       </c>
       <c r="C192" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D192" t="s">
         <v>62</v>
@@ -6234,7 +7043,7 @@
         <v>329</v>
       </c>
       <c r="C193" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D193" t="s">
         <v>49</v>
@@ -6251,7 +7060,7 @@
         <v>330</v>
       </c>
       <c r="C194" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D194" t="s">
         <v>62</v>
@@ -6268,7 +7077,7 @@
         <v>331</v>
       </c>
       <c r="C195" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D195" t="s">
         <v>49</v>
@@ -6285,7 +7094,7 @@
         <v>332</v>
       </c>
       <c r="C196" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D196" t="s">
         <v>62</v>
@@ -6302,7 +7111,7 @@
         <v>333</v>
       </c>
       <c r="C197" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D197" t="s">
         <v>49</v>
@@ -6319,7 +7128,7 @@
         <v>334</v>
       </c>
       <c r="C198" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D198" t="s">
         <v>62</v>
@@ -6336,7 +7145,7 @@
         <v>335</v>
       </c>
       <c r="C199" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D199" t="s">
         <v>49</v>
@@ -6353,7 +7162,7 @@
         <v>336</v>
       </c>
       <c r="C200" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D200" t="s">
         <v>62</v>
@@ -6370,7 +7179,7 @@
         <v>337</v>
       </c>
       <c r="C201" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D201" t="s">
         <v>49</v>
@@ -6387,7 +7196,7 @@
         <v>338</v>
       </c>
       <c r="C202" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D202" t="s">
         <v>62</v>
@@ -6404,7 +7213,7 @@
         <v>339</v>
       </c>
       <c r="C203" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D203" t="s">
         <v>49</v>
@@ -6421,7 +7230,7 @@
         <v>340</v>
       </c>
       <c r="C204" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D204" t="s">
         <v>62</v>
@@ -6438,7 +7247,7 @@
         <v>341</v>
       </c>
       <c r="C205" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D205" t="s">
         <v>49</v>
@@ -6455,7 +7264,7 @@
         <v>342</v>
       </c>
       <c r="C206" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D206" t="s">
         <v>62</v>
@@ -6472,7 +7281,7 @@
         <v>343</v>
       </c>
       <c r="C207" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D207" t="s">
         <v>49</v>
@@ -6489,7 +7298,7 @@
         <v>344</v>
       </c>
       <c r="C208" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D208" t="s">
         <v>62</v>
@@ -6506,7 +7315,7 @@
         <v>345</v>
       </c>
       <c r="C209" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D209" t="s">
         <v>49</v>
@@ -6523,7 +7332,7 @@
         <v>346</v>
       </c>
       <c r="C210" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D210" t="s">
         <v>62</v>
@@ -6540,7 +7349,7 @@
         <v>347</v>
       </c>
       <c r="C211" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D211" t="s">
         <v>49</v>
@@ -6557,7 +7366,7 @@
         <v>348</v>
       </c>
       <c r="C212" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D212" t="s">
         <v>62</v>
@@ -6574,7 +7383,7 @@
         <v>349</v>
       </c>
       <c r="C213" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D213" t="s">
         <v>49</v>
@@ -6591,7 +7400,7 @@
         <v>350</v>
       </c>
       <c r="C214" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D214" t="s">
         <v>62</v>
@@ -6608,7 +7417,7 @@
         <v>351</v>
       </c>
       <c r="C215" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D215" t="s">
         <v>49</v>
@@ -6625,7 +7434,7 @@
         <v>352</v>
       </c>
       <c r="C216" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D216" t="s">
         <v>62</v>
@@ -6642,7 +7451,7 @@
         <v>353</v>
       </c>
       <c r="C217" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D217" t="s">
         <v>49</v>
@@ -6659,7 +7468,7 @@
         <v>354</v>
       </c>
       <c r="C218" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D218" t="s">
         <v>62</v>
@@ -6676,7 +7485,7 @@
         <v>355</v>
       </c>
       <c r="C219" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D219" t="s">
         <v>49</v>
@@ -6693,7 +7502,7 @@
         <v>356</v>
       </c>
       <c r="C220" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D220" t="s">
         <v>62</v>
@@ -6710,7 +7519,7 @@
         <v>358</v>
       </c>
       <c r="C221" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D221" t="s">
         <v>62</v>
@@ -6727,7 +7536,7 @@
         <v>359</v>
       </c>
       <c r="C222" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D222" t="s">
         <v>49</v>
@@ -6744,7 +7553,7 @@
         <v>360</v>
       </c>
       <c r="C223" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D223" t="s">
         <v>62</v>
@@ -6761,7 +7570,7 @@
         <v>361</v>
       </c>
       <c r="C224" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D224" t="s">
         <v>49</v>
@@ -6778,7 +7587,7 @@
         <v>362</v>
       </c>
       <c r="C225" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D225" t="s">
         <v>62</v>
@@ -6795,7 +7604,7 @@
         <v>363</v>
       </c>
       <c r="C226" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D226" t="s">
         <v>49</v>
@@ -6812,7 +7621,7 @@
         <v>364</v>
       </c>
       <c r="C227" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D227" t="s">
         <v>62</v>
@@ -6829,7 +7638,7 @@
         <v>365</v>
       </c>
       <c r="C228" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D228" t="s">
         <v>49</v>
@@ -6846,7 +7655,7 @@
         <v>366</v>
       </c>
       <c r="C229" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D229" t="s">
         <v>62</v>
@@ -6863,7 +7672,7 @@
         <v>367</v>
       </c>
       <c r="C230" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D230" t="s">
         <v>49</v>
@@ -6880,7 +7689,7 @@
         <v>368</v>
       </c>
       <c r="C231" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D231" t="s">
         <v>62</v>
@@ -6897,7 +7706,7 @@
         <v>369</v>
       </c>
       <c r="C232" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D232" t="s">
         <v>49</v>
@@ -6914,7 +7723,7 @@
         <v>370</v>
       </c>
       <c r="C233" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D233" t="s">
         <v>62</v>
@@ -6931,7 +7740,7 @@
         <v>371</v>
       </c>
       <c r="C234" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D234" t="s">
         <v>49</v>
@@ -6948,7 +7757,7 @@
         <v>373</v>
       </c>
       <c r="C235" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D235" t="s">
         <v>49</v>
@@ -6999,7 +7808,7 @@
         <v>384</v>
       </c>
       <c r="C238" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D238" t="s">
         <v>62</v>
@@ -7016,7 +7825,7 @@
         <v>385</v>
       </c>
       <c r="C239" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D239" t="s">
         <v>49</v>
@@ -7033,7 +7842,7 @@
         <v>386</v>
       </c>
       <c r="C240" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D240" t="s">
         <v>62</v>
@@ -7050,7 +7859,7 @@
         <v>387</v>
       </c>
       <c r="C241" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D241" t="s">
         <v>49</v>
@@ -7067,7 +7876,7 @@
         <v>388</v>
       </c>
       <c r="C242" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D242" t="s">
         <v>62</v>
@@ -7084,7 +7893,7 @@
         <v>389</v>
       </c>
       <c r="C243" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D243" t="s">
         <v>49</v>
@@ -7101,7 +7910,7 @@
         <v>390</v>
       </c>
       <c r="C244" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D244" t="s">
         <v>62</v>
@@ -7118,7 +7927,7 @@
         <v>391</v>
       </c>
       <c r="C245" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D245" t="s">
         <v>49</v>
@@ -7135,7 +7944,7 @@
         <v>392</v>
       </c>
       <c r="C246" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D246" t="s">
         <v>62</v>
@@ -7152,7 +7961,7 @@
         <v>393</v>
       </c>
       <c r="C247" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D247" t="s">
         <v>49</v>
@@ -7169,7 +7978,7 @@
         <v>394</v>
       </c>
       <c r="C248" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D248" t="s">
         <v>62</v>
@@ -7186,7 +7995,7 @@
         <v>395</v>
       </c>
       <c r="C249" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D249" t="s">
         <v>49</v>
@@ -7203,7 +8012,7 @@
         <v>396</v>
       </c>
       <c r="C250" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D250" t="s">
         <v>62</v>
@@ -7220,7 +8029,7 @@
         <v>397</v>
       </c>
       <c r="C251" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D251" t="s">
         <v>49</v>
@@ -7470,36 +8279,516 @@
         <v>50</v>
       </c>
     </row>
-    <row r="266" spans="4:4"/>
-    <row r="267" spans="4:4"/>
-    <row r="268" spans="4:4"/>
-    <row r="269" spans="4:4"/>
-    <row r="270" spans="4:4"/>
-    <row r="271" spans="4:4"/>
-    <row r="272" spans="4:4"/>
-    <row r="273" spans="4:4"/>
-    <row r="274" spans="4:4"/>
-    <row r="275" spans="4:4"/>
-    <row r="276" spans="4:4"/>
-    <row r="277" spans="4:4"/>
-    <row r="278" spans="4:4"/>
-    <row r="279" spans="4:4"/>
-    <row r="280" spans="4:4"/>
-    <row r="281" spans="4:4"/>
-    <row r="282" spans="4:4"/>
-    <row r="283" spans="4:4"/>
-    <row r="284" spans="4:4"/>
-    <row r="285" spans="4:4"/>
-    <row r="286" spans="4:4"/>
-    <row r="287" spans="4:4"/>
-    <row r="288" spans="4:4"/>
-    <row r="289" spans="4:4"/>
-    <row r="290" spans="4:4"/>
-    <row r="291" spans="4:4"/>
-    <row r="292" spans="4:4"/>
-    <row r="293" spans="4:4"/>
-    <row r="294" spans="4:4"/>
-    <row r="295" spans="4:4"/>
+    <row r="266" spans="4:4">
+      <c r="B266" t="s">
+        <v>412</v>
+      </c>
+      <c r="C266" t="s">
+        <v>482</v>
+      </c>
+      <c r="D266" t="s">
+        <v>62</v>
+      </c>
+      <c r="E266" t="s">
+        <v>63</v>
+      </c>
+      <c r="F266" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="267" spans="4:4">
+      <c r="B267" t="s">
+        <v>413</v>
+      </c>
+      <c r="C267" t="s">
+        <v>482</v>
+      </c>
+      <c r="D267" t="s">
+        <v>49</v>
+      </c>
+      <c r="E267" t="s">
+        <v>78</v>
+      </c>
+      <c r="F267" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="268" spans="4:4">
+      <c r="B268" t="s">
+        <v>414</v>
+      </c>
+      <c r="C268" t="s">
+        <v>482</v>
+      </c>
+      <c r="D268" t="s">
+        <v>62</v>
+      </c>
+      <c r="E268" t="s">
+        <v>63</v>
+      </c>
+      <c r="F268" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="269" spans="4:4">
+      <c r="B269" t="s">
+        <v>415</v>
+      </c>
+      <c r="C269" t="s">
+        <v>482</v>
+      </c>
+      <c r="D269" t="s">
+        <v>49</v>
+      </c>
+      <c r="E269" t="s">
+        <v>91</v>
+      </c>
+      <c r="F269" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="270" spans="4:4">
+      <c r="B270" t="s">
+        <v>416</v>
+      </c>
+      <c r="C270" t="s">
+        <v>482</v>
+      </c>
+      <c r="D270" t="s">
+        <v>62</v>
+      </c>
+      <c r="E270" t="s">
+        <v>63</v>
+      </c>
+      <c r="F270" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="271" spans="4:4">
+      <c r="B271" t="s">
+        <v>417</v>
+      </c>
+      <c r="C271" t="s">
+        <v>482</v>
+      </c>
+      <c r="D271" t="s">
+        <v>49</v>
+      </c>
+      <c r="E271" t="s">
+        <v>483</v>
+      </c>
+      <c r="F271" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="272" spans="4:4">
+      <c r="B272" t="s">
+        <v>418</v>
+      </c>
+      <c r="C272" t="s">
+        <v>482</v>
+      </c>
+      <c r="D272" t="s">
+        <v>62</v>
+      </c>
+      <c r="E272" t="s">
+        <v>63</v>
+      </c>
+      <c r="F272" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="273" spans="4:4">
+      <c r="B273" t="s">
+        <v>419</v>
+      </c>
+      <c r="C273" t="s">
+        <v>482</v>
+      </c>
+      <c r="D273" t="s">
+        <v>49</v>
+      </c>
+      <c r="E273" t="s">
+        <v>678</v>
+      </c>
+      <c r="F273" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="274" spans="4:4">
+      <c r="B274" t="s">
+        <v>420</v>
+      </c>
+      <c r="C274" t="s">
+        <v>482</v>
+      </c>
+      <c r="D274" t="s">
+        <v>62</v>
+      </c>
+      <c r="E274" t="s">
+        <v>63</v>
+      </c>
+      <c r="F274" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="275" spans="4:4">
+      <c r="B275" t="s">
+        <v>421</v>
+      </c>
+      <c r="C275" t="s">
+        <v>482</v>
+      </c>
+      <c r="D275" t="s">
+        <v>49</v>
+      </c>
+      <c r="E275" t="s">
+        <v>91</v>
+      </c>
+      <c r="F275" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="276" spans="4:4">
+      <c r="B276" t="s">
+        <v>422</v>
+      </c>
+      <c r="C276" t="s">
+        <v>482</v>
+      </c>
+      <c r="D276" t="s">
+        <v>62</v>
+      </c>
+      <c r="E276" t="s">
+        <v>63</v>
+      </c>
+      <c r="F276" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="277" spans="4:4">
+      <c r="B277" t="s">
+        <v>423</v>
+      </c>
+      <c r="C277" t="s">
+        <v>482</v>
+      </c>
+      <c r="D277" t="s">
+        <v>49</v>
+      </c>
+      <c r="E277" t="s">
+        <v>91</v>
+      </c>
+      <c r="F277" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="278" spans="4:4">
+      <c r="B278" t="s">
+        <v>424</v>
+      </c>
+      <c r="C278" t="s">
+        <v>482</v>
+      </c>
+      <c r="D278" t="s">
+        <v>62</v>
+      </c>
+      <c r="E278" t="s">
+        <v>63</v>
+      </c>
+      <c r="F278" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="279" spans="4:4">
+      <c r="B279" t="s">
+        <v>425</v>
+      </c>
+      <c r="C279" t="s">
+        <v>482</v>
+      </c>
+      <c r="D279" t="s">
+        <v>49</v>
+      </c>
+      <c r="E279" t="s">
+        <v>483</v>
+      </c>
+      <c r="F279" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="280" spans="4:4">
+      <c r="B280" t="s">
+        <v>426</v>
+      </c>
+      <c r="C280" t="s">
+        <v>482</v>
+      </c>
+      <c r="D280" t="s">
+        <v>62</v>
+      </c>
+      <c r="E280" t="s">
+        <v>63</v>
+      </c>
+      <c r="F280" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="281" spans="4:4">
+      <c r="B281" t="s">
+        <v>427</v>
+      </c>
+      <c r="C281" t="s">
+        <v>482</v>
+      </c>
+      <c r="D281" t="s">
+        <v>49</v>
+      </c>
+      <c r="E281" t="s">
+        <v>78</v>
+      </c>
+      <c r="F281" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="282" spans="4:4">
+      <c r="B282" t="s">
+        <v>428</v>
+      </c>
+      <c r="C282" t="s">
+        <v>482</v>
+      </c>
+      <c r="D282" t="s">
+        <v>62</v>
+      </c>
+      <c r="E282" t="s">
+        <v>63</v>
+      </c>
+      <c r="F282" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="283" spans="4:4">
+      <c r="B283" t="s">
+        <v>429</v>
+      </c>
+      <c r="C283" t="s">
+        <v>482</v>
+      </c>
+      <c r="D283" t="s">
+        <v>49</v>
+      </c>
+      <c r="E283" t="s">
+        <v>518</v>
+      </c>
+      <c r="F283" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="284" spans="4:4">
+      <c r="B284" t="s">
+        <v>430</v>
+      </c>
+      <c r="C284" t="s">
+        <v>482</v>
+      </c>
+      <c r="D284" t="s">
+        <v>62</v>
+      </c>
+      <c r="E284" t="s">
+        <v>63</v>
+      </c>
+      <c r="F284" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="285" spans="4:4">
+      <c r="B285" t="s">
+        <v>431</v>
+      </c>
+      <c r="C285" t="s">
+        <v>482</v>
+      </c>
+      <c r="D285" t="s">
+        <v>49</v>
+      </c>
+      <c r="E285" t="s">
+        <v>91</v>
+      </c>
+      <c r="F285" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="286" spans="4:4">
+      <c r="B286" t="s">
+        <v>432</v>
+      </c>
+      <c r="C286" t="s">
+        <v>482</v>
+      </c>
+      <c r="D286" t="s">
+        <v>62</v>
+      </c>
+      <c r="E286" t="s">
+        <v>63</v>
+      </c>
+      <c r="F286" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="287" spans="4:4">
+      <c r="B287" t="s">
+        <v>433</v>
+      </c>
+      <c r="C287" t="s">
+        <v>482</v>
+      </c>
+      <c r="D287" t="s">
+        <v>49</v>
+      </c>
+      <c r="E287" t="s">
+        <v>91</v>
+      </c>
+      <c r="F287" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="288" spans="4:4">
+      <c r="B288" t="s">
+        <v>434</v>
+      </c>
+      <c r="C288" t="s">
+        <v>482</v>
+      </c>
+      <c r="D288" t="s">
+        <v>62</v>
+      </c>
+      <c r="E288" t="s">
+        <v>63</v>
+      </c>
+      <c r="F288" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="289" spans="4:4">
+      <c r="B289" t="s">
+        <v>435</v>
+      </c>
+      <c r="C289" t="s">
+        <v>482</v>
+      </c>
+      <c r="D289" t="s">
+        <v>49</v>
+      </c>
+      <c r="E289" t="s">
+        <v>91</v>
+      </c>
+      <c r="F289" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="290" spans="4:4">
+      <c r="B290" t="s">
+        <v>436</v>
+      </c>
+      <c r="C290" t="s">
+        <v>482</v>
+      </c>
+      <c r="D290" t="s">
+        <v>62</v>
+      </c>
+      <c r="E290" t="s">
+        <v>63</v>
+      </c>
+      <c r="F290" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="291" spans="4:4">
+      <c r="B291" t="s">
+        <v>437</v>
+      </c>
+      <c r="C291" t="s">
+        <v>482</v>
+      </c>
+      <c r="D291" t="s">
+        <v>49</v>
+      </c>
+      <c r="E291" t="s">
+        <v>679</v>
+      </c>
+      <c r="F291" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="292" spans="4:4">
+      <c r="B292" t="s">
+        <v>438</v>
+      </c>
+      <c r="C292" t="s">
+        <v>482</v>
+      </c>
+      <c r="D292" t="s">
+        <v>62</v>
+      </c>
+      <c r="E292" t="s">
+        <v>63</v>
+      </c>
+      <c r="F292" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="293" spans="4:4">
+      <c r="B293" t="s">
+        <v>439</v>
+      </c>
+      <c r="C293" t="s">
+        <v>482</v>
+      </c>
+      <c r="D293" t="s">
+        <v>49</v>
+      </c>
+      <c r="E293" t="s">
+        <v>91</v>
+      </c>
+      <c r="F293" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="294" spans="4:4">
+      <c r="B294" t="s">
+        <v>440</v>
+      </c>
+      <c r="C294" t="s">
+        <v>482</v>
+      </c>
+      <c r="D294" t="s">
+        <v>62</v>
+      </c>
+      <c r="E294" t="s">
+        <v>63</v>
+      </c>
+      <c r="F294" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="295" spans="4:4">
+      <c r="B295" t="s">
+        <v>441</v>
+      </c>
+      <c r="C295" t="s">
+        <v>482</v>
+      </c>
+      <c r="D295" t="s">
+        <v>49</v>
+      </c>
+      <c r="E295" t="s">
+        <v>91</v>
+      </c>
+      <c r="F295" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="296" spans="4:4"/>
     <row r="297" spans="4:4"/>
     <row r="298" spans="4:4"/>

</xml_diff>

<commit_message>
sistemate le schermate di debug, aggiunta anche la logica
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679794" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687026" uniqueCount="681">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2251,6 +2251,10 @@
   </si>
   <si>
     <t xml:space="preserve">ind_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_7
 </t>
   </si>
 </sst>
@@ -8409,7 +8413,7 @@
         <v>49</v>
       </c>
       <c r="E273" t="s">
-        <v>678</v>
+        <v>484</v>
       </c>
       <c r="F273" t="s">
         <v>50</v>
@@ -8715,7 +8719,7 @@
         <v>49</v>
       </c>
       <c r="E291" t="s">
-        <v>679</v>
+        <v>551</v>
       </c>
       <c r="F291" t="s">
         <v>50</v>
@@ -8789,12 +8793,108 @@
         <v>50</v>
       </c>
     </row>
-    <row r="296" spans="4:4"/>
-    <row r="297" spans="4:4"/>
-    <row r="298" spans="4:4"/>
-    <row r="299" spans="4:4"/>
-    <row r="300" spans="4:4"/>
-    <row r="301" spans="4:4"/>
+    <row r="296" spans="4:4">
+      <c r="B296" t="s">
+        <v>442</v>
+      </c>
+      <c r="C296" t="s">
+        <v>482</v>
+      </c>
+      <c r="D296" t="s">
+        <v>62</v>
+      </c>
+      <c r="E296" t="s">
+        <v>63</v>
+      </c>
+      <c r="F296" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="297" spans="4:4">
+      <c r="B297" t="s">
+        <v>443</v>
+      </c>
+      <c r="C297" t="s">
+        <v>482</v>
+      </c>
+      <c r="D297" t="s">
+        <v>49</v>
+      </c>
+      <c r="E297" t="s">
+        <v>680</v>
+      </c>
+      <c r="F297" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="298" spans="4:4">
+      <c r="B298" t="s">
+        <v>444</v>
+      </c>
+      <c r="C298" t="s">
+        <v>482</v>
+      </c>
+      <c r="D298" t="s">
+        <v>62</v>
+      </c>
+      <c r="E298" t="s">
+        <v>63</v>
+      </c>
+      <c r="F298" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="299" spans="4:4">
+      <c r="B299" t="s">
+        <v>445</v>
+      </c>
+      <c r="C299" t="s">
+        <v>482</v>
+      </c>
+      <c r="D299" t="s">
+        <v>49</v>
+      </c>
+      <c r="E299" t="s">
+        <v>91</v>
+      </c>
+      <c r="F299" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="300" spans="4:4">
+      <c r="B300" t="s">
+        <v>446</v>
+      </c>
+      <c r="C300" t="s">
+        <v>482</v>
+      </c>
+      <c r="D300" t="s">
+        <v>62</v>
+      </c>
+      <c r="E300" t="s">
+        <v>63</v>
+      </c>
+      <c r="F300" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="301" spans="4:4">
+      <c r="B301" t="s">
+        <v>447</v>
+      </c>
+      <c r="C301" t="s">
+        <v>482</v>
+      </c>
+      <c r="D301" t="s">
+        <v>49</v>
+      </c>
+      <c r="E301" t="s">
+        <v>91</v>
+      </c>
+      <c r="F301" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="302" spans="4:4"/>
     <row r="303" spans="4:4"/>
     <row r="304" spans="4:4"/>

</xml_diff>

<commit_message>
risolto glitch in settings, iniziato ad impostare la matrice ma c'è un problema di allocazione, encoder mappa mappato come destro
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687026" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688849" uniqueCount="681">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -6724,7 +6724,7 @@
         <v>292</v>
       </c>
       <c r="C174" t="s">
-        <v>56</v>
+        <v>482</v>
       </c>
       <c r="D174" t="s">
         <v>62</v>
@@ -6775,7 +6775,7 @@
         <v>304</v>
       </c>
       <c r="C177" t="s">
-        <v>56</v>
+        <v>482</v>
       </c>
       <c r="D177" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
conversioni efi ok - ? in tutte le schermate - board debug modificato - da controllare gli indicatori - init ok
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688849" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794791" uniqueCount="769">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2255,6 +2255,315 @@
   </si>
   <si>
     <t xml:space="preserve">ind_7
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId329</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId334</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId335</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId336</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId338</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-ggh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId339</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId342</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId343</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId347</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId348</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId352</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId353</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId357</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId361</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId362</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
 </t>
   </si>
 </sst>
@@ -6789,16 +7098,16 @@
     </row>
     <row r="178" spans="4:4">
       <c r="B178" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="C178" t="s">
-        <v>59</v>
+        <v>482</v>
       </c>
       <c r="D178" t="s">
         <v>62</v>
       </c>
       <c r="E178" t="s">
-        <v>310</v>
+        <v>63</v>
       </c>
       <c r="F178" t="s">
         <v>50</v>
@@ -6806,16 +7115,16 @@
     </row>
     <row r="179" spans="4:4">
       <c r="B179" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="C179" t="s">
-        <v>59</v>
+        <v>482</v>
       </c>
       <c r="D179" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E179" t="s">
-        <v>309</v>
+        <v>81</v>
       </c>
       <c r="F179" t="s">
         <v>50</v>
@@ -6823,7 +7132,7 @@
     </row>
     <row r="180" spans="4:4">
       <c r="B180" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C180" t="s">
         <v>482</v>
@@ -6840,7 +7149,7 @@
     </row>
     <row r="181" spans="4:4">
       <c r="B181" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="C181" t="s">
         <v>482</v>
@@ -6849,7 +7158,7 @@
         <v>49</v>
       </c>
       <c r="E181" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F181" t="s">
         <v>50</v>
@@ -6857,7 +7166,7 @@
     </row>
     <row r="182" spans="4:4">
       <c r="B182" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C182" t="s">
         <v>482</v>
@@ -6874,7 +7183,7 @@
     </row>
     <row r="183" spans="4:4">
       <c r="B183" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C183" t="s">
         <v>482</v>
@@ -6883,7 +7192,7 @@
         <v>49</v>
       </c>
       <c r="E183" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F183" t="s">
         <v>50</v>
@@ -6891,7 +7200,7 @@
     </row>
     <row r="184" spans="4:4">
       <c r="B184" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C184" t="s">
         <v>482</v>
@@ -6908,7 +7217,7 @@
     </row>
     <row r="185" spans="4:4">
       <c r="B185" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C185" t="s">
         <v>482</v>
@@ -6917,7 +7226,7 @@
         <v>49</v>
       </c>
       <c r="E185" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F185" t="s">
         <v>50</v>
@@ -6925,7 +7234,7 @@
     </row>
     <row r="186" spans="4:4">
       <c r="B186" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C186" t="s">
         <v>482</v>
@@ -6942,7 +7251,7 @@
     </row>
     <row r="187" spans="4:4">
       <c r="B187" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C187" t="s">
         <v>482</v>
@@ -6951,7 +7260,7 @@
         <v>49</v>
       </c>
       <c r="E187" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="F187" t="s">
         <v>50</v>
@@ -6959,7 +7268,7 @@
     </row>
     <row r="188" spans="4:4">
       <c r="B188" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C188" t="s">
         <v>482</v>
@@ -6976,7 +7285,7 @@
     </row>
     <row r="189" spans="4:4">
       <c r="B189" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C189" t="s">
         <v>482</v>
@@ -6993,7 +7302,7 @@
     </row>
     <row r="190" spans="4:4">
       <c r="B190" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C190" t="s">
         <v>482</v>
@@ -7010,7 +7319,7 @@
     </row>
     <row r="191" spans="4:4">
       <c r="B191" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C191" t="s">
         <v>482</v>
@@ -7027,7 +7336,7 @@
     </row>
     <row r="192" spans="4:4">
       <c r="B192" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C192" t="s">
         <v>482</v>
@@ -7044,7 +7353,7 @@
     </row>
     <row r="193" spans="4:4">
       <c r="B193" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C193" t="s">
         <v>482</v>
@@ -7061,7 +7370,7 @@
     </row>
     <row r="194" spans="4:4">
       <c r="B194" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C194" t="s">
         <v>482</v>
@@ -7078,7 +7387,7 @@
     </row>
     <row r="195" spans="4:4">
       <c r="B195" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C195" t="s">
         <v>482</v>
@@ -7095,7 +7404,7 @@
     </row>
     <row r="196" spans="4:4">
       <c r="B196" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C196" t="s">
         <v>482</v>
@@ -7112,7 +7421,7 @@
     </row>
     <row r="197" spans="4:4">
       <c r="B197" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C197" t="s">
         <v>482</v>
@@ -7129,7 +7438,7 @@
     </row>
     <row r="198" spans="4:4">
       <c r="B198" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C198" t="s">
         <v>482</v>
@@ -7146,7 +7455,7 @@
     </row>
     <row r="199" spans="4:4">
       <c r="B199" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C199" t="s">
         <v>482</v>
@@ -7163,7 +7472,7 @@
     </row>
     <row r="200" spans="4:4">
       <c r="B200" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C200" t="s">
         <v>482</v>
@@ -7180,7 +7489,7 @@
     </row>
     <row r="201" spans="4:4">
       <c r="B201" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C201" t="s">
         <v>482</v>
@@ -7197,7 +7506,7 @@
     </row>
     <row r="202" spans="4:4">
       <c r="B202" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C202" t="s">
         <v>482</v>
@@ -7214,7 +7523,7 @@
     </row>
     <row r="203" spans="4:4">
       <c r="B203" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C203" t="s">
         <v>482</v>
@@ -7223,7 +7532,7 @@
         <v>49</v>
       </c>
       <c r="E203" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F203" t="s">
         <v>50</v>
@@ -7231,7 +7540,7 @@
     </row>
     <row r="204" spans="4:4">
       <c r="B204" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C204" t="s">
         <v>482</v>
@@ -7248,7 +7557,7 @@
     </row>
     <row r="205" spans="4:4">
       <c r="B205" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C205" t="s">
         <v>482</v>
@@ -7257,7 +7566,7 @@
         <v>49</v>
       </c>
       <c r="E205" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F205" t="s">
         <v>50</v>
@@ -7265,7 +7574,7 @@
     </row>
     <row r="206" spans="4:4">
       <c r="B206" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C206" t="s">
         <v>482</v>
@@ -7282,7 +7591,7 @@
     </row>
     <row r="207" spans="4:4">
       <c r="B207" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C207" t="s">
         <v>482</v>
@@ -7291,7 +7600,7 @@
         <v>49</v>
       </c>
       <c r="E207" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F207" t="s">
         <v>50</v>
@@ -7299,7 +7608,7 @@
     </row>
     <row r="208" spans="4:4">
       <c r="B208" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C208" t="s">
         <v>482</v>
@@ -7316,7 +7625,7 @@
     </row>
     <row r="209" spans="4:4">
       <c r="B209" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C209" t="s">
         <v>482</v>
@@ -7325,7 +7634,7 @@
         <v>49</v>
       </c>
       <c r="E209" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F209" t="s">
         <v>50</v>
@@ -7333,7 +7642,7 @@
     </row>
     <row r="210" spans="4:4">
       <c r="B210" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C210" t="s">
         <v>482</v>
@@ -7350,7 +7659,7 @@
     </row>
     <row r="211" spans="4:4">
       <c r="B211" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C211" t="s">
         <v>482</v>
@@ -7359,7 +7668,7 @@
         <v>49</v>
       </c>
       <c r="E211" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F211" t="s">
         <v>50</v>
@@ -7367,7 +7676,7 @@
     </row>
     <row r="212" spans="4:4">
       <c r="B212" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C212" t="s">
         <v>482</v>
@@ -7384,7 +7693,7 @@
     </row>
     <row r="213" spans="4:4">
       <c r="B213" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C213" t="s">
         <v>482</v>
@@ -7393,7 +7702,7 @@
         <v>49</v>
       </c>
       <c r="E213" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F213" t="s">
         <v>50</v>
@@ -7401,7 +7710,7 @@
     </row>
     <row r="214" spans="4:4">
       <c r="B214" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C214" t="s">
         <v>482</v>
@@ -7418,7 +7727,7 @@
     </row>
     <row r="215" spans="4:4">
       <c r="B215" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C215" t="s">
         <v>482</v>
@@ -7427,7 +7736,7 @@
         <v>49</v>
       </c>
       <c r="E215" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F215" t="s">
         <v>50</v>
@@ -7435,7 +7744,7 @@
     </row>
     <row r="216" spans="4:4">
       <c r="B216" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C216" t="s">
         <v>482</v>
@@ -7452,7 +7761,7 @@
     </row>
     <row r="217" spans="4:4">
       <c r="B217" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C217" t="s">
         <v>482</v>
@@ -7461,7 +7770,7 @@
         <v>49</v>
       </c>
       <c r="E217" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F217" t="s">
         <v>50</v>
@@ -7469,7 +7778,7 @@
     </row>
     <row r="218" spans="4:4">
       <c r="B218" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C218" t="s">
         <v>482</v>
@@ -7486,16 +7795,16 @@
     </row>
     <row r="219" spans="4:4">
       <c r="B219" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C219" t="s">
         <v>482</v>
       </c>
       <c r="D219" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E219" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="F219" t="s">
         <v>50</v>
@@ -7503,16 +7812,16 @@
     </row>
     <row r="220" spans="4:4">
       <c r="B220" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C220" t="s">
         <v>482</v>
       </c>
       <c r="D220" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E220" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F220" t="s">
         <v>50</v>
@@ -7520,7 +7829,7 @@
     </row>
     <row r="221" spans="4:4">
       <c r="B221" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C221" t="s">
         <v>482</v>
@@ -7537,7 +7846,7 @@
     </row>
     <row r="222" spans="4:4">
       <c r="B222" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C222" t="s">
         <v>482</v>
@@ -7554,7 +7863,7 @@
     </row>
     <row r="223" spans="4:4">
       <c r="B223" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C223" t="s">
         <v>482</v>
@@ -7571,7 +7880,7 @@
     </row>
     <row r="224" spans="4:4">
       <c r="B224" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C224" t="s">
         <v>482</v>
@@ -7588,7 +7897,7 @@
     </row>
     <row r="225" spans="4:4">
       <c r="B225" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C225" t="s">
         <v>482</v>
@@ -7605,7 +7914,7 @@
     </row>
     <row r="226" spans="4:4">
       <c r="B226" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C226" t="s">
         <v>482</v>
@@ -7622,7 +7931,7 @@
     </row>
     <row r="227" spans="4:4">
       <c r="B227" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C227" t="s">
         <v>482</v>
@@ -7639,7 +7948,7 @@
     </row>
     <row r="228" spans="4:4">
       <c r="B228" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C228" t="s">
         <v>482</v>
@@ -7656,7 +7965,7 @@
     </row>
     <row r="229" spans="4:4">
       <c r="B229" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C229" t="s">
         <v>482</v>
@@ -7673,7 +7982,7 @@
     </row>
     <row r="230" spans="4:4">
       <c r="B230" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C230" t="s">
         <v>482</v>
@@ -7690,7 +7999,7 @@
     </row>
     <row r="231" spans="4:4">
       <c r="B231" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C231" t="s">
         <v>482</v>
@@ -7707,7 +8016,7 @@
     </row>
     <row r="232" spans="4:4">
       <c r="B232" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C232" t="s">
         <v>482</v>
@@ -7724,16 +8033,16 @@
     </row>
     <row r="233" spans="4:4">
       <c r="B233" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="C233" t="s">
         <v>482</v>
       </c>
       <c r="D233" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E233" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F233" t="s">
         <v>50</v>
@@ -7741,16 +8050,16 @@
     </row>
     <row r="234" spans="4:4">
       <c r="B234" t="s">
-        <v>371</v>
+        <v>379</v>
       </c>
       <c r="C234" t="s">
-        <v>482</v>
+        <v>105</v>
       </c>
       <c r="D234" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E234" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F234" t="s">
         <v>50</v>
@@ -7758,16 +8067,16 @@
     </row>
     <row r="235" spans="4:4">
       <c r="B235" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="C235" t="s">
-        <v>482</v>
+        <v>105</v>
       </c>
       <c r="D235" t="s">
         <v>49</v>
       </c>
       <c r="E235" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="F235" t="s">
         <v>50</v>
@@ -7775,10 +8084,10 @@
     </row>
     <row r="236" spans="4:4">
       <c r="B236" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="C236" t="s">
-        <v>105</v>
+        <v>482</v>
       </c>
       <c r="D236" t="s">
         <v>62</v>
@@ -7792,16 +8101,16 @@
     </row>
     <row r="237" spans="4:4">
       <c r="B237" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="C237" t="s">
-        <v>105</v>
+        <v>482</v>
       </c>
       <c r="D237" t="s">
         <v>49</v>
       </c>
       <c r="E237" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="F237" t="s">
         <v>50</v>
@@ -7809,7 +8118,7 @@
     </row>
     <row r="238" spans="4:4">
       <c r="B238" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C238" t="s">
         <v>482</v>
@@ -7826,7 +8135,7 @@
     </row>
     <row r="239" spans="4:4">
       <c r="B239" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C239" t="s">
         <v>482</v>
@@ -7835,7 +8144,7 @@
         <v>49</v>
       </c>
       <c r="E239" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F239" t="s">
         <v>50</v>
@@ -7843,7 +8152,7 @@
     </row>
     <row r="240" spans="4:4">
       <c r="B240" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C240" t="s">
         <v>482</v>
@@ -7860,7 +8169,7 @@
     </row>
     <row r="241" spans="4:4">
       <c r="B241" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C241" t="s">
         <v>482</v>
@@ -7877,7 +8186,7 @@
     </row>
     <row r="242" spans="4:4">
       <c r="B242" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C242" t="s">
         <v>482</v>
@@ -7894,7 +8203,7 @@
     </row>
     <row r="243" spans="4:4">
       <c r="B243" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C243" t="s">
         <v>482</v>
@@ -7903,7 +8212,7 @@
         <v>49</v>
       </c>
       <c r="E243" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F243" t="s">
         <v>50</v>
@@ -7911,7 +8220,7 @@
     </row>
     <row r="244" spans="4:4">
       <c r="B244" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C244" t="s">
         <v>482</v>
@@ -7928,7 +8237,7 @@
     </row>
     <row r="245" spans="4:4">
       <c r="B245" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C245" t="s">
         <v>482</v>
@@ -7937,7 +8246,7 @@
         <v>49</v>
       </c>
       <c r="E245" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F245" t="s">
         <v>50</v>
@@ -7945,7 +8254,7 @@
     </row>
     <row r="246" spans="4:4">
       <c r="B246" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C246" t="s">
         <v>482</v>
@@ -7962,7 +8271,7 @@
     </row>
     <row r="247" spans="4:4">
       <c r="B247" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C247" t="s">
         <v>482</v>
@@ -7971,7 +8280,7 @@
         <v>49</v>
       </c>
       <c r="E247" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F247" t="s">
         <v>50</v>
@@ -7979,7 +8288,7 @@
     </row>
     <row r="248" spans="4:4">
       <c r="B248" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C248" t="s">
         <v>482</v>
@@ -7996,7 +8305,7 @@
     </row>
     <row r="249" spans="4:4">
       <c r="B249" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C249" t="s">
         <v>482</v>
@@ -8005,7 +8314,7 @@
         <v>49</v>
       </c>
       <c r="E249" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F249" t="s">
         <v>50</v>
@@ -8013,16 +8322,16 @@
     </row>
     <row r="250" spans="4:4">
       <c r="B250" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C250" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="D250" t="s">
         <v>62</v>
       </c>
       <c r="E250" t="s">
-        <v>63</v>
+        <v>242</v>
       </c>
       <c r="F250" t="s">
         <v>50</v>
@@ -8030,16 +8339,16 @@
     </row>
     <row r="251" spans="4:4">
       <c r="B251" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C251" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="D251" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E251" t="s">
-        <v>91</v>
+        <v>133</v>
       </c>
       <c r="F251" t="s">
         <v>50</v>
@@ -8047,7 +8356,7 @@
     </row>
     <row r="252" spans="4:4">
       <c r="B252" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C252" t="s">
         <v>469</v>
@@ -8056,7 +8365,7 @@
         <v>62</v>
       </c>
       <c r="E252" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F252" t="s">
         <v>50</v>
@@ -8064,7 +8373,7 @@
     </row>
     <row r="253" spans="4:4">
       <c r="B253" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C253" t="s">
         <v>469</v>
@@ -8073,7 +8382,7 @@
         <v>62</v>
       </c>
       <c r="E253" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="F253" t="s">
         <v>50</v>
@@ -8081,16 +8390,16 @@
     </row>
     <row r="254" spans="4:4">
       <c r="B254" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="C254" t="s">
-        <v>469</v>
+        <v>105</v>
       </c>
       <c r="D254" t="s">
         <v>62</v>
       </c>
       <c r="E254" t="s">
-        <v>241</v>
+        <v>63</v>
       </c>
       <c r="F254" t="s">
         <v>50</v>
@@ -8098,16 +8407,16 @@
     </row>
     <row r="255" spans="4:4">
       <c r="B255" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="C255" t="s">
-        <v>469</v>
+        <v>105</v>
       </c>
       <c r="D255" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E255" t="s">
-        <v>170</v>
+        <v>106</v>
       </c>
       <c r="F255" t="s">
         <v>50</v>
@@ -8115,7 +8424,7 @@
     </row>
     <row r="256" spans="4:4">
       <c r="B256" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C256" t="s">
         <v>105</v>
@@ -8132,7 +8441,7 @@
     </row>
     <row r="257" spans="4:4">
       <c r="B257" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C257" t="s">
         <v>105</v>
@@ -8149,7 +8458,7 @@
     </row>
     <row r="258" spans="4:4">
       <c r="B258" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C258" t="s">
         <v>105</v>
@@ -8166,7 +8475,7 @@
     </row>
     <row r="259" spans="4:4">
       <c r="B259" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C259" t="s">
         <v>105</v>
@@ -8183,10 +8492,10 @@
     </row>
     <row r="260" spans="4:4">
       <c r="B260" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C260" t="s">
-        <v>105</v>
+        <v>473</v>
       </c>
       <c r="D260" t="s">
         <v>62</v>
@@ -8200,16 +8509,16 @@
     </row>
     <row r="261" spans="4:4">
       <c r="B261" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C261" t="s">
-        <v>105</v>
+        <v>473</v>
       </c>
       <c r="D261" t="s">
         <v>49</v>
       </c>
       <c r="E261" t="s">
-        <v>106</v>
+        <v>463</v>
       </c>
       <c r="F261" t="s">
         <v>50</v>
@@ -8217,7 +8526,7 @@
     </row>
     <row r="262" spans="4:4">
       <c r="B262" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
       <c r="C262" t="s">
         <v>473</v>
@@ -8234,7 +8543,7 @@
     </row>
     <row r="263" spans="4:4">
       <c r="B263" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C263" t="s">
         <v>473</v>
@@ -8251,10 +8560,10 @@
     </row>
     <row r="264" spans="4:4">
       <c r="B264" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C264" t="s">
-        <v>473</v>
+        <v>482</v>
       </c>
       <c r="D264" t="s">
         <v>62</v>
@@ -8268,16 +8577,16 @@
     </row>
     <row r="265" spans="4:4">
       <c r="B265" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C265" t="s">
-        <v>473</v>
+        <v>482</v>
       </c>
       <c r="D265" t="s">
         <v>49</v>
       </c>
       <c r="E265" t="s">
-        <v>463</v>
+        <v>78</v>
       </c>
       <c r="F265" t="s">
         <v>50</v>
@@ -8285,7 +8594,7 @@
     </row>
     <row r="266" spans="4:4">
       <c r="B266" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C266" t="s">
         <v>482</v>
@@ -8302,7 +8611,7 @@
     </row>
     <row r="267" spans="4:4">
       <c r="B267" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C267" t="s">
         <v>482</v>
@@ -8311,7 +8620,7 @@
         <v>49</v>
       </c>
       <c r="E267" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="F267" t="s">
         <v>50</v>
@@ -8319,7 +8628,7 @@
     </row>
     <row r="268" spans="4:4">
       <c r="B268" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C268" t="s">
         <v>482</v>
@@ -8336,7 +8645,7 @@
     </row>
     <row r="269" spans="4:4">
       <c r="B269" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C269" t="s">
         <v>482</v>
@@ -8345,7 +8654,7 @@
         <v>49</v>
       </c>
       <c r="E269" t="s">
-        <v>91</v>
+        <v>483</v>
       </c>
       <c r="F269" t="s">
         <v>50</v>
@@ -8353,7 +8662,7 @@
     </row>
     <row r="270" spans="4:4">
       <c r="B270" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C270" t="s">
         <v>482</v>
@@ -8370,7 +8679,7 @@
     </row>
     <row r="271" spans="4:4">
       <c r="B271" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C271" t="s">
         <v>482</v>
@@ -8379,7 +8688,7 @@
         <v>49</v>
       </c>
       <c r="E271" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="F271" t="s">
         <v>50</v>
@@ -8387,7 +8696,7 @@
     </row>
     <row r="272" spans="4:4">
       <c r="B272" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C272" t="s">
         <v>482</v>
@@ -8404,7 +8713,7 @@
     </row>
     <row r="273" spans="4:4">
       <c r="B273" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C273" t="s">
         <v>482</v>
@@ -8413,7 +8722,7 @@
         <v>49</v>
       </c>
       <c r="E273" t="s">
-        <v>484</v>
+        <v>91</v>
       </c>
       <c r="F273" t="s">
         <v>50</v>
@@ -8421,7 +8730,7 @@
     </row>
     <row r="274" spans="4:4">
       <c r="B274" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C274" t="s">
         <v>482</v>
@@ -8438,7 +8747,7 @@
     </row>
     <row r="275" spans="4:4">
       <c r="B275" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C275" t="s">
         <v>482</v>
@@ -8455,7 +8764,7 @@
     </row>
     <row r="276" spans="4:4">
       <c r="B276" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C276" t="s">
         <v>482</v>
@@ -8472,7 +8781,7 @@
     </row>
     <row r="277" spans="4:4">
       <c r="B277" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C277" t="s">
         <v>482</v>
@@ -8481,7 +8790,7 @@
         <v>49</v>
       </c>
       <c r="E277" t="s">
-        <v>91</v>
+        <v>483</v>
       </c>
       <c r="F277" t="s">
         <v>50</v>
@@ -8489,7 +8798,7 @@
     </row>
     <row r="278" spans="4:4">
       <c r="B278" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C278" t="s">
         <v>482</v>
@@ -8506,7 +8815,7 @@
     </row>
     <row r="279" spans="4:4">
       <c r="B279" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C279" t="s">
         <v>482</v>
@@ -8515,7 +8824,7 @@
         <v>49</v>
       </c>
       <c r="E279" t="s">
-        <v>483</v>
+        <v>78</v>
       </c>
       <c r="F279" t="s">
         <v>50</v>
@@ -8523,7 +8832,7 @@
     </row>
     <row r="280" spans="4:4">
       <c r="B280" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C280" t="s">
         <v>482</v>
@@ -8540,7 +8849,7 @@
     </row>
     <row r="281" spans="4:4">
       <c r="B281" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C281" t="s">
         <v>482</v>
@@ -8549,7 +8858,7 @@
         <v>49</v>
       </c>
       <c r="E281" t="s">
-        <v>78</v>
+        <v>518</v>
       </c>
       <c r="F281" t="s">
         <v>50</v>
@@ -8557,7 +8866,7 @@
     </row>
     <row r="282" spans="4:4">
       <c r="B282" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C282" t="s">
         <v>482</v>
@@ -8574,7 +8883,7 @@
     </row>
     <row r="283" spans="4:4">
       <c r="B283" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C283" t="s">
         <v>482</v>
@@ -8583,7 +8892,7 @@
         <v>49</v>
       </c>
       <c r="E283" t="s">
-        <v>518</v>
+        <v>91</v>
       </c>
       <c r="F283" t="s">
         <v>50</v>
@@ -8591,7 +8900,7 @@
     </row>
     <row r="284" spans="4:4">
       <c r="B284" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C284" t="s">
         <v>482</v>
@@ -8608,7 +8917,7 @@
     </row>
     <row r="285" spans="4:4">
       <c r="B285" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C285" t="s">
         <v>482</v>
@@ -8625,7 +8934,7 @@
     </row>
     <row r="286" spans="4:4">
       <c r="B286" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C286" t="s">
         <v>482</v>
@@ -8642,7 +8951,7 @@
     </row>
     <row r="287" spans="4:4">
       <c r="B287" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C287" t="s">
         <v>482</v>
@@ -8659,7 +8968,7 @@
     </row>
     <row r="288" spans="4:4">
       <c r="B288" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C288" t="s">
         <v>482</v>
@@ -8676,7 +8985,7 @@
     </row>
     <row r="289" spans="4:4">
       <c r="B289" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C289" t="s">
         <v>482</v>
@@ -8685,7 +8994,7 @@
         <v>49</v>
       </c>
       <c r="E289" t="s">
-        <v>91</v>
+        <v>551</v>
       </c>
       <c r="F289" t="s">
         <v>50</v>
@@ -8693,7 +9002,7 @@
     </row>
     <row r="290" spans="4:4">
       <c r="B290" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C290" t="s">
         <v>482</v>
@@ -8710,7 +9019,7 @@
     </row>
     <row r="291" spans="4:4">
       <c r="B291" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C291" t="s">
         <v>482</v>
@@ -8719,7 +9028,7 @@
         <v>49</v>
       </c>
       <c r="E291" t="s">
-        <v>551</v>
+        <v>91</v>
       </c>
       <c r="F291" t="s">
         <v>50</v>
@@ -8727,7 +9036,7 @@
     </row>
     <row r="292" spans="4:4">
       <c r="B292" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C292" t="s">
         <v>482</v>
@@ -8744,7 +9053,7 @@
     </row>
     <row r="293" spans="4:4">
       <c r="B293" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C293" t="s">
         <v>482</v>
@@ -8761,7 +9070,7 @@
     </row>
     <row r="294" spans="4:4">
       <c r="B294" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C294" t="s">
         <v>482</v>
@@ -8778,7 +9087,7 @@
     </row>
     <row r="295" spans="4:4">
       <c r="B295" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="C295" t="s">
         <v>482</v>
@@ -8787,7 +9096,7 @@
         <v>49</v>
       </c>
       <c r="E295" t="s">
-        <v>91</v>
+        <v>680</v>
       </c>
       <c r="F295" t="s">
         <v>50</v>
@@ -8795,7 +9104,7 @@
     </row>
     <row r="296" spans="4:4">
       <c r="B296" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C296" t="s">
         <v>482</v>
@@ -8812,7 +9121,7 @@
     </row>
     <row r="297" spans="4:4">
       <c r="B297" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C297" t="s">
         <v>482</v>
@@ -8821,7 +9130,7 @@
         <v>49</v>
       </c>
       <c r="E297" t="s">
-        <v>680</v>
+        <v>91</v>
       </c>
       <c r="F297" t="s">
         <v>50</v>
@@ -8829,7 +9138,7 @@
     </row>
     <row r="298" spans="4:4">
       <c r="B298" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C298" t="s">
         <v>482</v>
@@ -8846,7 +9155,7 @@
     </row>
     <row r="299" spans="4:4">
       <c r="B299" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C299" t="s">
         <v>482</v>
@@ -8863,7 +9172,7 @@
     </row>
     <row r="300" spans="4:4">
       <c r="B300" t="s">
-        <v>446</v>
+        <v>681</v>
       </c>
       <c r="C300" t="s">
         <v>482</v>
@@ -8880,7 +9189,7 @@
     </row>
     <row r="301" spans="4:4">
       <c r="B301" t="s">
-        <v>447</v>
+        <v>682</v>
       </c>
       <c r="C301" t="s">
         <v>482</v>
@@ -8889,50 +9198,658 @@
         <v>49</v>
       </c>
       <c r="E301" t="s">
+        <v>687</v>
+      </c>
+      <c r="F301" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="302" spans="4:4">
+      <c r="B302" t="s">
+        <v>683</v>
+      </c>
+      <c r="C302" t="s">
+        <v>482</v>
+      </c>
+      <c r="D302" t="s">
+        <v>62</v>
+      </c>
+      <c r="E302" t="s">
+        <v>63</v>
+      </c>
+      <c r="F302" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="303" spans="4:4">
+      <c r="B303" t="s">
+        <v>684</v>
+      </c>
+      <c r="C303" t="s">
+        <v>482</v>
+      </c>
+      <c r="D303" t="s">
+        <v>49</v>
+      </c>
+      <c r="E303" t="s">
         <v>91</v>
       </c>
-      <c r="F301" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="302" spans="4:4"/>
-    <row r="303" spans="4:4"/>
-    <row r="304" spans="4:4"/>
-    <row r="305" spans="4:4"/>
-    <row r="306" spans="4:4"/>
-    <row r="307" spans="4:4"/>
-    <row r="308" spans="4:4"/>
-    <row r="309" spans="4:4"/>
-    <row r="310" spans="4:4"/>
-    <row r="311" spans="4:4"/>
-    <row r="312" spans="4:4"/>
-    <row r="313" spans="4:4"/>
-    <row r="314" spans="4:4"/>
-    <row r="315" spans="4:4"/>
-    <row r="316" spans="4:4"/>
-    <row r="317" spans="4:4"/>
-    <row r="318" spans="4:4"/>
-    <row r="319" spans="4:4"/>
-    <row r="320" spans="4:4"/>
-    <row r="321" spans="4:4"/>
-    <row r="322" spans="4:4"/>
-    <row r="323" spans="4:4"/>
-    <row r="324" spans="4:4"/>
-    <row r="325" spans="4:4"/>
-    <row r="326" spans="4:4"/>
-    <row r="327" spans="4:4"/>
-    <row r="328" spans="4:4"/>
-    <row r="329" spans="4:4"/>
-    <row r="330" spans="4:4"/>
-    <row r="331" spans="4:4"/>
-    <row r="332" spans="4:4"/>
-    <row r="333" spans="4:4"/>
-    <row r="334" spans="4:4"/>
-    <row r="335" spans="4:4"/>
-    <row r="336" spans="4:4"/>
-    <row r="337" spans="4:4"/>
-    <row r="338" spans="4:4"/>
-    <row r="339" spans="4:4"/>
+      <c r="F303" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="304" spans="4:4">
+      <c r="B304" t="s">
+        <v>685</v>
+      </c>
+      <c r="C304" t="s">
+        <v>482</v>
+      </c>
+      <c r="D304" t="s">
+        <v>62</v>
+      </c>
+      <c r="E304" t="s">
+        <v>63</v>
+      </c>
+      <c r="F304" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="305" spans="4:4">
+      <c r="B305" t="s">
+        <v>686</v>
+      </c>
+      <c r="C305" t="s">
+        <v>482</v>
+      </c>
+      <c r="D305" t="s">
+        <v>49</v>
+      </c>
+      <c r="E305" t="s">
+        <v>91</v>
+      </c>
+      <c r="F305" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="306" spans="4:4">
+      <c r="B306" t="s">
+        <v>688</v>
+      </c>
+      <c r="C306" t="s">
+        <v>56</v>
+      </c>
+      <c r="D306" t="s">
+        <v>62</v>
+      </c>
+      <c r="E306" t="s">
+        <v>63</v>
+      </c>
+      <c r="F306" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="307" spans="4:4">
+      <c r="B307" t="s">
+        <v>689</v>
+      </c>
+      <c r="C307" t="s">
+        <v>56</v>
+      </c>
+      <c r="D307" t="s">
+        <v>49</v>
+      </c>
+      <c r="E307" t="s">
+        <v>768</v>
+      </c>
+      <c r="F307" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="308" spans="4:4">
+      <c r="B308" t="s">
+        <v>690</v>
+      </c>
+      <c r="C308" t="s">
+        <v>56</v>
+      </c>
+      <c r="D308" t="s">
+        <v>62</v>
+      </c>
+      <c r="E308" t="s">
+        <v>63</v>
+      </c>
+      <c r="F308" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="309" spans="4:4">
+      <c r="B309" t="s">
+        <v>692</v>
+      </c>
+      <c r="C309" t="s">
+        <v>56</v>
+      </c>
+      <c r="D309" t="s">
+        <v>62</v>
+      </c>
+      <c r="E309" t="s">
+        <v>63</v>
+      </c>
+      <c r="F309" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="310" spans="4:4">
+      <c r="B310" t="s">
+        <v>693</v>
+      </c>
+      <c r="C310" t="s">
+        <v>56</v>
+      </c>
+      <c r="D310" t="s">
+        <v>49</v>
+      </c>
+      <c r="E310" t="s">
+        <v>694</v>
+      </c>
+      <c r="F310" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="311" spans="4:4">
+      <c r="B311" t="s">
+        <v>695</v>
+      </c>
+      <c r="C311" t="s">
+        <v>56</v>
+      </c>
+      <c r="D311" t="s">
+        <v>49</v>
+      </c>
+      <c r="E311" t="s">
+        <v>694</v>
+      </c>
+      <c r="F311" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="312" spans="4:4">
+      <c r="B312" t="s">
+        <v>703</v>
+      </c>
+      <c r="C312" t="s">
+        <v>56</v>
+      </c>
+      <c r="D312" t="s">
+        <v>62</v>
+      </c>
+      <c r="E312" t="s">
+        <v>63</v>
+      </c>
+      <c r="F312" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="313" spans="4:4">
+      <c r="B313" t="s">
+        <v>704</v>
+      </c>
+      <c r="C313" t="s">
+        <v>56</v>
+      </c>
+      <c r="D313" t="s">
+        <v>49</v>
+      </c>
+      <c r="E313" t="s">
+        <v>694</v>
+      </c>
+      <c r="F313" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="314" spans="4:4">
+      <c r="B314" t="s">
+        <v>706</v>
+      </c>
+      <c r="C314" t="s">
+        <v>56</v>
+      </c>
+      <c r="D314" t="s">
+        <v>62</v>
+      </c>
+      <c r="E314" t="s">
+        <v>63</v>
+      </c>
+      <c r="F314" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="315" spans="4:4">
+      <c r="B315" t="s">
+        <v>707</v>
+      </c>
+      <c r="C315" t="s">
+        <v>56</v>
+      </c>
+      <c r="D315" t="s">
+        <v>49</v>
+      </c>
+      <c r="E315" t="s">
+        <v>694</v>
+      </c>
+      <c r="F315" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="316" spans="4:4">
+      <c r="B316" t="s">
+        <v>715</v>
+      </c>
+      <c r="C316" t="s">
+        <v>56</v>
+      </c>
+      <c r="D316" t="s">
+        <v>62</v>
+      </c>
+      <c r="E316" t="s">
+        <v>63</v>
+      </c>
+      <c r="F316" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="317" spans="4:4">
+      <c r="B317" t="s">
+        <v>716</v>
+      </c>
+      <c r="C317" t="s">
+        <v>56</v>
+      </c>
+      <c r="D317" t="s">
+        <v>49</v>
+      </c>
+      <c r="E317" t="s">
+        <v>694</v>
+      </c>
+      <c r="F317" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="318" spans="4:4">
+      <c r="B318" t="s">
+        <v>718</v>
+      </c>
+      <c r="C318" t="s">
+        <v>56</v>
+      </c>
+      <c r="D318" t="s">
+        <v>62</v>
+      </c>
+      <c r="E318" t="s">
+        <v>63</v>
+      </c>
+      <c r="F318" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="319" spans="4:4">
+      <c r="B319" t="s">
+        <v>719</v>
+      </c>
+      <c r="C319" t="s">
+        <v>56</v>
+      </c>
+      <c r="D319" t="s">
+        <v>49</v>
+      </c>
+      <c r="E319" t="s">
+        <v>694</v>
+      </c>
+      <c r="F319" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="320" spans="4:4">
+      <c r="B320" t="s">
+        <v>720</v>
+      </c>
+      <c r="C320" t="s">
+        <v>56</v>
+      </c>
+      <c r="D320" t="s">
+        <v>62</v>
+      </c>
+      <c r="E320" t="s">
+        <v>63</v>
+      </c>
+      <c r="F320" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="321" spans="4:4">
+      <c r="B321" t="s">
+        <v>721</v>
+      </c>
+      <c r="C321" t="s">
+        <v>56</v>
+      </c>
+      <c r="D321" t="s">
+        <v>49</v>
+      </c>
+      <c r="E321" t="s">
+        <v>694</v>
+      </c>
+      <c r="F321" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="322" spans="4:4">
+      <c r="B322" t="s">
+        <v>723</v>
+      </c>
+      <c r="C322" t="s">
+        <v>56</v>
+      </c>
+      <c r="D322" t="s">
+        <v>62</v>
+      </c>
+      <c r="E322" t="s">
+        <v>63</v>
+      </c>
+      <c r="F322" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="323" spans="4:4">
+      <c r="B323" t="s">
+        <v>724</v>
+      </c>
+      <c r="C323" t="s">
+        <v>56</v>
+      </c>
+      <c r="D323" t="s">
+        <v>49</v>
+      </c>
+      <c r="E323" t="s">
+        <v>694</v>
+      </c>
+      <c r="F323" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="324" spans="4:4">
+      <c r="B324" t="s">
+        <v>725</v>
+      </c>
+      <c r="C324" t="s">
+        <v>56</v>
+      </c>
+      <c r="D324" t="s">
+        <v>62</v>
+      </c>
+      <c r="E324" t="s">
+        <v>63</v>
+      </c>
+      <c r="F324" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="325" spans="4:4">
+      <c r="B325" t="s">
+        <v>726</v>
+      </c>
+      <c r="C325" t="s">
+        <v>56</v>
+      </c>
+      <c r="D325" t="s">
+        <v>49</v>
+      </c>
+      <c r="E325" t="s">
+        <v>694</v>
+      </c>
+      <c r="F325" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="326" spans="4:4">
+      <c r="B326" t="s">
+        <v>732</v>
+      </c>
+      <c r="C326" t="s">
+        <v>56</v>
+      </c>
+      <c r="D326" t="s">
+        <v>62</v>
+      </c>
+      <c r="E326" t="s">
+        <v>63</v>
+      </c>
+      <c r="F326" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="327" spans="4:4">
+      <c r="B327" t="s">
+        <v>733</v>
+      </c>
+      <c r="C327" t="s">
+        <v>56</v>
+      </c>
+      <c r="D327" t="s">
+        <v>49</v>
+      </c>
+      <c r="E327" t="s">
+        <v>694</v>
+      </c>
+      <c r="F327" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="328" spans="4:4">
+      <c r="B328" t="s">
+        <v>736</v>
+      </c>
+      <c r="C328" t="s">
+        <v>56</v>
+      </c>
+      <c r="D328" t="s">
+        <v>62</v>
+      </c>
+      <c r="E328" t="s">
+        <v>63</v>
+      </c>
+      <c r="F328" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="329" spans="4:4">
+      <c r="B329" t="s">
+        <v>737</v>
+      </c>
+      <c r="C329" t="s">
+        <v>56</v>
+      </c>
+      <c r="D329" t="s">
+        <v>49</v>
+      </c>
+      <c r="E329" t="s">
+        <v>694</v>
+      </c>
+      <c r="F329" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="330" spans="4:4">
+      <c r="B330" t="s">
+        <v>738</v>
+      </c>
+      <c r="C330" t="s">
+        <v>56</v>
+      </c>
+      <c r="D330" t="s">
+        <v>62</v>
+      </c>
+      <c r="E330" t="s">
+        <v>63</v>
+      </c>
+      <c r="F330" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="331" spans="4:4">
+      <c r="B331" t="s">
+        <v>739</v>
+      </c>
+      <c r="C331" t="s">
+        <v>56</v>
+      </c>
+      <c r="D331" t="s">
+        <v>49</v>
+      </c>
+      <c r="E331" t="s">
+        <v>694</v>
+      </c>
+      <c r="F331" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="332" spans="4:4">
+      <c r="B332" t="s">
+        <v>740</v>
+      </c>
+      <c r="C332" t="s">
+        <v>56</v>
+      </c>
+      <c r="D332" t="s">
+        <v>62</v>
+      </c>
+      <c r="E332" t="s">
+        <v>63</v>
+      </c>
+      <c r="F332" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="333" spans="4:4">
+      <c r="B333" t="s">
+        <v>741</v>
+      </c>
+      <c r="C333" t="s">
+        <v>56</v>
+      </c>
+      <c r="D333" t="s">
+        <v>49</v>
+      </c>
+      <c r="E333" t="s">
+        <v>694</v>
+      </c>
+      <c r="F333" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="334" spans="4:4">
+      <c r="B334" t="s">
+        <v>743</v>
+      </c>
+      <c r="C334" t="s">
+        <v>56</v>
+      </c>
+      <c r="D334" t="s">
+        <v>62</v>
+      </c>
+      <c r="E334" t="s">
+        <v>63</v>
+      </c>
+      <c r="F334" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="335" spans="4:4">
+      <c r="B335" t="s">
+        <v>744</v>
+      </c>
+      <c r="C335" t="s">
+        <v>56</v>
+      </c>
+      <c r="D335" t="s">
+        <v>49</v>
+      </c>
+      <c r="E335" t="s">
+        <v>694</v>
+      </c>
+      <c r="F335" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="336" spans="4:4">
+      <c r="B336" t="s">
+        <v>746</v>
+      </c>
+      <c r="C336" t="s">
+        <v>56</v>
+      </c>
+      <c r="D336" t="s">
+        <v>62</v>
+      </c>
+      <c r="E336" t="s">
+        <v>63</v>
+      </c>
+      <c r="F336" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="337" spans="4:4">
+      <c r="B337" t="s">
+        <v>747</v>
+      </c>
+      <c r="C337" t="s">
+        <v>56</v>
+      </c>
+      <c r="D337" t="s">
+        <v>49</v>
+      </c>
+      <c r="E337" t="s">
+        <v>694</v>
+      </c>
+      <c r="F337" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="338" spans="4:4">
+      <c r="B338" t="s">
+        <v>748</v>
+      </c>
+      <c r="C338" t="s">
+        <v>56</v>
+      </c>
+      <c r="D338" t="s">
+        <v>62</v>
+      </c>
+      <c r="E338" t="s">
+        <v>63</v>
+      </c>
+      <c r="F338" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="339" spans="4:4">
+      <c r="B339" t="s">
+        <v>749</v>
+      </c>
+      <c r="C339" t="s">
+        <v>56</v>
+      </c>
+      <c r="D339" t="s">
+        <v>49</v>
+      </c>
+      <c r="E339" t="s">
+        <v>694</v>
+      </c>
+      <c r="F339" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="340" spans="4:4"/>
     <row r="341" spans="4:4"/>
     <row r="342" spans="4:4"/>

</xml_diff>

<commit_message>
indicatori ok - lunghezza titoli indicators ok - schermata board debug not ok
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794791" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870678" uniqueCount="770">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2565,6 +2565,9 @@
   <si>
     <t xml:space="preserve">-
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cind_1</t>
   </si>
 </sst>
 </file>
@@ -4146,7 +4149,7 @@
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
         <v>63</v>
@@ -4180,7 +4183,7 @@
         <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
         <v>63</v>
@@ -4214,7 +4217,7 @@
         <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
         <v>63</v>
@@ -4248,7 +4251,7 @@
         <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
         <v>63</v>
@@ -4282,7 +4285,7 @@
         <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
         <v>63</v>
@@ -4316,7 +4319,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
         <v>63</v>
@@ -4724,7 +4727,7 @@
         <v>56</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E38" t="s">
         <v>63</v>
@@ -4758,7 +4761,7 @@
         <v>56</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E40" t="s">
         <v>63</v>
@@ -4792,7 +4795,7 @@
         <v>56</v>
       </c>
       <c r="D42" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E42" t="s">
         <v>63</v>
@@ -4826,7 +4829,7 @@
         <v>56</v>
       </c>
       <c r="D44" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E44" t="s">
         <v>63</v>
@@ -4860,7 +4863,7 @@
         <v>56</v>
       </c>
       <c r="D46" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E46" t="s">
         <v>63</v>
@@ -4894,7 +4897,7 @@
         <v>56</v>
       </c>
       <c r="D48" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E48" t="s">
         <v>63</v>
@@ -5302,7 +5305,7 @@
         <v>56</v>
       </c>
       <c r="D72" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E72" t="s">
         <v>63</v>
@@ -5336,7 +5339,7 @@
         <v>56</v>
       </c>
       <c r="D74" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E74" t="s">
         <v>63</v>
@@ -5370,7 +5373,7 @@
         <v>56</v>
       </c>
       <c r="D76" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E76" t="s">
         <v>63</v>
@@ -5404,7 +5407,7 @@
         <v>56</v>
       </c>
       <c r="D78" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E78" t="s">
         <v>63</v>
@@ -5438,7 +5441,7 @@
         <v>56</v>
       </c>
       <c r="D80" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E80" t="s">
         <v>63</v>
@@ -5472,7 +5475,7 @@
         <v>56</v>
       </c>
       <c r="D82" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E82" t="s">
         <v>63</v>
@@ -5880,7 +5883,7 @@
         <v>56</v>
       </c>
       <c r="D106" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E106" t="s">
         <v>63</v>
@@ -5914,7 +5917,7 @@
         <v>56</v>
       </c>
       <c r="D108" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E108" t="s">
         <v>63</v>
@@ -5948,7 +5951,7 @@
         <v>56</v>
       </c>
       <c r="D110" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E110" t="s">
         <v>63</v>
@@ -5982,7 +5985,7 @@
         <v>56</v>
       </c>
       <c r="D112" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E112" t="s">
         <v>63</v>
@@ -6016,7 +6019,7 @@
         <v>56</v>
       </c>
       <c r="D114" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E114" t="s">
         <v>63</v>
@@ -6050,7 +6053,7 @@
         <v>56</v>
       </c>
       <c r="D116" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E116" t="s">
         <v>63</v>
@@ -6628,7 +6631,7 @@
         <v>56</v>
       </c>
       <c r="D150" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E150" t="s">
         <v>63</v>
@@ -6662,7 +6665,7 @@
         <v>56</v>
       </c>
       <c r="D152" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E152" t="s">
         <v>63</v>
@@ -6696,7 +6699,7 @@
         <v>56</v>
       </c>
       <c r="D154" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E154" t="s">
         <v>63</v>
@@ -6730,7 +6733,7 @@
         <v>56</v>
       </c>
       <c r="D156" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E156" t="s">
         <v>63</v>
@@ -6764,7 +6767,7 @@
         <v>56</v>
       </c>
       <c r="D158" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E158" t="s">
         <v>63</v>
@@ -6798,7 +6801,7 @@
         <v>56</v>
       </c>
       <c r="D160" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E160" t="s">
         <v>63</v>
@@ -7512,7 +7515,7 @@
         <v>482</v>
       </c>
       <c r="D202" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E202" t="s">
         <v>63</v>
@@ -7546,7 +7549,7 @@
         <v>482</v>
       </c>
       <c r="D204" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E204" t="s">
         <v>63</v>
@@ -7580,7 +7583,7 @@
         <v>482</v>
       </c>
       <c r="D206" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E206" t="s">
         <v>63</v>
@@ -7614,7 +7617,7 @@
         <v>482</v>
       </c>
       <c r="D208" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E208" t="s">
         <v>63</v>
@@ -7648,7 +7651,7 @@
         <v>482</v>
       </c>
       <c r="D210" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E210" t="s">
         <v>63</v>
@@ -7682,7 +7685,7 @@
         <v>482</v>
       </c>
       <c r="D212" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E212" t="s">
         <v>63</v>
@@ -7716,7 +7719,7 @@
         <v>482</v>
       </c>
       <c r="D214" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E214" t="s">
         <v>63</v>
@@ -7750,7 +7753,7 @@
         <v>482</v>
       </c>
       <c r="D216" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E216" t="s">
         <v>63</v>
@@ -8192,7 +8195,7 @@
         <v>482</v>
       </c>
       <c r="D242" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E242" t="s">
         <v>63</v>
@@ -8260,7 +8263,7 @@
         <v>482</v>
       </c>
       <c r="D246" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E246" t="s">
         <v>63</v>
@@ -8566,7 +8569,7 @@
         <v>482</v>
       </c>
       <c r="D264" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E264" t="s">
         <v>63</v>
@@ -8634,7 +8637,7 @@
         <v>482</v>
       </c>
       <c r="D268" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E268" t="s">
         <v>63</v>
@@ -8668,7 +8671,7 @@
         <v>482</v>
       </c>
       <c r="D270" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E270" t="s">
         <v>63</v>
@@ -8770,7 +8773,7 @@
         <v>482</v>
       </c>
       <c r="D276" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E276" t="s">
         <v>63</v>
@@ -8804,7 +8807,7 @@
         <v>482</v>
       </c>
       <c r="D278" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E278" t="s">
         <v>63</v>
@@ -8838,7 +8841,7 @@
         <v>482</v>
       </c>
       <c r="D280" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E280" t="s">
         <v>63</v>
@@ -9300,7 +9303,7 @@
         <v>49</v>
       </c>
       <c r="E307" t="s">
-        <v>768</v>
+        <v>696</v>
       </c>
       <c r="F307" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
routine di acc e autox modificate
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870678" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872723" uniqueCount="770">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -8512,16 +8512,16 @@
     </row>
     <row r="261" spans="4:4">
       <c r="B261" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C261" t="s">
         <v>473</v>
       </c>
       <c r="D261" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E261" t="s">
-        <v>463</v>
+        <v>63</v>
       </c>
       <c r="F261" t="s">
         <v>50</v>
@@ -8529,16 +8529,16 @@
     </row>
     <row r="262" spans="4:4">
       <c r="B262" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C262" t="s">
         <v>473</v>
       </c>
       <c r="D262" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E262" t="s">
-        <v>63</v>
+        <v>463</v>
       </c>
       <c r="F262" t="s">
         <v>50</v>
@@ -8546,16 +8546,16 @@
     </row>
     <row r="263" spans="4:4">
       <c r="B263" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C263" t="s">
-        <v>473</v>
+        <v>482</v>
       </c>
       <c r="D263" t="s">
         <v>49</v>
       </c>
       <c r="E263" t="s">
-        <v>463</v>
+        <v>63</v>
       </c>
       <c r="F263" t="s">
         <v>50</v>
@@ -8563,7 +8563,7 @@
     </row>
     <row r="264" spans="4:4">
       <c r="B264" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C264" t="s">
         <v>482</v>
@@ -8572,7 +8572,7 @@
         <v>49</v>
       </c>
       <c r="E264" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F264" t="s">
         <v>50</v>
@@ -8580,16 +8580,16 @@
     </row>
     <row r="265" spans="4:4">
       <c r="B265" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C265" t="s">
         <v>482</v>
       </c>
       <c r="D265" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E265" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="F265" t="s">
         <v>50</v>
@@ -8597,16 +8597,16 @@
     </row>
     <row r="266" spans="4:4">
       <c r="B266" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C266" t="s">
         <v>482</v>
       </c>
       <c r="D266" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E266" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F266" t="s">
         <v>50</v>
@@ -8614,7 +8614,7 @@
     </row>
     <row r="267" spans="4:4">
       <c r="B267" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C267" t="s">
         <v>482</v>
@@ -8623,7 +8623,7 @@
         <v>49</v>
       </c>
       <c r="E267" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F267" t="s">
         <v>50</v>
@@ -8631,7 +8631,7 @@
     </row>
     <row r="268" spans="4:4">
       <c r="B268" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C268" t="s">
         <v>482</v>
@@ -8640,7 +8640,7 @@
         <v>49</v>
       </c>
       <c r="E268" t="s">
-        <v>63</v>
+        <v>483</v>
       </c>
       <c r="F268" t="s">
         <v>50</v>
@@ -8648,7 +8648,7 @@
     </row>
     <row r="269" spans="4:4">
       <c r="B269" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C269" t="s">
         <v>482</v>
@@ -8657,7 +8657,7 @@
         <v>49</v>
       </c>
       <c r="E269" t="s">
-        <v>483</v>
+        <v>63</v>
       </c>
       <c r="F269" t="s">
         <v>50</v>
@@ -8665,7 +8665,7 @@
     </row>
     <row r="270" spans="4:4">
       <c r="B270" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C270" t="s">
         <v>482</v>
@@ -8674,7 +8674,7 @@
         <v>49</v>
       </c>
       <c r="E270" t="s">
-        <v>63</v>
+        <v>484</v>
       </c>
       <c r="F270" t="s">
         <v>50</v>
@@ -8682,16 +8682,16 @@
     </row>
     <row r="271" spans="4:4">
       <c r="B271" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C271" t="s">
         <v>482</v>
       </c>
       <c r="D271" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E271" t="s">
-        <v>484</v>
+        <v>63</v>
       </c>
       <c r="F271" t="s">
         <v>50</v>
@@ -8699,16 +8699,16 @@
     </row>
     <row r="272" spans="4:4">
       <c r="B272" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C272" t="s">
         <v>482</v>
       </c>
       <c r="D272" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E272" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F272" t="s">
         <v>50</v>
@@ -8716,16 +8716,16 @@
     </row>
     <row r="273" spans="4:4">
       <c r="B273" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C273" t="s">
         <v>482</v>
       </c>
       <c r="D273" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E273" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F273" t="s">
         <v>50</v>
@@ -8733,16 +8733,16 @@
     </row>
     <row r="274" spans="4:4">
       <c r="B274" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C274" t="s">
         <v>482</v>
       </c>
       <c r="D274" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E274" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F274" t="s">
         <v>50</v>
@@ -8750,7 +8750,7 @@
     </row>
     <row r="275" spans="4:4">
       <c r="B275" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C275" t="s">
         <v>482</v>
@@ -8759,7 +8759,7 @@
         <v>49</v>
       </c>
       <c r="E275" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F275" t="s">
         <v>50</v>
@@ -8767,7 +8767,7 @@
     </row>
     <row r="276" spans="4:4">
       <c r="B276" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C276" t="s">
         <v>482</v>
@@ -8776,7 +8776,7 @@
         <v>49</v>
       </c>
       <c r="E276" t="s">
-        <v>63</v>
+        <v>483</v>
       </c>
       <c r="F276" t="s">
         <v>50</v>
@@ -8784,7 +8784,7 @@
     </row>
     <row r="277" spans="4:4">
       <c r="B277" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C277" t="s">
         <v>482</v>
@@ -8793,7 +8793,7 @@
         <v>49</v>
       </c>
       <c r="E277" t="s">
-        <v>483</v>
+        <v>63</v>
       </c>
       <c r="F277" t="s">
         <v>50</v>
@@ -8801,7 +8801,7 @@
     </row>
     <row r="278" spans="4:4">
       <c r="B278" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C278" t="s">
         <v>482</v>
@@ -8810,7 +8810,7 @@
         <v>49</v>
       </c>
       <c r="E278" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F278" t="s">
         <v>50</v>
@@ -8818,7 +8818,7 @@
     </row>
     <row r="279" spans="4:4">
       <c r="B279" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C279" t="s">
         <v>482</v>
@@ -8827,7 +8827,7 @@
         <v>49</v>
       </c>
       <c r="E279" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="F279" t="s">
         <v>50</v>
@@ -8835,7 +8835,7 @@
     </row>
     <row r="280" spans="4:4">
       <c r="B280" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C280" t="s">
         <v>482</v>
@@ -8844,7 +8844,7 @@
         <v>49</v>
       </c>
       <c r="E280" t="s">
-        <v>63</v>
+        <v>518</v>
       </c>
       <c r="F280" t="s">
         <v>50</v>
@@ -8852,16 +8852,16 @@
     </row>
     <row r="281" spans="4:4">
       <c r="B281" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C281" t="s">
         <v>482</v>
       </c>
       <c r="D281" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E281" t="s">
-        <v>518</v>
+        <v>63</v>
       </c>
       <c r="F281" t="s">
         <v>50</v>
@@ -8869,16 +8869,16 @@
     </row>
     <row r="282" spans="4:4">
       <c r="B282" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C282" t="s">
         <v>482</v>
       </c>
       <c r="D282" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E282" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F282" t="s">
         <v>50</v>
@@ -8886,16 +8886,16 @@
     </row>
     <row r="283" spans="4:4">
       <c r="B283" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C283" t="s">
         <v>482</v>
       </c>
       <c r="D283" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E283" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F283" t="s">
         <v>50</v>
@@ -8903,16 +8903,16 @@
     </row>
     <row r="284" spans="4:4">
       <c r="B284" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C284" t="s">
         <v>482</v>
       </c>
       <c r="D284" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E284" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F284" t="s">
         <v>50</v>
@@ -8920,16 +8920,16 @@
     </row>
     <row r="285" spans="4:4">
       <c r="B285" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C285" t="s">
         <v>482</v>
       </c>
       <c r="D285" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E285" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F285" t="s">
         <v>50</v>
@@ -8937,16 +8937,16 @@
     </row>
     <row r="286" spans="4:4">
       <c r="B286" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C286" t="s">
         <v>482</v>
       </c>
       <c r="D286" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E286" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F286" t="s">
         <v>50</v>
@@ -8954,16 +8954,16 @@
     </row>
     <row r="287" spans="4:4">
       <c r="B287" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C287" t="s">
         <v>482</v>
       </c>
       <c r="D287" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E287" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F287" t="s">
         <v>50</v>
@@ -8971,16 +8971,16 @@
     </row>
     <row r="288" spans="4:4">
       <c r="B288" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C288" t="s">
         <v>482</v>
       </c>
       <c r="D288" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E288" t="s">
-        <v>63</v>
+        <v>551</v>
       </c>
       <c r="F288" t="s">
         <v>50</v>
@@ -8988,16 +8988,16 @@
     </row>
     <row r="289" spans="4:4">
       <c r="B289" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C289" t="s">
         <v>482</v>
       </c>
       <c r="D289" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E289" t="s">
-        <v>551</v>
+        <v>63</v>
       </c>
       <c r="F289" t="s">
         <v>50</v>
@@ -9005,16 +9005,16 @@
     </row>
     <row r="290" spans="4:4">
       <c r="B290" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C290" t="s">
         <v>482</v>
       </c>
       <c r="D290" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E290" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F290" t="s">
         <v>50</v>
@@ -9022,16 +9022,16 @@
     </row>
     <row r="291" spans="4:4">
       <c r="B291" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C291" t="s">
         <v>482</v>
       </c>
       <c r="D291" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E291" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F291" t="s">
         <v>50</v>
@@ -9039,16 +9039,16 @@
     </row>
     <row r="292" spans="4:4">
       <c r="B292" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C292" t="s">
         <v>482</v>
       </c>
       <c r="D292" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E292" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F292" t="s">
         <v>50</v>
@@ -9056,16 +9056,16 @@
     </row>
     <row r="293" spans="4:4">
       <c r="B293" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C293" t="s">
         <v>482</v>
       </c>
       <c r="D293" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E293" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F293" t="s">
         <v>50</v>
@@ -9073,16 +9073,16 @@
     </row>
     <row r="294" spans="4:4">
       <c r="B294" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C294" t="s">
         <v>482</v>
       </c>
       <c r="D294" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E294" t="s">
-        <v>63</v>
+        <v>680</v>
       </c>
       <c r="F294" t="s">
         <v>50</v>
@@ -9090,16 +9090,16 @@
     </row>
     <row r="295" spans="4:4">
       <c r="B295" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C295" t="s">
         <v>482</v>
       </c>
       <c r="D295" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E295" t="s">
-        <v>680</v>
+        <v>63</v>
       </c>
       <c r="F295" t="s">
         <v>50</v>
@@ -9107,16 +9107,16 @@
     </row>
     <row r="296" spans="4:4">
       <c r="B296" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C296" t="s">
         <v>482</v>
       </c>
       <c r="D296" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E296" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F296" t="s">
         <v>50</v>
@@ -9124,16 +9124,16 @@
     </row>
     <row r="297" spans="4:4">
       <c r="B297" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C297" t="s">
         <v>482</v>
       </c>
       <c r="D297" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E297" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F297" t="s">
         <v>50</v>
@@ -9141,16 +9141,16 @@
     </row>
     <row r="298" spans="4:4">
       <c r="B298" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C298" t="s">
         <v>482</v>
       </c>
       <c r="D298" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E298" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F298" t="s">
         <v>50</v>
@@ -9158,16 +9158,16 @@
     </row>
     <row r="299" spans="4:4">
       <c r="B299" t="s">
-        <v>447</v>
+        <v>681</v>
       </c>
       <c r="C299" t="s">
         <v>482</v>
       </c>
       <c r="D299" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E299" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F299" t="s">
         <v>50</v>
@@ -9175,16 +9175,16 @@
     </row>
     <row r="300" spans="4:4">
       <c r="B300" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="C300" t="s">
         <v>482</v>
       </c>
       <c r="D300" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E300" t="s">
-        <v>63</v>
+        <v>687</v>
       </c>
       <c r="F300" t="s">
         <v>50</v>
@@ -9192,16 +9192,16 @@
     </row>
     <row r="301" spans="4:4">
       <c r="B301" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C301" t="s">
         <v>482</v>
       </c>
       <c r="D301" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E301" t="s">
-        <v>687</v>
+        <v>63</v>
       </c>
       <c r="F301" t="s">
         <v>50</v>
@@ -9209,16 +9209,16 @@
     </row>
     <row r="302" spans="4:4">
       <c r="B302" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C302" t="s">
         <v>482</v>
       </c>
       <c r="D302" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E302" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F302" t="s">
         <v>50</v>
@@ -9226,16 +9226,16 @@
     </row>
     <row r="303" spans="4:4">
       <c r="B303" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="C303" t="s">
         <v>482</v>
       </c>
       <c r="D303" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E303" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F303" t="s">
         <v>50</v>
@@ -9243,16 +9243,16 @@
     </row>
     <row r="304" spans="4:4">
       <c r="B304" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="C304" t="s">
         <v>482</v>
       </c>
       <c r="D304" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E304" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F304" t="s">
         <v>50</v>
@@ -9260,16 +9260,16 @@
     </row>
     <row r="305" spans="4:4">
       <c r="B305" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="C305" t="s">
-        <v>482</v>
+        <v>56</v>
       </c>
       <c r="D305" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E305" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="F305" t="s">
         <v>50</v>
@@ -9277,16 +9277,16 @@
     </row>
     <row r="306" spans="4:4">
       <c r="B306" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="C306" t="s">
         <v>56</v>
       </c>
       <c r="D306" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E306" t="s">
-        <v>63</v>
+        <v>696</v>
       </c>
       <c r="F306" t="s">
         <v>50</v>
@@ -9294,16 +9294,16 @@
     </row>
     <row r="307" spans="4:4">
       <c r="B307" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="C307" t="s">
         <v>56</v>
       </c>
       <c r="D307" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E307" t="s">
-        <v>696</v>
+        <v>63</v>
       </c>
       <c r="F307" t="s">
         <v>50</v>
@@ -9311,7 +9311,7 @@
     </row>
     <row r="308" spans="4:4">
       <c r="B308" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="C308" t="s">
         <v>56</v>
@@ -9328,16 +9328,16 @@
     </row>
     <row r="309" spans="4:4">
       <c r="B309" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C309" t="s">
         <v>56</v>
       </c>
       <c r="D309" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E309" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F309" t="s">
         <v>50</v>
@@ -9345,7 +9345,7 @@
     </row>
     <row r="310" spans="4:4">
       <c r="B310" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="C310" t="s">
         <v>56</v>
@@ -9362,16 +9362,16 @@
     </row>
     <row r="311" spans="4:4">
       <c r="B311" t="s">
-        <v>695</v>
+        <v>703</v>
       </c>
       <c r="C311" t="s">
         <v>56</v>
       </c>
       <c r="D311" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E311" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F311" t="s">
         <v>50</v>
@@ -9379,16 +9379,16 @@
     </row>
     <row r="312" spans="4:4">
       <c r="B312" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="C312" t="s">
         <v>56</v>
       </c>
       <c r="D312" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E312" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F312" t="s">
         <v>50</v>
@@ -9396,16 +9396,16 @@
     </row>
     <row r="313" spans="4:4">
       <c r="B313" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="C313" t="s">
         <v>56</v>
       </c>
       <c r="D313" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E313" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F313" t="s">
         <v>50</v>
@@ -9413,16 +9413,16 @@
     </row>
     <row r="314" spans="4:4">
       <c r="B314" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C314" t="s">
         <v>56</v>
       </c>
       <c r="D314" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E314" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F314" t="s">
         <v>50</v>
@@ -9430,16 +9430,16 @@
     </row>
     <row r="315" spans="4:4">
       <c r="B315" t="s">
-        <v>707</v>
+        <v>715</v>
       </c>
       <c r="C315" t="s">
         <v>56</v>
       </c>
       <c r="D315" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E315" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F315" t="s">
         <v>50</v>
@@ -9447,16 +9447,16 @@
     </row>
     <row r="316" spans="4:4">
       <c r="B316" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="C316" t="s">
         <v>56</v>
       </c>
       <c r="D316" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E316" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F316" t="s">
         <v>50</v>
@@ -9464,16 +9464,16 @@
     </row>
     <row r="317" spans="4:4">
       <c r="B317" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C317" t="s">
         <v>56</v>
       </c>
       <c r="D317" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E317" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F317" t="s">
         <v>50</v>
@@ -9481,16 +9481,16 @@
     </row>
     <row r="318" spans="4:4">
       <c r="B318" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C318" t="s">
         <v>56</v>
       </c>
       <c r="D318" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E318" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F318" t="s">
         <v>50</v>
@@ -9498,16 +9498,16 @@
     </row>
     <row r="319" spans="4:4">
       <c r="B319" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C319" t="s">
         <v>56</v>
       </c>
       <c r="D319" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E319" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F319" t="s">
         <v>50</v>
@@ -9515,16 +9515,16 @@
     </row>
     <row r="320" spans="4:4">
       <c r="B320" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C320" t="s">
         <v>56</v>
       </c>
       <c r="D320" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E320" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F320" t="s">
         <v>50</v>
@@ -9532,16 +9532,16 @@
     </row>
     <row r="321" spans="4:4">
       <c r="B321" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="C321" t="s">
         <v>56</v>
       </c>
       <c r="D321" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E321" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F321" t="s">
         <v>50</v>
@@ -9549,16 +9549,16 @@
     </row>
     <row r="322" spans="4:4">
       <c r="B322" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C322" t="s">
         <v>56</v>
       </c>
       <c r="D322" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E322" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F322" t="s">
         <v>50</v>
@@ -9566,16 +9566,16 @@
     </row>
     <row r="323" spans="4:4">
       <c r="B323" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C323" t="s">
         <v>56</v>
       </c>
       <c r="D323" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E323" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F323" t="s">
         <v>50</v>
@@ -9583,16 +9583,16 @@
     </row>
     <row r="324" spans="4:4">
       <c r="B324" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C324" t="s">
         <v>56</v>
       </c>
       <c r="D324" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E324" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F324" t="s">
         <v>50</v>
@@ -9600,16 +9600,16 @@
     </row>
     <row r="325" spans="4:4">
       <c r="B325" t="s">
-        <v>726</v>
+        <v>732</v>
       </c>
       <c r="C325" t="s">
         <v>56</v>
       </c>
       <c r="D325" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E325" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F325" t="s">
         <v>50</v>
@@ -9617,16 +9617,16 @@
     </row>
     <row r="326" spans="4:4">
       <c r="B326" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C326" t="s">
         <v>56</v>
       </c>
       <c r="D326" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E326" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F326" t="s">
         <v>50</v>
@@ -9634,16 +9634,16 @@
     </row>
     <row r="327" spans="4:4">
       <c r="B327" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="C327" t="s">
         <v>56</v>
       </c>
       <c r="D327" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E327" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F327" t="s">
         <v>50</v>
@@ -9651,16 +9651,16 @@
     </row>
     <row r="328" spans="4:4">
       <c r="B328" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C328" t="s">
         <v>56</v>
       </c>
       <c r="D328" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E328" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F328" t="s">
         <v>50</v>
@@ -9668,16 +9668,16 @@
     </row>
     <row r="329" spans="4:4">
       <c r="B329" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="C329" t="s">
         <v>56</v>
       </c>
       <c r="D329" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E329" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F329" t="s">
         <v>50</v>
@@ -9685,16 +9685,16 @@
     </row>
     <row r="330" spans="4:4">
       <c r="B330" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="C330" t="s">
         <v>56</v>
       </c>
       <c r="D330" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E330" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F330" t="s">
         <v>50</v>
@@ -9702,16 +9702,16 @@
     </row>
     <row r="331" spans="4:4">
       <c r="B331" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="C331" t="s">
         <v>56</v>
       </c>
       <c r="D331" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E331" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F331" t="s">
         <v>50</v>
@@ -9719,16 +9719,16 @@
     </row>
     <row r="332" spans="4:4">
       <c r="B332" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C332" t="s">
         <v>56</v>
       </c>
       <c r="D332" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E332" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F332" t="s">
         <v>50</v>
@@ -9736,16 +9736,16 @@
     </row>
     <row r="333" spans="4:4">
       <c r="B333" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="C333" t="s">
         <v>56</v>
       </c>
       <c r="D333" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E333" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F333" t="s">
         <v>50</v>
@@ -9753,16 +9753,16 @@
     </row>
     <row r="334" spans="4:4">
       <c r="B334" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="C334" t="s">
         <v>56</v>
       </c>
       <c r="D334" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E334" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F334" t="s">
         <v>50</v>
@@ -9770,16 +9770,16 @@
     </row>
     <row r="335" spans="4:4">
       <c r="B335" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="C335" t="s">
         <v>56</v>
       </c>
       <c r="D335" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E335" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F335" t="s">
         <v>50</v>
@@ -9787,16 +9787,16 @@
     </row>
     <row r="336" spans="4:4">
       <c r="B336" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C336" t="s">
         <v>56</v>
       </c>
       <c r="D336" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E336" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F336" t="s">
         <v>50</v>
@@ -9804,16 +9804,16 @@
     </row>
     <row r="337" spans="4:4">
       <c r="B337" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="C337" t="s">
         <v>56</v>
       </c>
       <c r="D337" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E337" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="F337" t="s">
         <v>50</v>
@@ -9821,38 +9821,22 @@
     </row>
     <row r="338" spans="4:4">
       <c r="B338" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C338" t="s">
         <v>56</v>
       </c>
       <c r="D338" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E338" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="F338" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="339" spans="4:4">
-      <c r="B339" t="s">
-        <v>749</v>
-      </c>
-      <c r="C339" t="s">
-        <v>56</v>
-      </c>
-      <c r="D339" t="s">
-        <v>49</v>
-      </c>
-      <c r="E339" t="s">
-        <v>694</v>
-      </c>
-      <c r="F339" t="s">
-        <v>50</v>
-      </c>
-    </row>
+    <row r="339" spans="4:4"/>
     <row r="340" spans="4:4"/>
     <row r="341" spans="4:4"/>
     <row r="342" spans="4:4"/>

</xml_diff>

<commit_message>
board debug sistemata a metà
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872723" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878858" uniqueCount="773">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2568,6 +2568,15 @@
   </si>
   <si>
     <t xml:space="preserve">Cind_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42-248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42-249</t>
   </si>
 </sst>
 </file>
@@ -3807,7 +3816,7 @@
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4" t="s">
-        <v>455</v>
+        <v>772</v>
       </c>
       <c r="I4"/>
       <c r="K4" s="5" t="s">

</xml_diff>

<commit_message>
aggiunta schermata e logica per i dinamici, da testare
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878858" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947304" uniqueCount="800">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2577,6 +2577,87 @@
   </si>
   <si>
     <t xml:space="preserve">42-249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId363</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIBRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPS 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPS 0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPS 100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPS 100Indicators[RPM].intValore%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW ANGLE 100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW ANGLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId367</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINEARS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINEAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId368</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOAD CELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId369</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOAD CELL DONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;valueDON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; DONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId370</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTHING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
   </si>
 </sst>
 </file>
@@ -3848,7 +3929,9 @@
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5"/>
+      <c r="F5" t="s">
+        <v>799</v>
+      </c>
       <c r="G5"/>
       <c r="H5" t="s">
         <v>455</v>
@@ -9845,14 +9928,142 @@
         <v>50</v>
       </c>
     </row>
-    <row r="339" spans="4:4"/>
-    <row r="340" spans="4:4"/>
-    <row r="341" spans="4:4"/>
-    <row r="342" spans="4:4"/>
-    <row r="343" spans="4:4"/>
-    <row r="344" spans="4:4"/>
-    <row r="345" spans="4:4"/>
-    <row r="346" spans="4:4"/>
+    <row r="339" spans="4:4">
+      <c r="B339" t="s">
+        <v>773</v>
+      </c>
+      <c r="C339" t="s">
+        <v>59</v>
+      </c>
+      <c r="D339" t="s">
+        <v>49</v>
+      </c>
+      <c r="E339" t="s">
+        <v>775</v>
+      </c>
+      <c r="F339" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="340" spans="4:4">
+      <c r="B340" t="s">
+        <v>776</v>
+      </c>
+      <c r="C340" t="s">
+        <v>59</v>
+      </c>
+      <c r="D340" t="s">
+        <v>49</v>
+      </c>
+      <c r="E340" t="s">
+        <v>778</v>
+      </c>
+      <c r="F340" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="341" spans="4:4">
+      <c r="B341" t="s">
+        <v>779</v>
+      </c>
+      <c r="C341" t="s">
+        <v>59</v>
+      </c>
+      <c r="D341" t="s">
+        <v>49</v>
+      </c>
+      <c r="E341" t="s">
+        <v>780</v>
+      </c>
+      <c r="F341" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="342" spans="4:4">
+      <c r="B342" t="s">
+        <v>782</v>
+      </c>
+      <c r="C342" t="s">
+        <v>59</v>
+      </c>
+      <c r="D342" t="s">
+        <v>49</v>
+      </c>
+      <c r="E342" t="s">
+        <v>784</v>
+      </c>
+      <c r="F342" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="343" spans="4:4">
+      <c r="B343" t="s">
+        <v>785</v>
+      </c>
+      <c r="C343" t="s">
+        <v>59</v>
+      </c>
+      <c r="D343" t="s">
+        <v>49</v>
+      </c>
+      <c r="E343" t="s">
+        <v>787</v>
+      </c>
+      <c r="F343" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="344" spans="4:4">
+      <c r="B344" t="s">
+        <v>788</v>
+      </c>
+      <c r="C344" t="s">
+        <v>59</v>
+      </c>
+      <c r="D344" t="s">
+        <v>49</v>
+      </c>
+      <c r="E344" t="s">
+        <v>789</v>
+      </c>
+      <c r="F344" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="345" spans="4:4">
+      <c r="B345" t="s">
+        <v>790</v>
+      </c>
+      <c r="C345" t="s">
+        <v>59</v>
+      </c>
+      <c r="D345" t="s">
+        <v>62</v>
+      </c>
+      <c r="E345" t="s">
+        <v>794</v>
+      </c>
+      <c r="F345" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="346" spans="4:4">
+      <c r="B346" t="s">
+        <v>795</v>
+      </c>
+      <c r="C346" t="s">
+        <v>59</v>
+      </c>
+      <c r="D346" t="s">
+        <v>49</v>
+      </c>
+      <c r="E346" t="s">
+        <v>798</v>
+      </c>
+      <c r="F346" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="347" spans="4:4"/>
     <row r="348" spans="4:4"/>
     <row r="349" spans="4:4"/>

</xml_diff>

<commit_message>
problema ok button risolto (forse)
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947304" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951492" uniqueCount="800">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -7199,7 +7199,7 @@
         <v>482</v>
       </c>
       <c r="D178" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E178" t="s">
         <v>63</v>
@@ -7233,7 +7233,7 @@
         <v>482</v>
       </c>
       <c r="D180" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E180" t="s">
         <v>63</v>
@@ -7267,7 +7267,7 @@
         <v>482</v>
       </c>
       <c r="D182" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E182" t="s">
         <v>63</v>
@@ -7301,7 +7301,7 @@
         <v>482</v>
       </c>
       <c r="D184" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E184" t="s">
         <v>63</v>
@@ -8185,7 +8185,7 @@
         <v>482</v>
       </c>
       <c r="D236" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E236" t="s">
         <v>63</v>
@@ -9052,7 +9052,7 @@
         <v>482</v>
       </c>
       <c r="D287" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E287" t="s">
         <v>63</v>
@@ -9154,7 +9154,7 @@
         <v>482</v>
       </c>
       <c r="D293" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E293" t="s">
         <v>63</v>
@@ -9256,7 +9256,7 @@
         <v>482</v>
       </c>
       <c r="D299" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E299" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
dcu dead e dcu ready quando c'è usb
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951492" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972654" uniqueCount="808">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2658,6 +2658,30 @@
   </si>
   <si>
     <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCU DEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId372</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId373</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId374</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId376</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId377</t>
   </si>
 </sst>
 </file>
@@ -10064,13 +10088,125 @@
         <v>50</v>
       </c>
     </row>
-    <row r="347" spans="4:4"/>
-    <row r="348" spans="4:4"/>
-    <row r="349" spans="4:4"/>
-    <row r="350" spans="4:4"/>
-    <row r="351" spans="4:4"/>
-    <row r="352" spans="4:4"/>
-    <row r="353" spans="4:4"/>
+    <row r="347" spans="4:4">
+      <c r="B347" t="s">
+        <v>800</v>
+      </c>
+      <c r="C347" t="s">
+        <v>473</v>
+      </c>
+      <c r="D347" t="s">
+        <v>49</v>
+      </c>
+      <c r="E347" t="s">
+        <v>801</v>
+      </c>
+      <c r="F347" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="348" spans="4:4">
+      <c r="B348" t="s">
+        <v>802</v>
+      </c>
+      <c r="C348" t="s">
+        <v>473</v>
+      </c>
+      <c r="D348" t="s">
+        <v>49</v>
+      </c>
+      <c r="E348" t="s">
+        <v>801</v>
+      </c>
+      <c r="F348" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="349" spans="4:4">
+      <c r="B349" t="s">
+        <v>803</v>
+      </c>
+      <c r="C349" t="s">
+        <v>473</v>
+      </c>
+      <c r="D349" t="s">
+        <v>49</v>
+      </c>
+      <c r="E349" t="s">
+        <v>801</v>
+      </c>
+      <c r="F349" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="350" spans="4:4">
+      <c r="B350" t="s">
+        <v>804</v>
+      </c>
+      <c r="C350" t="s">
+        <v>473</v>
+      </c>
+      <c r="D350" t="s">
+        <v>49</v>
+      </c>
+      <c r="E350" t="s">
+        <v>801</v>
+      </c>
+      <c r="F350" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="351" spans="4:4">
+      <c r="B351" t="s">
+        <v>806</v>
+      </c>
+      <c r="C351" t="s">
+        <v>473</v>
+      </c>
+      <c r="D351" t="s">
+        <v>49</v>
+      </c>
+      <c r="E351" t="s">
+        <v>801</v>
+      </c>
+      <c r="F351" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="352" spans="4:4">
+      <c r="B352" t="s">
+        <v>807</v>
+      </c>
+      <c r="C352" t="s">
+        <v>473</v>
+      </c>
+      <c r="D352" t="s">
+        <v>49</v>
+      </c>
+      <c r="E352" t="s">
+        <v>801</v>
+      </c>
+      <c r="F352" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="353" spans="4:4">
+      <c r="B353" t="s">
+        <v>805</v>
+      </c>
+      <c r="C353" t="s">
+        <v>473</v>
+      </c>
+      <c r="D353" t="s">
+        <v>49</v>
+      </c>
+      <c r="E353" t="s">
+        <v>801</v>
+      </c>
+      <c r="F353" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="354" spans="4:4"/>
     <row r="355" spans="4:4"/>
     <row r="356" spans="4:4"/>

</xml_diff>

<commit_message>
modificato i colori della marcia, messo ? sulla marcia, sistemata acquisition, da sistemare la scrittura su eeprom del traction
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972654" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976938" uniqueCount="810">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2682,6 +2682,12 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId377</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId378</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FE</t>
   </si>
 </sst>
 </file>
@@ -10207,7 +10213,23 @@
         <v>50</v>
       </c>
     </row>
-    <row r="354" spans="4:4"/>
+    <row r="354" spans="4:4">
+      <c r="B354" t="s">
+        <v>808</v>
+      </c>
+      <c r="C354" t="s">
+        <v>473</v>
+      </c>
+      <c r="D354" t="s">
+        <v>49</v>
+      </c>
+      <c r="E354" t="s">
+        <v>463</v>
+      </c>
+      <c r="F354" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="355" spans="4:4"/>
     <row r="356" spans="4:4"/>
     <row r="357" spans="4:4"/>

</xml_diff>

<commit_message>
aggiunta la schermata NOISE_MODE con logica, inserito il controllo sul valore massimo degli indicatori e controllo sull'indicatore Fuel Level
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976938" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376040" uniqueCount="966">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2688,6 +2688,598 @@
   </si>
   <si>
     <t xml:space="preserve">FE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId379</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOISE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOISE MODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPM:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId381</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId382</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId383</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId385</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPS:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId386</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId387</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IND:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRMC:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRMC_1:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId391</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRMC 1:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+MAP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId393</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId396</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId397</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRMC 2:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
   </si>
 </sst>
 </file>
@@ -10230,22 +10822,278 @@
         <v>50</v>
       </c>
     </row>
-    <row r="355" spans="4:4"/>
-    <row r="356" spans="4:4"/>
-    <row r="357" spans="4:4"/>
-    <row r="358" spans="4:4"/>
-    <row r="359" spans="4:4"/>
-    <row r="360" spans="4:4"/>
-    <row r="361" spans="4:4"/>
-    <row r="362" spans="4:4"/>
-    <row r="363" spans="4:4"/>
-    <row r="364" spans="4:4"/>
-    <row r="365" spans="4:4"/>
-    <row r="366" spans="4:4"/>
-    <row r="367" spans="4:4"/>
-    <row r="368" spans="4:4"/>
-    <row r="369" spans="4:4"/>
-    <row r="370" spans="4:4"/>
+    <row r="355" spans="4:4">
+      <c r="B355" t="s">
+        <v>810</v>
+      </c>
+      <c r="C355" t="s">
+        <v>56</v>
+      </c>
+      <c r="D355" t="s">
+        <v>62</v>
+      </c>
+      <c r="E355" t="s">
+        <v>812</v>
+      </c>
+      <c r="F355" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="356" spans="4:4">
+      <c r="B356" t="s">
+        <v>813</v>
+      </c>
+      <c r="C356" t="s">
+        <v>462</v>
+      </c>
+      <c r="D356" t="s">
+        <v>62</v>
+      </c>
+      <c r="E356" t="s">
+        <v>814</v>
+      </c>
+      <c r="F356" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="357" spans="4:4">
+      <c r="B357" t="s">
+        <v>815</v>
+      </c>
+      <c r="C357" t="s">
+        <v>59</v>
+      </c>
+      <c r="D357" t="s">
+        <v>965</v>
+      </c>
+      <c r="E357" t="s">
+        <v>63</v>
+      </c>
+      <c r="F357" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="358" spans="4:4">
+      <c r="B358" t="s">
+        <v>818</v>
+      </c>
+      <c r="C358" t="s">
+        <v>462</v>
+      </c>
+      <c r="D358" t="s">
+        <v>62</v>
+      </c>
+      <c r="E358" t="s">
+        <v>821</v>
+      </c>
+      <c r="F358" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="359" spans="4:4">
+      <c r="B359" t="s">
+        <v>819</v>
+      </c>
+      <c r="C359" t="s">
+        <v>59</v>
+      </c>
+      <c r="D359" t="s">
+        <v>965</v>
+      </c>
+      <c r="E359" t="s">
+        <v>63</v>
+      </c>
+      <c r="F359" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="360" spans="4:4">
+      <c r="B360" t="s">
+        <v>820</v>
+      </c>
+      <c r="C360" t="s">
+        <v>59</v>
+      </c>
+      <c r="D360" t="s">
+        <v>49</v>
+      </c>
+      <c r="E360" t="s">
+        <v>817</v>
+      </c>
+      <c r="F360" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="361" spans="4:4">
+      <c r="B361" t="s">
+        <v>822</v>
+      </c>
+      <c r="C361" t="s">
+        <v>462</v>
+      </c>
+      <c r="D361" t="s">
+        <v>62</v>
+      </c>
+      <c r="E361" t="s">
+        <v>964</v>
+      </c>
+      <c r="F361" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="362" spans="4:4">
+      <c r="B362" t="s">
+        <v>823</v>
+      </c>
+      <c r="C362" t="s">
+        <v>59</v>
+      </c>
+      <c r="D362" t="s">
+        <v>965</v>
+      </c>
+      <c r="E362" t="s">
+        <v>63</v>
+      </c>
+      <c r="F362" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="363" spans="4:4">
+      <c r="B363" t="s">
+        <v>824</v>
+      </c>
+      <c r="C363" t="s">
+        <v>59</v>
+      </c>
+      <c r="D363" t="s">
+        <v>49</v>
+      </c>
+      <c r="E363" t="s">
+        <v>817</v>
+      </c>
+      <c r="F363" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="364" spans="4:4">
+      <c r="B364" t="s">
+        <v>826</v>
+      </c>
+      <c r="C364" t="s">
+        <v>473</v>
+      </c>
+      <c r="D364" t="s">
+        <v>62</v>
+      </c>
+      <c r="E364" t="s">
+        <v>828</v>
+      </c>
+      <c r="F364" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="365" spans="4:4">
+      <c r="B365" t="s">
+        <v>869</v>
+      </c>
+      <c r="C365" t="s">
+        <v>462</v>
+      </c>
+      <c r="D365" t="s">
+        <v>62</v>
+      </c>
+      <c r="E365" t="s">
+        <v>891</v>
+      </c>
+      <c r="F365" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="366" spans="4:4">
+      <c r="B366" t="s">
+        <v>870</v>
+      </c>
+      <c r="C366" t="s">
+        <v>59</v>
+      </c>
+      <c r="D366" t="s">
+        <v>965</v>
+      </c>
+      <c r="E366" t="s">
+        <v>63</v>
+      </c>
+      <c r="F366" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="367" spans="4:4">
+      <c r="B367" t="s">
+        <v>871</v>
+      </c>
+      <c r="C367" t="s">
+        <v>59</v>
+      </c>
+      <c r="D367" t="s">
+        <v>49</v>
+      </c>
+      <c r="E367" t="s">
+        <v>817</v>
+      </c>
+      <c r="F367" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="368" spans="4:4">
+      <c r="B368" t="s">
+        <v>959</v>
+      </c>
+      <c r="C368" t="s">
+        <v>42</v>
+      </c>
+      <c r="D368" t="s">
+        <v>62</v>
+      </c>
+      <c r="E368" t="s">
+        <v>63</v>
+      </c>
+      <c r="F368" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="369" spans="4:4">
+      <c r="B369" t="s">
+        <v>962</v>
+      </c>
+      <c r="C369" t="s">
+        <v>59</v>
+      </c>
+      <c r="D369" t="s">
+        <v>49</v>
+      </c>
+      <c r="E369" t="s">
+        <v>817</v>
+      </c>
+      <c r="F369" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="370" spans="4:4">
+      <c r="B370" t="s">
+        <v>963</v>
+      </c>
+      <c r="C370" t="s">
+        <v>42</v>
+      </c>
+      <c r="D370" t="s">
+        <v>49</v>
+      </c>
+      <c r="E370" t="s">
+        <v>106</v>
+      </c>
+      <c r="F370" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="371" spans="4:4"/>
     <row r="372" spans="4:4"/>
     <row r="373" spans="4:4"/>

</xml_diff>

<commit_message>
antistall ok - schermata noise ok - tc e rpmlimiter ok
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387296" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428942" uniqueCount="992">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -3295,6 +3295,69 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V_BAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId409</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_OIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId414</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_FUEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VBAT</t>
   </si>
 </sst>
 </file>
@@ -11026,13 +11089,13 @@
     </row>
     <row r="366" spans="4:4">
       <c r="B366" t="s">
-        <v>870</v>
+        <v>959</v>
       </c>
       <c r="C366" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D366" t="s">
-        <v>965</v>
+        <v>62</v>
       </c>
       <c r="E366" t="s">
         <v>63</v>
@@ -11043,7 +11106,7 @@
     </row>
     <row r="367" spans="4:4">
       <c r="B367" t="s">
-        <v>871</v>
+        <v>962</v>
       </c>
       <c r="C367" t="s">
         <v>59</v>
@@ -11060,16 +11123,16 @@
     </row>
     <row r="368" spans="4:4">
       <c r="B368" t="s">
-        <v>959</v>
+        <v>963</v>
       </c>
       <c r="C368" t="s">
         <v>42</v>
       </c>
       <c r="D368" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E368" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="F368" t="s">
         <v>50</v>
@@ -11077,16 +11140,16 @@
     </row>
     <row r="369" spans="4:4">
       <c r="B369" t="s">
-        <v>962</v>
+        <v>966</v>
       </c>
       <c r="C369" t="s">
-        <v>59</v>
+        <v>473</v>
       </c>
       <c r="D369" t="s">
         <v>49</v>
       </c>
       <c r="E369" t="s">
-        <v>817</v>
+        <v>967</v>
       </c>
       <c r="F369" t="s">
         <v>50</v>
@@ -11094,16 +11157,16 @@
     </row>
     <row r="370" spans="4:4">
       <c r="B370" t="s">
-        <v>963</v>
+        <v>968</v>
       </c>
       <c r="C370" t="s">
-        <v>42</v>
+        <v>473</v>
       </c>
       <c r="D370" t="s">
         <v>49</v>
       </c>
       <c r="E370" t="s">
-        <v>106</v>
+        <v>967</v>
       </c>
       <c r="F370" t="s">
         <v>50</v>
@@ -11111,7 +11174,7 @@
     </row>
     <row r="371" spans="4:4">
       <c r="B371" t="s">
-        <v>966</v>
+        <v>969</v>
       </c>
       <c r="C371" t="s">
         <v>473</v>
@@ -11128,7 +11191,7 @@
     </row>
     <row r="372" spans="4:4">
       <c r="B372" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="C372" t="s">
         <v>473</v>
@@ -11145,16 +11208,16 @@
     </row>
     <row r="373" spans="4:4">
       <c r="B373" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="C373" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="D373" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E373" t="s">
-        <v>967</v>
+        <v>891</v>
       </c>
       <c r="F373" t="s">
         <v>50</v>
@@ -11162,28 +11225,140 @@
     </row>
     <row r="374" spans="4:4">
       <c r="B374" t="s">
-        <v>970</v>
+        <v>976</v>
       </c>
       <c r="C374" t="s">
-        <v>473</v>
+        <v>59</v>
       </c>
       <c r="D374" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E374" t="s">
-        <v>967</v>
+        <v>63</v>
       </c>
       <c r="F374" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="375" spans="4:4"/>
-    <row r="376" spans="4:4"/>
-    <row r="377" spans="4:4"/>
-    <row r="378" spans="4:4"/>
-    <row r="379" spans="4:4"/>
-    <row r="380" spans="4:4"/>
-    <row r="381" spans="4:4"/>
+    <row r="375" spans="4:4">
+      <c r="B375" t="s">
+        <v>977</v>
+      </c>
+      <c r="C375" t="s">
+        <v>59</v>
+      </c>
+      <c r="D375" t="s">
+        <v>49</v>
+      </c>
+      <c r="E375" t="s">
+        <v>91</v>
+      </c>
+      <c r="F375" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="376" spans="4:4">
+      <c r="B376" t="s">
+        <v>981</v>
+      </c>
+      <c r="C376" t="s">
+        <v>59</v>
+      </c>
+      <c r="D376" t="s">
+        <v>62</v>
+      </c>
+      <c r="E376" t="s">
+        <v>63</v>
+      </c>
+      <c r="F376" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="377" spans="4:4">
+      <c r="B377" t="s">
+        <v>982</v>
+      </c>
+      <c r="C377" t="s">
+        <v>59</v>
+      </c>
+      <c r="D377" t="s">
+        <v>49</v>
+      </c>
+      <c r="E377" t="s">
+        <v>91</v>
+      </c>
+      <c r="F377" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="378" spans="4:4">
+      <c r="B378" t="s">
+        <v>983</v>
+      </c>
+      <c r="C378" t="s">
+        <v>56</v>
+      </c>
+      <c r="D378" t="s">
+        <v>49</v>
+      </c>
+      <c r="E378" t="s">
+        <v>991</v>
+      </c>
+      <c r="F378" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="379" spans="4:4">
+      <c r="B379" t="s">
+        <v>986</v>
+      </c>
+      <c r="C379" t="s">
+        <v>56</v>
+      </c>
+      <c r="D379" t="s">
+        <v>49</v>
+      </c>
+      <c r="E379" t="s">
+        <v>989</v>
+      </c>
+      <c r="F379" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="380" spans="4:4">
+      <c r="B380" t="s">
+        <v>972</v>
+      </c>
+      <c r="C380" t="s">
+        <v>59</v>
+      </c>
+      <c r="D380" t="s">
+        <v>965</v>
+      </c>
+      <c r="E380" t="s">
+        <v>63</v>
+      </c>
+      <c r="F380" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="381" spans="4:4">
+      <c r="B381" t="s">
+        <v>973</v>
+      </c>
+      <c r="C381" t="s">
+        <v>59</v>
+      </c>
+      <c r="D381" t="s">
+        <v>49</v>
+      </c>
+      <c r="E381" t="s">
+        <v>817</v>
+      </c>
+      <c r="F381" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="382" spans="4:4"/>
     <row r="383" spans="4:4"/>
     <row r="384" spans="4:4"/>

</xml_diff>

<commit_message>
risolto prblema mode e grafica
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435854" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438176" uniqueCount="995">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -3361,6 +3361,12 @@
   </si>
   <si>
     <t xml:space="preserve">CLUTCH_TRGT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId417</t>
   </si>
 </sst>
 </file>
@@ -11362,9 +11368,57 @@
         <v>50</v>
       </c>
     </row>
-    <row r="382" spans="4:4"/>
-    <row r="383" spans="4:4"/>
-    <row r="384" spans="4:4"/>
+    <row r="382" spans="4:4">
+      <c r="B382" t="s">
+        <v>988</v>
+      </c>
+      <c r="C382" t="s">
+        <v>56</v>
+      </c>
+      <c r="D382" t="s">
+        <v>62</v>
+      </c>
+      <c r="E382" t="s">
+        <v>246</v>
+      </c>
+      <c r="F382" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="383" spans="4:4">
+      <c r="B383" t="s">
+        <v>993</v>
+      </c>
+      <c r="C383" t="s">
+        <v>59</v>
+      </c>
+      <c r="D383" t="s">
+        <v>62</v>
+      </c>
+      <c r="E383" t="s">
+        <v>63</v>
+      </c>
+      <c r="F383" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="384" spans="4:4">
+      <c r="B384" t="s">
+        <v>994</v>
+      </c>
+      <c r="C384" t="s">
+        <v>59</v>
+      </c>
+      <c r="D384" t="s">
+        <v>49</v>
+      </c>
+      <c r="E384" t="s">
+        <v>119</v>
+      </c>
+      <c r="F384" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="385" spans="4:4"/>
     <row r="386" spans="4:4"/>
     <row r="387" spans="4:4"/>

</xml_diff>

<commit_message>
rettangolo schermata 1 ok
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428942" uniqueCount="992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533042" uniqueCount="1046">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -3358,6 +3358,168 @@
   </si>
   <si>
     <t xml:space="preserve">VBAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId417</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIBRATION_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIBRATE_ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId418</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId419</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIBRATE_BASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIBRATE_AGM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId420</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIBRATE_PLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIBRATE_PLANAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId422</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId423</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAVE_CALIBRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId424</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESET_CALIBRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIBRATE ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIBRATE AGM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIBRATE PLANAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAVE DCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESET DCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId426</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId427</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId428</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TARE NOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESET TARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOP CLIBRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOP CALIBRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE_INIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE INIT IMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELATIVE TO ABS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE-INIT IMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMU 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMU 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId435</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId436</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId439</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId440</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId442</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId443</t>
   </si>
 </sst>
 </file>
@@ -11359,31 +11521,431 @@
         <v>50</v>
       </c>
     </row>
-    <row r="382" spans="4:4"/>
-    <row r="383" spans="4:4"/>
-    <row r="384" spans="4:4"/>
-    <row r="385" spans="4:4"/>
-    <row r="386" spans="4:4"/>
-    <row r="387" spans="4:4"/>
-    <row r="388" spans="4:4"/>
-    <row r="389" spans="4:4"/>
-    <row r="390" spans="4:4"/>
-    <row r="391" spans="4:4"/>
-    <row r="392" spans="4:4"/>
-    <row r="393" spans="4:4"/>
-    <row r="394" spans="4:4"/>
-    <row r="395" spans="4:4"/>
-    <row r="396" spans="4:4"/>
-    <row r="397" spans="4:4"/>
-    <row r="398" spans="4:4"/>
-    <row r="399" spans="4:4"/>
-    <row r="400" spans="4:4"/>
-    <row r="401" spans="4:4"/>
-    <row r="402" spans="4:4"/>
-    <row r="403" spans="4:4"/>
-    <row r="404" spans="4:4"/>
-    <row r="405" spans="4:4"/>
-    <row r="406" spans="4:4"/>
+    <row r="382" spans="4:4">
+      <c r="B382" t="s">
+        <v>988</v>
+      </c>
+      <c r="C382" t="s">
+        <v>59</v>
+      </c>
+      <c r="D382" t="s">
+        <v>49</v>
+      </c>
+      <c r="E382" t="s">
+        <v>992</v>
+      </c>
+      <c r="F382" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="383" spans="4:4">
+      <c r="B383" t="s">
+        <v>993</v>
+      </c>
+      <c r="C383" t="s">
+        <v>482</v>
+      </c>
+      <c r="D383" t="s">
+        <v>62</v>
+      </c>
+      <c r="E383" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F383" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="384" spans="4:4">
+      <c r="B384" t="s">
+        <v>997</v>
+      </c>
+      <c r="C384" t="s">
+        <v>482</v>
+      </c>
+      <c r="D384" t="s">
+        <v>62</v>
+      </c>
+      <c r="E384" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F384" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="385" spans="4:4">
+      <c r="B385" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C385" t="s">
+        <v>482</v>
+      </c>
+      <c r="D385" t="s">
+        <v>62</v>
+      </c>
+      <c r="E385" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F385" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="386" spans="4:4">
+      <c r="B386" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C386" t="s">
+        <v>482</v>
+      </c>
+      <c r="D386" t="s">
+        <v>62</v>
+      </c>
+      <c r="E386" t="s">
+        <v>1014</v>
+      </c>
+      <c r="F386" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="387" spans="4:4">
+      <c r="B387" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C387" t="s">
+        <v>482</v>
+      </c>
+      <c r="D387" t="s">
+        <v>62</v>
+      </c>
+      <c r="E387" t="s">
+        <v>1015</v>
+      </c>
+      <c r="F387" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="388" spans="4:4">
+      <c r="B388" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C388" t="s">
+        <v>482</v>
+      </c>
+      <c r="D388" t="s">
+        <v>62</v>
+      </c>
+      <c r="E388" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F388" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="389" spans="4:4">
+      <c r="B389" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C389" t="s">
+        <v>482</v>
+      </c>
+      <c r="D389" t="s">
+        <v>62</v>
+      </c>
+      <c r="E389" t="s">
+        <v>1021</v>
+      </c>
+      <c r="F389" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="390" spans="4:4">
+      <c r="B390" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C390" t="s">
+        <v>482</v>
+      </c>
+      <c r="D390" t="s">
+        <v>62</v>
+      </c>
+      <c r="E390" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F390" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="391" spans="4:4">
+      <c r="B391" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C391" t="s">
+        <v>482</v>
+      </c>
+      <c r="D391" t="s">
+        <v>62</v>
+      </c>
+      <c r="E391" t="s">
+        <v>1027</v>
+      </c>
+      <c r="F391" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="392" spans="4:4">
+      <c r="B392" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C392" t="s">
+        <v>482</v>
+      </c>
+      <c r="D392" t="s">
+        <v>62</v>
+      </c>
+      <c r="E392" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F392" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="393" spans="4:4">
+      <c r="B393" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C393" t="s">
+        <v>482</v>
+      </c>
+      <c r="D393" t="s">
+        <v>62</v>
+      </c>
+      <c r="E393" t="s">
+        <v>1029</v>
+      </c>
+      <c r="F393" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="394" spans="4:4">
+      <c r="B394" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C394" t="s">
+        <v>482</v>
+      </c>
+      <c r="D394" t="s">
+        <v>62</v>
+      </c>
+      <c r="E394" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F394" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="395" spans="4:4">
+      <c r="B395" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C395" t="s">
+        <v>482</v>
+      </c>
+      <c r="D395" t="s">
+        <v>62</v>
+      </c>
+      <c r="E395" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F395" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="396" spans="4:4">
+      <c r="B396" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C396" t="s">
+        <v>482</v>
+      </c>
+      <c r="D396" t="s">
+        <v>62</v>
+      </c>
+      <c r="E396" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F396" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="397" spans="4:4">
+      <c r="B397" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C397" t="s">
+        <v>482</v>
+      </c>
+      <c r="D397" t="s">
+        <v>62</v>
+      </c>
+      <c r="E397" t="s">
+        <v>57</v>
+      </c>
+      <c r="F397" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="398" spans="4:4">
+      <c r="B398" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C398" t="s">
+        <v>482</v>
+      </c>
+      <c r="D398" t="s">
+        <v>62</v>
+      </c>
+      <c r="E398" t="s">
+        <v>60</v>
+      </c>
+      <c r="F398" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="399" spans="4:4">
+      <c r="B399" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C399" t="s">
+        <v>469</v>
+      </c>
+      <c r="D399" t="s">
+        <v>62</v>
+      </c>
+      <c r="E399" t="s">
+        <v>63</v>
+      </c>
+      <c r="F399" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="400" spans="4:4">
+      <c r="B400" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C400" t="s">
+        <v>469</v>
+      </c>
+      <c r="D400" t="s">
+        <v>49</v>
+      </c>
+      <c r="E400" t="s">
+        <v>119</v>
+      </c>
+      <c r="F400" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="401" spans="4:4">
+      <c r="B401" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C401" t="s">
+        <v>469</v>
+      </c>
+      <c r="D401" t="s">
+        <v>62</v>
+      </c>
+      <c r="E401" t="s">
+        <v>63</v>
+      </c>
+      <c r="F401" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="402" spans="4:4">
+      <c r="B402" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C402" t="s">
+        <v>469</v>
+      </c>
+      <c r="D402" t="s">
+        <v>49</v>
+      </c>
+      <c r="E402" t="s">
+        <v>119</v>
+      </c>
+      <c r="F402" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="403" spans="4:4">
+      <c r="B403" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C403" t="s">
+        <v>469</v>
+      </c>
+      <c r="D403" t="s">
+        <v>62</v>
+      </c>
+      <c r="E403" t="s">
+        <v>63</v>
+      </c>
+      <c r="F403" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="404" spans="4:4">
+      <c r="B404" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C404" t="s">
+        <v>469</v>
+      </c>
+      <c r="D404" t="s">
+        <v>49</v>
+      </c>
+      <c r="E404" t="s">
+        <v>119</v>
+      </c>
+      <c r="F404" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="405" spans="4:4">
+      <c r="B405" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C405" t="s">
+        <v>469</v>
+      </c>
+      <c r="D405" t="s">
+        <v>62</v>
+      </c>
+      <c r="E405" t="s">
+        <v>63</v>
+      </c>
+      <c r="F405" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="406" spans="4:4">
+      <c r="B406" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C406" t="s">
+        <v>469</v>
+      </c>
+      <c r="D406" t="s">
+        <v>49</v>
+      </c>
+      <c r="E406" t="s">
+        <v>119</v>
+      </c>
+      <c r="F406" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="407" spans="4:4"/>
     <row r="408" spans="4:4"/>
     <row r="409" spans="4:4"/>

</xml_diff>

<commit_message>
parte calibrzioni imu da finire
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533042" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537950" uniqueCount="1048">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -3520,6 +3520,12 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIBRATE PLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIBRATE PLAN</t>
   </si>
 </sst>
 </file>
@@ -11583,7 +11589,7 @@
         <v>62</v>
       </c>
       <c r="E385" t="s">
-        <v>1013</v>
+        <v>1047</v>
       </c>
       <c r="F385" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
modifiche inutili perchè ho sbagliato branch
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537950" uniqueCount="1048">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547778" uniqueCount="1052">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -3526,6 +3526,18 @@
   </si>
   <si>
     <t xml:space="preserve">CALIBRATE PLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLUTCH_TRGT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId444</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId445</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId446</t>
   </si>
 </sst>
 </file>
@@ -6098,7 +6110,7 @@
         <v>62</v>
       </c>
       <c r="E62" t="s">
-        <v>111</v>
+        <v>1048</v>
       </c>
       <c r="F62" t="s">
         <v>50</v>
@@ -6126,7 +6138,7 @@
         <v>161</v>
       </c>
       <c r="C64" t="s">
-        <v>42</v>
+        <v>473</v>
       </c>
       <c r="D64" t="s">
         <v>62</v>
@@ -6143,7 +6155,7 @@
         <v>162</v>
       </c>
       <c r="C65" t="s">
-        <v>42</v>
+        <v>473</v>
       </c>
       <c r="D65" t="s">
         <v>49</v>
@@ -11952,9 +11964,57 @@
         <v>50</v>
       </c>
     </row>
-    <row r="407" spans="4:4"/>
-    <row r="408" spans="4:4"/>
-    <row r="409" spans="4:4"/>
+    <row r="407" spans="4:4">
+      <c r="B407" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C407" t="s">
+        <v>56</v>
+      </c>
+      <c r="D407" t="s">
+        <v>62</v>
+      </c>
+      <c r="E407" t="s">
+        <v>246</v>
+      </c>
+      <c r="F407" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="408" spans="4:4">
+      <c r="B408" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C408" t="s">
+        <v>59</v>
+      </c>
+      <c r="D408" t="s">
+        <v>62</v>
+      </c>
+      <c r="E408" t="s">
+        <v>63</v>
+      </c>
+      <c r="F408" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="409" spans="4:4">
+      <c r="B409" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C409" t="s">
+        <v>59</v>
+      </c>
+      <c r="D409" t="s">
+        <v>49</v>
+      </c>
+      <c r="E409" t="s">
+        <v>119</v>
+      </c>
+      <c r="F409" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="410" spans="4:4"/>
     <row r="411" spans="4:4"/>
     <row r="412" spans="4:4"/>

</xml_diff>

<commit_message>
aggiunto rpm_limiter a skidpad, sistemato display calibrazione imu, da controllare i valori di calibrazione delle imu
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537950" uniqueCount="1048">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545366" uniqueCount="1052">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -3526,6 +3526,18 @@
   </si>
   <si>
     <t xml:space="preserve">CALIBRATE PLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId444</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId445</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; DO</t>
   </si>
 </sst>
 </file>
@@ -11952,9 +11964,57 @@
         <v>50</v>
       </c>
     </row>
-    <row r="407" spans="4:4"/>
-    <row r="408" spans="4:4"/>
-    <row r="409" spans="4:4"/>
+    <row r="407" spans="4:4">
+      <c r="B407" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C407" t="s">
+        <v>56</v>
+      </c>
+      <c r="D407" t="s">
+        <v>62</v>
+      </c>
+      <c r="E407" t="s">
+        <v>246</v>
+      </c>
+      <c r="F407" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="408" spans="4:4">
+      <c r="B408" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C408" t="s">
+        <v>59</v>
+      </c>
+      <c r="D408" t="s">
+        <v>62</v>
+      </c>
+      <c r="E408" t="s">
+        <v>63</v>
+      </c>
+      <c r="F408" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="409" spans="4:4">
+      <c r="B409" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C409" t="s">
+        <v>59</v>
+      </c>
+      <c r="D409" t="s">
+        <v>49</v>
+      </c>
+      <c r="E409" t="s">
+        <v>119</v>
+      </c>
+      <c r="F409" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="410" spans="4:4"/>
     <row r="411" spans="4:4"/>
     <row r="412" spans="4:4"/>

</xml_diff>

<commit_message>
da provare cambio volante 1 2 in settings
</commit_message>
<xml_diff>
--- a/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
+++ b/SW_DP11_INIT/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574952" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617120" uniqueCount="1067">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -3562,6 +3562,27 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId451</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId452</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId453</t>
   </si>
 </sst>
 </file>
@@ -12039,9 +12060,57 @@
         <v>50</v>
       </c>
     </row>
-    <row r="410" spans="4:4"/>
-    <row r="411" spans="4:4"/>
-    <row r="412" spans="4:4"/>
+    <row r="410" spans="4:4">
+      <c r="B410" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C410" t="s">
+        <v>56</v>
+      </c>
+      <c r="D410" t="s">
+        <v>49</v>
+      </c>
+      <c r="E410" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F410" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="411" spans="4:4">
+      <c r="B411" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C411" t="s">
+        <v>462</v>
+      </c>
+      <c r="D411" t="s">
+        <v>49</v>
+      </c>
+      <c r="E411" t="s">
+        <v>63</v>
+      </c>
+      <c r="F411" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="412" spans="4:4">
+      <c r="B412" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C412" t="s">
+        <v>462</v>
+      </c>
+      <c r="D412" t="s">
+        <v>49</v>
+      </c>
+      <c r="E412" t="s">
+        <v>86</v>
+      </c>
+      <c r="F412" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="413" spans="4:4"/>
     <row r="414" spans="4:4"/>
     <row r="415" spans="4:4"/>

</xml_diff>